<commit_message>
added trailing stop limit order into algoritm
</commit_message>
<xml_diff>
--- a/db/real_trade_db.xlsx
+++ b/db/real_trade_db.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,30 +515,40 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>trailing_ratio</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>profit</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>buy_order_id</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>limit_if_touched_order_id</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>stop_order_id</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>trailing_LIT_order_id</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>trailing_stop_limit_order_id</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>timezone</t>
         </is>
@@ -598,29 +608,37 @@
         <v>1.007</v>
       </c>
       <c r="Q2" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R2" t="n">
         <v>1.73</v>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>FA1956DF73E03B2000</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>FA1956E75EBF44A000</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>FA1956E877FC84A000</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>FA1956EEE2AC3B2000</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>FAXXXX</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -680,25 +698,33 @@
         <v>1.005</v>
       </c>
       <c r="Q3" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R3" t="n">
         <v>1.180000000000027</v>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>FA1951CACA1BBB2000</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>FA1958EED98D44A000</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>FA1951CB1F203B2000</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr">
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>FAXXXX</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -758,25 +784,33 @@
         <v>1.005</v>
       </c>
       <c r="Q4" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R4" t="n">
         <v>1.09</v>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>FA1951E1BCC384A000</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>FA1951E253C07B2000</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>FA1951E5847EC4A000</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr">
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>FAXXXX</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -834,21 +868,29 @@
         <v>1.007</v>
       </c>
       <c r="Q5" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R5" t="n">
         <v>3</v>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>FA195825A91F04A000</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>FA19582868EDBB2000</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr">
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>FAXXXX</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -908,25 +950,33 @@
         <v>1.007</v>
       </c>
       <c r="Q6" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R6" t="n">
         <v>3.05</v>
       </c>
-      <c r="R6" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>FA19582A946244A000</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
+      <c r="T6" t="inlineStr">
         <is>
           <t>FA1956E75EBF44A000</t>
         </is>
       </c>
-      <c r="T6" t="inlineStr">
+      <c r="U6" t="inlineStr">
         <is>
           <t>FA19582C2F87C4A000</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr">
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>FAXXXX</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -986,25 +1036,33 @@
         <v>1.007</v>
       </c>
       <c r="Q7" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R7" t="n">
         <v>3.706299999999888</v>
       </c>
-      <c r="R7" t="inlineStr">
+      <c r="S7" t="inlineStr">
         <is>
           <t>FA195832F268FB2000</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
+      <c r="T7" t="inlineStr">
         <is>
           <t>FA1958EE17A944A000</t>
         </is>
       </c>
-      <c r="T7" t="inlineStr">
+      <c r="U7" t="inlineStr">
         <is>
           <t>FA19583383217B2000</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr">
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>FAXXXX</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -1064,25 +1122,33 @@
         <v>1.007</v>
       </c>
       <c r="Q8" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R8" t="n">
         <v>3.460000000000023</v>
       </c>
-      <c r="R8" t="inlineStr">
+      <c r="S8" t="inlineStr">
         <is>
           <t>FA19583495733B2000</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
+      <c r="T8" t="inlineStr">
         <is>
           <t>FA1958EED5DB3B2000</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr">
+      <c r="U8" t="inlineStr">
         <is>
           <t>FA195834E6D27B2000</t>
         </is>
       </c>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr">
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>FAXXXX</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -1093,7 +1159,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1142,25 +1208,33 @@
         <v>1.006640023500978</v>
       </c>
       <c r="Q9" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R9" t="n">
         <v>7.330000000000246</v>
       </c>
-      <c r="R9" t="inlineStr">
+      <c r="S9" t="inlineStr">
         <is>
           <t>FA195ABB6245FB2000</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
+      <c r="T9" t="inlineStr">
         <is>
           <t>FA195ABBA93BC4A000</t>
         </is>
       </c>
-      <c r="T9" t="inlineStr">
+      <c r="U9" t="inlineStr">
         <is>
           <t>FA195ABBA9777B2000</t>
         </is>
       </c>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr">
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>FAXXXX</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -1171,7 +1245,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1218,25 +1292,37 @@
         <v>1.007</v>
       </c>
       <c r="Q10" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R10" t="n">
         <v>0</v>
       </c>
-      <c r="R10" t="inlineStr">
+      <c r="S10" t="inlineStr">
         <is>
           <t>FA195AC7644AFB2000</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="T10" t="inlineStr">
         <is>
           <t>FA195ADCDD993B2000</t>
         </is>
       </c>
-      <c r="T10" t="inlineStr">
+      <c r="U10" t="inlineStr">
         <is>
           <t>FA195ADCDE0A04A000</t>
         </is>
       </c>
-      <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr">
+        <is>
+          <t>FA195D1252483B2000</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>FAXXXX</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -1247,7 +1333,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1294,25 +1380,37 @@
         <v>1.007</v>
       </c>
       <c r="Q11" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R11" t="n">
         <v>0</v>
       </c>
-      <c r="R11" t="inlineStr">
+      <c r="S11" t="inlineStr">
         <is>
           <t>FA195AC992643B2000</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr">
+      <c r="T11" t="inlineStr">
         <is>
           <t>FA195ADCDEA384A000</t>
         </is>
       </c>
-      <c r="T11" t="inlineStr">
+      <c r="U11" t="inlineStr">
         <is>
           <t>FA195ADCDFD9FB2000</t>
         </is>
       </c>
-      <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr">
+        <is>
+          <t>FA195D120DDD84A000</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>FAXXXX</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -1323,7 +1421,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1370,25 +1468,37 @@
         <v>1.007</v>
       </c>
       <c r="Q12" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R12" t="n">
         <v>0</v>
       </c>
-      <c r="R12" t="inlineStr">
+      <c r="S12" t="inlineStr">
         <is>
           <t>FA195AE1D1EF04A000</t>
         </is>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="T12" t="inlineStr">
         <is>
           <t>FA195AE220BF3B2000</t>
         </is>
       </c>
-      <c r="T12" t="inlineStr">
+      <c r="U12" t="inlineStr">
         <is>
           <t>FA195AE22108FB2000</t>
         </is>
       </c>
-      <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr">
+        <is>
+          <t>FA195D12895904A000</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>FAXXXX</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -1399,7 +1509,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="n">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1448,25 +1558,33 @@
         <v>1.007</v>
       </c>
       <c r="Q13" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R13" t="n">
         <v>3.780000000000023</v>
       </c>
-      <c r="R13" t="inlineStr">
+      <c r="S13" t="inlineStr">
         <is>
           <t>FA195AF8385384A000</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr">
+      <c r="T13" t="inlineStr">
         <is>
           <t>FA195AFE0795BB2000</t>
         </is>
       </c>
-      <c r="T13" t="inlineStr">
+      <c r="U13" t="inlineStr">
         <is>
           <t>FA195AFE07D3FB2000</t>
         </is>
       </c>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr">
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>FAXXXX</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -1477,7 +1595,7 @@
         <v>34</v>
       </c>
       <c r="B14" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1524,25 +1642,33 @@
         <v>1.007</v>
       </c>
       <c r="Q14" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R14" t="n">
         <v>0</v>
       </c>
-      <c r="R14" t="inlineStr">
+      <c r="S14" t="inlineStr">
         <is>
           <t>FA195B109E9C7B2000</t>
         </is>
       </c>
-      <c r="S14" t="inlineStr">
+      <c r="T14" t="inlineStr">
         <is>
           <t>FA195B1180D144A000</t>
         </is>
       </c>
-      <c r="T14" t="inlineStr">
+      <c r="U14" t="inlineStr">
         <is>
           <t>FA195B11811144A000</t>
         </is>
       </c>
-      <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr">
+        <is>
+          <t>FA195D120A9BBB2000</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>

</xml_diff>

<commit_message>
added  dynamic trailing stop limit order
</commit_message>
<xml_diff>
--- a/db/real_trade_db.xlsx
+++ b/db/real_trade_db.xlsx
@@ -1286,7 +1286,7 @@
         <v>1.005</v>
       </c>
       <c r="O10" t="n">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="P10" t="n">
         <v>1.007</v>
@@ -1374,7 +1374,7 @@
         <v>1.005</v>
       </c>
       <c r="O11" t="n">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="P11" t="n">
         <v>1.007</v>
@@ -1462,7 +1462,7 @@
         <v>1.005</v>
       </c>
       <c r="O12" t="n">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="P12" t="n">
         <v>1.007</v>
@@ -1636,7 +1636,7 @@
         <v>1.005</v>
       </c>
       <c r="O14" t="n">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="P14" t="n">
         <v>1.007</v>

</xml_diff>

<commit_message>
buy price defined more complicated
</commit_message>
<xml_diff>
--- a/db/real_trade_db.xlsx
+++ b/db/real_trade_db.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X14"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,7 +579,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45526.05625</v>
+        <v>45526.05630086805</v>
       </c>
       <c r="I2" t="n">
         <v>375.94</v>
@@ -602,7 +602,7 @@
         <v>1.005</v>
       </c>
       <c r="O2" t="n">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="P2" t="n">
         <v>1.007</v>
@@ -611,7 +611,7 @@
         <v>0.15</v>
       </c>
       <c r="R2" t="n">
-        <v>1.73</v>
+        <v>1.729999999999991</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
@@ -692,7 +692,7 @@
         <v>1.005</v>
       </c>
       <c r="O3" t="n">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="P3" t="n">
         <v>1.005</v>
@@ -755,13 +755,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>45524.27847222222</v>
+        <v>45521.1478715625</v>
       </c>
       <c r="I4" t="n">
-        <v>208.9</v>
+        <v>207.64</v>
       </c>
       <c r="J4" t="n">
-        <v>626.7</v>
+        <v>622.92</v>
       </c>
       <c r="K4" t="n">
         <v>1.03</v>
@@ -778,7 +778,7 @@
         <v>1.005</v>
       </c>
       <c r="O4" t="n">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="P4" t="n">
         <v>1.005</v>
@@ -787,7 +787,7 @@
         <v>0.15</v>
       </c>
       <c r="R4" t="n">
-        <v>1.09</v>
+        <v>-2.690000000000082</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
@@ -841,14 +841,16 @@
         <v>1.02</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>45526.05625</v>
-      </c>
-      <c r="I5" t="inlineStr"/>
+        <v>45526.03125480324</v>
+      </c>
+      <c r="I5" t="n">
+        <v>92.61</v>
+      </c>
       <c r="J5" t="n">
         <v>926.1</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>1.06</v>
       </c>
       <c r="L5" t="n">
         <v>10</v>
@@ -862,7 +864,7 @@
         <v>1.005</v>
       </c>
       <c r="O5" t="n">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="P5" t="n">
         <v>1.007</v>
@@ -871,7 +873,7 @@
         <v>0.15</v>
       </c>
       <c r="R5" t="n">
-        <v>3</v>
+        <v>2.620000000000045</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
@@ -921,16 +923,16 @@
         <v>1.04</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>45526.05625</v>
+        <v>45526.05752585648</v>
       </c>
       <c r="I6" t="n">
-        <v>375.94</v>
+        <v>56.51</v>
       </c>
       <c r="J6" t="n">
         <v>960.67</v>
       </c>
       <c r="K6" t="n">
-        <v>1.03</v>
+        <v>1.08</v>
       </c>
       <c r="L6" t="n">
         <v>17</v>
@@ -944,7 +946,7 @@
         <v>1.005</v>
       </c>
       <c r="O6" t="n">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="P6" t="n">
         <v>1.007</v>
@@ -953,7 +955,7 @@
         <v>0.15</v>
       </c>
       <c r="R6" t="n">
-        <v>3.05</v>
+        <v>3.002099999999932</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
@@ -1030,7 +1032,7 @@
         <v>1.005</v>
       </c>
       <c r="O7" t="n">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="P7" t="n">
         <v>1.007</v>
@@ -1116,7 +1118,7 @@
         <v>1.005</v>
       </c>
       <c r="O8" t="n">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="P8" t="n">
         <v>1.007</v>
@@ -1188,7 +1190,7 @@
         <v>1409.3</v>
       </c>
       <c r="K9" t="n">
-        <v>0.09999999999999989</v>
+        <v>0.09999999999999999</v>
       </c>
       <c r="L9" t="n">
         <v>17</v>
@@ -1202,7 +1204,7 @@
         <v>1.005</v>
       </c>
       <c r="O9" t="n">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="P9" t="n">
         <v>1.006640023500978</v>
@@ -1265,37 +1267,39 @@
         <v>0.02</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I10" t="inlineStr"/>
+        <v>45532.18769878472</v>
+      </c>
+      <c r="I10" t="n">
+        <v>253.46</v>
+      </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>1267.3</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>0.06999999999999999</v>
       </c>
       <c r="L10" t="n">
         <v>5</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N10" t="n">
         <v>1.005</v>
       </c>
       <c r="O10" t="n">
-        <v>0.93</v>
+        <v>0.97</v>
       </c>
       <c r="P10" t="n">
-        <v>1.007</v>
+        <v>1.005</v>
       </c>
       <c r="Q10" t="n">
         <v>0.15</v>
       </c>
       <c r="R10" t="n">
-        <v>0</v>
+        <v>4.795499999999866</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
@@ -1309,12 +1313,12 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>FA195ADCDE0A04A000</t>
+          <t>FA195EA9F212FB2000</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>FA195D1252483B2000</t>
+          <t>FA195EA9F212FB2000</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
@@ -1353,37 +1357,39 @@
         <v>0.02</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I11" t="inlineStr"/>
+        <v>45531.01981105324</v>
+      </c>
+      <c r="I11" t="n">
+        <v>156.6</v>
+      </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>1096.2</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="L11" t="n">
         <v>7</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N11" t="n">
         <v>1.005</v>
       </c>
       <c r="O11" t="n">
-        <v>0.93</v>
+        <v>0.97</v>
       </c>
       <c r="P11" t="n">
-        <v>1.007</v>
+        <v>1.013549948403156</v>
       </c>
       <c r="Q11" t="n">
         <v>0.15</v>
       </c>
       <c r="R11" t="n">
-        <v>0</v>
+        <v>8.530000000000127</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
@@ -1402,7 +1408,7 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>FA195D120DDD84A000</t>
+          <t>FA195ADCDFD9FB2000</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
@@ -1441,37 +1447,39 @@
         <v>0.05</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I12" t="inlineStr"/>
+        <v>45531.01995215278</v>
+      </c>
+      <c r="I12" t="n">
+        <v>54.12</v>
+      </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>974.16</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="L12" t="n">
         <v>18</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N12" t="n">
         <v>1.005</v>
       </c>
       <c r="O12" t="n">
-        <v>0.93</v>
+        <v>0.97</v>
       </c>
       <c r="P12" t="n">
-        <v>1.007</v>
+        <v>1.013327680836198</v>
       </c>
       <c r="Q12" t="n">
         <v>0.15</v>
       </c>
       <c r="R12" t="n">
-        <v>0</v>
+        <v>6.708999999999933</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
@@ -1490,7 +1498,7 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>FA195D12895904A000</t>
+          <t>FA195AE22108FB2000</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
@@ -1506,7 +1514,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B13" t="n">
         <v>11</v>
@@ -1552,7 +1560,7 @@
         <v>1.005</v>
       </c>
       <c r="O13" t="n">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="P13" t="n">
         <v>1.007</v>
@@ -1592,7 +1600,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B14" t="n">
         <v>12</v>
@@ -1615,28 +1623,30 @@
         <v>0.02</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I14" t="inlineStr"/>
+        <v>45530.89049074074</v>
+      </c>
+      <c r="I14" t="n">
+        <v>166.95</v>
+      </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>834.75</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="L14" t="n">
         <v>5</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N14" t="n">
         <v>1.005</v>
       </c>
       <c r="O14" t="n">
-        <v>0.93</v>
+        <v>0.97</v>
       </c>
       <c r="P14" t="n">
         <v>1.007</v>
@@ -1645,7 +1655,7 @@
         <v>0.15</v>
       </c>
       <c r="R14" t="n">
-        <v>0</v>
+        <v>4.93400000000002</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
@@ -1664,11 +1674,1101 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>FA195D120A9BBB2000</t>
+          <t>FA195E5F46693B2000</t>
         </is>
       </c>
       <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>BSX</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>45530.97930672453</v>
+      </c>
+      <c r="E15" t="n">
+        <v>79.02</v>
+      </c>
+      <c r="F15" t="n">
+        <v>790.1999999999999</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>45531.03027651621</v>
+      </c>
+      <c r="I15" t="n">
+        <v>79.41</v>
+      </c>
+      <c r="J15" t="n">
+        <v>794.0999999999999</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L15" t="n">
+        <v>10</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="P15" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R15" t="n">
+        <v>3.809999999999977</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>FA195E950EC684A000</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>FA195E95F6D67B2000</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>FA195E95F6D67B2000</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>FA195E96E5E044A000</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>7</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>PYPL</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>45530.98132490741</v>
+      </c>
+      <c r="E16" t="n">
+        <v>71.70959999999999</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1434.192</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>45531.02524922453</v>
+      </c>
+      <c r="I16" t="n">
+        <v>72.2608</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1445.216</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L16" t="n">
+        <v>20</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="P16" t="n">
+        <v>1.008279092339101</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R16" t="n">
+        <v>10.85400000000011</v>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>FA195E95B90EBB2000</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>FA195E9670D744A000</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>FA195E9670D744A000</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>FA195E96E53F84A000</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>10</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>INTU</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>45530.98640965277</v>
+      </c>
+      <c r="E17" t="n">
+        <v>620.21</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2474.36</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>45532.15297071759</v>
+      </c>
+      <c r="I17" t="n">
+        <v>621.8200000000001</v>
+      </c>
+      <c r="J17" t="n">
+        <v>2487.28</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="L17" t="n">
+        <v>4</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="P17" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R17" t="n">
+        <v>11.71900000000007</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>FA195E976617C4A000</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>FA195EA9F51404A000</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>FA1960089A40BB2000</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>30</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>IDXX</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>45530.99175415509</v>
+      </c>
+      <c r="E18" t="n">
+        <v>487.87</v>
+      </c>
+      <c r="F18" t="n">
+        <v>975.74</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>45531.04146706018</v>
+      </c>
+      <c r="I18" t="n">
+        <v>489.53</v>
+      </c>
+      <c r="J18" t="n">
+        <v>979.0599999999999</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="L18" t="n">
+        <v>2</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="P18" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R18" t="n">
+        <v>3.259999999999937</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>FA195E992905BB2000</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>FA195E9A2240BB2000</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>FA195E9A279E7B2000</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>FA195E9B8DAC84A000</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>35</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>AVGO</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>45532.11452482639</v>
+      </c>
+      <c r="E19" t="n">
+        <v>159.64</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1436.76</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>45532.15930564815</v>
+      </c>
+      <c r="I19" t="n">
+        <v>160.5009</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1444.5081</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L19" t="n">
+        <v>9</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="P19" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R19" t="n">
+        <v>7.638100000000022</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>FA19600B36CFFB2000</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>FA19600C095384A000</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>FA19600C095384A000</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>FA19600C7A8FC4A000</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>54</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>HLT</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>45532.12140657407</v>
+      </c>
+      <c r="E20" t="n">
+        <v>218.22</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1309.32</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>45532.22512471065</v>
+      </c>
+      <c r="I20" t="n">
+        <v>219.0016</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1314.0096</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.06999999999999999</v>
+      </c>
+      <c r="L20" t="n">
+        <v>6</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="P20" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R20" t="n">
+        <v>4.599599999999928</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>FA19600D7B73FB2000</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>FA19600F6A8344A000</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>FA19600F6AF17B2000</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>115</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>45532.14689203704</v>
+      </c>
+      <c r="E21" t="n">
+        <v>149.8292</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1348.4628</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>45532.31330984954</v>
+      </c>
+      <c r="I21" t="n">
+        <v>150.2605</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1352.3445</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L21" t="n">
+        <v>9</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N21" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="P21" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R21" t="n">
+        <v>3.771700000000137</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>FA196015E1C77B2000</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>FA196016F6A2FB2000</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>FA196016F716C4A000</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>FA1960381EC3BB2000</t>
+        </is>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>218</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>IDXX</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>45532.1707453125</v>
+      </c>
+      <c r="E22" t="n">
+        <v>482.72</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1448.16</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>45533.02499002315</v>
+      </c>
+      <c r="I22" t="n">
+        <v>484.08</v>
+      </c>
+      <c r="J22" t="n">
+        <v>1452.24</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1.101</v>
+      </c>
+      <c r="L22" t="n">
+        <v>3</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N22" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="P22" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R22" t="n">
+        <v>2.968999999999927</v>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>FA19601DBE643B2000</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>FA1960388FBF44A000</t>
+        </is>
+      </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>FA196038902FC4A000</t>
+        </is>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>FA19612852A8FB2000</t>
+        </is>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>227</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ANET</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>45532.17232325231</v>
+      </c>
+      <c r="E23" t="n">
+        <v>345.42</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1381.68</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>45533.01956805556</v>
+      </c>
+      <c r="I23" t="n">
+        <v>345.81</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1383.24</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L23" t="n">
+        <v>4</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N23" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="P23" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R23" t="n">
+        <v>1.489999999999945</v>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>FA19601E4388C4A000</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>FA19603890CAC4A000</t>
+        </is>
+      </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>FA196038914404A000</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>FA19612855533B2000</t>
+        </is>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B24" t="n">
+        <v>236</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ANET</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>45532.98230893518</v>
+      </c>
+      <c r="E24" t="n">
+        <v>344.96</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1379.84</v>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>4</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N24" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P24" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>FA1961293A04C4A000</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>FA19612A070244A000</t>
+        </is>
+      </c>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>FA19612A0765BB2000</t>
+        </is>
+      </c>
+      <c r="W24" t="inlineStr"/>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B25" t="n">
+        <v>240</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>SHW</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>45532.98296216435</v>
+      </c>
+      <c r="E25" t="n">
+        <v>360.13</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1440.52</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>45533.03831487268</v>
+      </c>
+      <c r="I25" t="n">
+        <v>362.21</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1448.84</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L25" t="n">
+        <v>4</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N25" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P25" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R25" t="n">
+        <v>8.249999999999936</v>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>FA196129712444A000</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr"/>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>FA19612B11D2FB2000</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>FA19612B121FC4A000</t>
+        </is>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>FA19612CA0AEBB2000</t>
+        </is>
+      </c>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B26" t="n">
+        <v>243</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ETN</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>45532.98513773148</v>
+      </c>
+      <c r="E26" t="n">
+        <v>296.17</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1184.68</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>4</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N26" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P26" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>FA19612A28B3BB2000</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr"/>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>FA19612ACBAA7B2000</t>
+        </is>
+      </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>FA19612ACBF83B2000</t>
+        </is>
+      </c>
+      <c r="W26" t="inlineStr"/>
+      <c r="X26" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B27" t="n">
+        <v>342</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>SCHW</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>45533.02051811342</v>
+      </c>
+      <c r="E27" t="n">
+        <v>63.81</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1403.82</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>22</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N27" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P27" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>FA196135D1E5C4A000</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr"/>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>FA19613654C2BB2000</t>
+        </is>
+      </c>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>FA1961365517BB2000</t>
+        </is>
+      </c>
+      <c r="W27" t="inlineStr"/>
+      <c r="X27" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>

</xml_diff>

<commit_message>
added buy condition 1m
</commit_message>
<xml_diff>
--- a/db/real_trade_db.xlsx
+++ b/db/real_trade_db.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X39"/>
+  <dimension ref="A1:Y39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -550,6 +550,11 @@
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
+          <t>buy_condition_type</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
           <t>timezone</t>
         </is>
       </c>
@@ -640,6 +645,11 @@
       </c>
       <c r="X2" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -726,6 +736,11 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -812,6 +827,11 @@
       </c>
       <c r="X4" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -894,6 +914,11 @@
       </c>
       <c r="X5" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -980,6 +1005,11 @@
       </c>
       <c r="X6" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -1066,6 +1096,11 @@
       </c>
       <c r="X7" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -1152,6 +1187,11 @@
       </c>
       <c r="X8" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -1238,6 +1278,11 @@
       </c>
       <c r="X9" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -1328,6 +1373,11 @@
       </c>
       <c r="X10" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -1418,6 +1468,11 @@
       </c>
       <c r="X11" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -1508,6 +1563,11 @@
       </c>
       <c r="X12" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -1594,6 +1654,11 @@
       </c>
       <c r="X13" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -1680,6 +1745,11 @@
       <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -1766,6 +1836,11 @@
       </c>
       <c r="X15" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -1852,6 +1927,11 @@
       </c>
       <c r="X16" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -1934,6 +2014,11 @@
       </c>
       <c r="X17" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -2020,6 +2105,11 @@
       </c>
       <c r="X18" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -2106,6 +2196,11 @@
       </c>
       <c r="X19" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -2188,6 +2283,11 @@
       <c r="W20" t="inlineStr"/>
       <c r="X20" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -2274,6 +2374,11 @@
       </c>
       <c r="X21" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -2360,6 +2465,11 @@
       </c>
       <c r="X22" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -2446,6 +2556,11 @@
       </c>
       <c r="X23" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -2524,6 +2639,11 @@
       <c r="W24" t="inlineStr"/>
       <c r="X24" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y24" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -2610,6 +2730,11 @@
       </c>
       <c r="X25" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y25" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -2692,6 +2817,11 @@
       <c r="W26" t="inlineStr"/>
       <c r="X26" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -2774,6 +2904,11 @@
       <c r="W27" t="inlineStr"/>
       <c r="X27" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -2860,6 +2995,11 @@
       </c>
       <c r="X28" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -2946,6 +3086,11 @@
       </c>
       <c r="X29" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -3032,6 +3177,11 @@
       </c>
       <c r="X30" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
@@ -3112,13 +3262,18 @@
       <c r="W31" t="inlineStr"/>
       <c r="X31" t="inlineStr">
         <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
           <t>E. Australia Standard Time</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B32" t="n">
         <v>574</v>
@@ -3197,6 +3352,11 @@
         </is>
       </c>
       <c r="X32" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y32" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -3204,7 +3364,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B33" t="n">
         <v>601</v>
@@ -3279,6 +3439,11 @@
       </c>
       <c r="W33" t="inlineStr"/>
       <c r="X33" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y33" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -3286,7 +3451,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B34" t="n">
         <v>1</v>
@@ -3365,6 +3530,11 @@
         </is>
       </c>
       <c r="X34" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y34" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -3372,7 +3542,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B35" t="n">
         <v>10</v>
@@ -3451,6 +3621,11 @@
         </is>
       </c>
       <c r="X35" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y35" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -3458,7 +3633,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B36" t="n">
         <v>23</v>
@@ -3537,6 +3712,11 @@
         </is>
       </c>
       <c r="X36" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y36" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -3544,7 +3724,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>92</v>
+        <v>35</v>
       </c>
       <c r="B37" t="n">
         <v>13</v>
@@ -3623,6 +3803,11 @@
         </is>
       </c>
       <c r="X37" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y37" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -3630,7 +3815,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>110</v>
+        <v>36</v>
       </c>
       <c r="B38" t="n">
         <v>4</v>
@@ -3709,6 +3894,11 @@
         </is>
       </c>
       <c r="X38" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y38" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>
@@ -3716,7 +3906,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>333</v>
+        <v>37</v>
       </c>
       <c r="B39" t="n">
         <v>185</v>
@@ -3787,6 +3977,11 @@
         </is>
       </c>
       <c r="X39" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y39" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>

</xml_diff>

<commit_message>
added norm100 and befor market opening condition
</commit_message>
<xml_diff>
--- a/db/real_trade_db.xlsx
+++ b/db/real_trade_db.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA269"/>
+  <dimension ref="A1:AA276"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>stop_limit_sell_order_id</t>
+          <t>stop_limit_order_id</t>
         </is>
       </c>
     </row>
@@ -25959,6 +25959,617 @@
       </c>
       <c r="AA269" t="inlineStr"/>
     </row>
+    <row r="270">
+      <c r="A270" s="1" t="n">
+        <v>268</v>
+      </c>
+      <c r="B270" t="n">
+        <v>290</v>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>FTNT</t>
+        </is>
+      </c>
+      <c r="D270" s="2" t="n">
+        <v>45580.18006612269</v>
+      </c>
+      <c r="E270" t="n">
+        <v>82.5492</v>
+      </c>
+      <c r="F270" t="n">
+        <v>3136.8696</v>
+      </c>
+      <c r="G270" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H270" s="2" t="n">
+        <v>45580.28755964121</v>
+      </c>
+      <c r="I270" t="n">
+        <v>82.66030000000001</v>
+      </c>
+      <c r="J270" t="n">
+        <v>3141.0914</v>
+      </c>
+      <c r="K270" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="L270" t="n">
+        <v>38</v>
+      </c>
+      <c r="M270" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N270" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O270" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P270" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q270" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="R270" t="n">
+        <v>1.921800000000257</v>
+      </c>
+      <c r="S270" t="inlineStr">
+        <is>
+          <t>FA199DDF65447B2000</t>
+        </is>
+      </c>
+      <c r="T270" t="inlineStr"/>
+      <c r="U270" t="inlineStr"/>
+      <c r="V270" t="inlineStr"/>
+      <c r="W270" t="inlineStr">
+        <is>
+          <t>FA199DE6C57A44A000</t>
+        </is>
+      </c>
+      <c r="X270" t="inlineStr">
+        <is>
+          <t>1230</t>
+        </is>
+      </c>
+      <c r="Y270" t="inlineStr">
+        <is>
+          <t>mv :-1.14, mv_2m:-0.15,      mv_5m : -0.21, mv_30m : -0.60, mv_60m: -0.05</t>
+        </is>
+      </c>
+      <c r="Z270" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA270" t="inlineStr"/>
+    </row>
+    <row r="271">
+      <c r="A271" s="1" t="n">
+        <v>269</v>
+      </c>
+      <c r="B271" t="n">
+        <v>293</v>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>CMG</t>
+        </is>
+      </c>
+      <c r="D271" s="2" t="n">
+        <v>45581.15869940972</v>
+      </c>
+      <c r="E271" t="n">
+        <v>59.72</v>
+      </c>
+      <c r="F271" t="n">
+        <v>3165.16</v>
+      </c>
+      <c r="G271" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="H271" s="2" t="n">
+        <v>45581.28762678241</v>
+      </c>
+      <c r="I271" t="n">
+        <v>59.9001</v>
+      </c>
+      <c r="J271" t="n">
+        <v>3174.7053</v>
+      </c>
+      <c r="K271" t="n">
+        <v>1.101</v>
+      </c>
+      <c r="L271" t="n">
+        <v>53</v>
+      </c>
+      <c r="M271" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N271" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O271" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P271" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q271" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="R271" t="n">
+        <v>7.294300000000224</v>
+      </c>
+      <c r="S271" t="inlineStr">
+        <is>
+          <t>FA199F21F15A44A000</t>
+        </is>
+      </c>
+      <c r="T271" t="inlineStr"/>
+      <c r="U271" t="inlineStr"/>
+      <c r="V271" t="inlineStr"/>
+      <c r="W271" t="inlineStr">
+        <is>
+          <t>FA199F2BC9BBBB2000</t>
+        </is>
+      </c>
+      <c r="X271" t="inlineStr">
+        <is>
+          <t>1230</t>
+        </is>
+      </c>
+      <c r="Y271" t="inlineStr">
+        <is>
+          <t>mv :-22.67, mv_2m:-0.50,      mv_5m : -1.72, mv_30m : 1.23, mv_60m: 3.43</t>
+        </is>
+      </c>
+      <c r="Z271" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA271" t="inlineStr"/>
+    </row>
+    <row r="272">
+      <c r="A272" s="1" t="n">
+        <v>270</v>
+      </c>
+      <c r="B272" t="n">
+        <v>295</v>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>BAC</t>
+        </is>
+      </c>
+      <c r="D272" s="2" t="n">
+        <v>45582.17252115741</v>
+      </c>
+      <c r="E272" t="n">
+        <v>42.915</v>
+      </c>
+      <c r="F272" t="n">
+        <v>3175.71</v>
+      </c>
+      <c r="G272" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="H272" s="2" t="n">
+        <v>45582.24687973379</v>
+      </c>
+      <c r="I272" t="n">
+        <v>42.975</v>
+      </c>
+      <c r="J272" t="n">
+        <v>3180.15</v>
+      </c>
+      <c r="K272" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="L272" t="n">
+        <v>74</v>
+      </c>
+      <c r="M272" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N272" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O272" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P272" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q272" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="R272" t="n">
+        <v>1.920000000000055</v>
+      </c>
+      <c r="S272" t="inlineStr">
+        <is>
+          <t>FA19A070169E04A000</t>
+        </is>
+      </c>
+      <c r="T272" t="inlineStr"/>
+      <c r="U272" t="inlineStr"/>
+      <c r="V272" t="inlineStr"/>
+      <c r="W272" t="inlineStr">
+        <is>
+          <t>FA19A07897EE7B2000</t>
+        </is>
+      </c>
+      <c r="X272" t="inlineStr">
+        <is>
+          <t>1230</t>
+        </is>
+      </c>
+      <c r="Y272" t="inlineStr">
+        <is>
+          <t>mv :-1.77, mv_2m:-0.15,      mv_5m : -0.28, mv_30m : -1.13, mv_60m: -2.30</t>
+        </is>
+      </c>
+      <c r="Z272" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA272" t="inlineStr"/>
+    </row>
+    <row r="273">
+      <c r="A273" s="1" t="n">
+        <v>271</v>
+      </c>
+      <c r="B273" t="n">
+        <v>298</v>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>ADSK</t>
+        </is>
+      </c>
+      <c r="D273" s="2" t="n">
+        <v>45582.2124253125</v>
+      </c>
+      <c r="E273" t="n">
+        <v>287.83</v>
+      </c>
+      <c r="F273" t="n">
+        <v>3166.13</v>
+      </c>
+      <c r="G273" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="H273" s="2" t="n">
+        <v>45582.28688711805</v>
+      </c>
+      <c r="I273" t="n">
+        <v>288.39</v>
+      </c>
+      <c r="J273" t="n">
+        <v>3172.29</v>
+      </c>
+      <c r="K273" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="L273" t="n">
+        <v>11</v>
+      </c>
+      <c r="M273" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N273" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O273" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P273" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q273" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="R273" t="n">
+        <v>4.02000000000031</v>
+      </c>
+      <c r="S273" t="inlineStr">
+        <is>
+          <t>FA19A07D3D8B3B2000</t>
+        </is>
+      </c>
+      <c r="T273" t="inlineStr"/>
+      <c r="U273" t="inlineStr"/>
+      <c r="V273" t="inlineStr"/>
+      <c r="W273" t="inlineStr">
+        <is>
+          <t>FA19A081561684A000</t>
+        </is>
+      </c>
+      <c r="X273" t="inlineStr">
+        <is>
+          <t>1230</t>
+        </is>
+      </c>
+      <c r="Y273" t="inlineStr">
+        <is>
+          <t>mv :-1.50, mv_2m:0.41,      mv_5m : 0.26, mv_30m : 0.60, mv_60m: 0.35</t>
+        </is>
+      </c>
+      <c r="Z273" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA273" t="inlineStr"/>
+    </row>
+    <row r="274">
+      <c r="A274" s="1" t="n">
+        <v>274</v>
+      </c>
+      <c r="B274" t="n">
+        <v>301</v>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>TT</t>
+        </is>
+      </c>
+      <c r="D274" s="2" t="n">
+        <v>45583.1528390625</v>
+      </c>
+      <c r="E274" t="n">
+        <v>401.62</v>
+      </c>
+      <c r="F274" t="n">
+        <v>3212.96</v>
+      </c>
+      <c r="G274" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H274" s="2" t="n">
+        <v>45583.28773255787</v>
+      </c>
+      <c r="I274" t="n">
+        <v>401.35</v>
+      </c>
+      <c r="J274" t="n">
+        <v>3210.8</v>
+      </c>
+      <c r="K274" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="L274" t="n">
+        <v>8</v>
+      </c>
+      <c r="M274" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N274" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O274" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P274" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q274" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="R274" t="n">
+        <v>-4.279999999999855</v>
+      </c>
+      <c r="S274" t="inlineStr">
+        <is>
+          <t>FA19A1B3310AC4A000</t>
+        </is>
+      </c>
+      <c r="T274" t="inlineStr"/>
+      <c r="U274" t="inlineStr"/>
+      <c r="V274" t="inlineStr"/>
+      <c r="W274" t="inlineStr">
+        <is>
+          <t>FA19A1D24FB7BB2000</t>
+        </is>
+      </c>
+      <c r="X274" t="inlineStr">
+        <is>
+          <t>1230</t>
+        </is>
+      </c>
+      <c r="Y274" t="inlineStr">
+        <is>
+          <t>mv :0.89, mv_2m:0.81,      mv_5m : 1.66, mv_30m : -1.27, mv_60m: -1.63</t>
+        </is>
+      </c>
+      <c r="Z274" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA274" t="inlineStr"/>
+    </row>
+    <row r="275">
+      <c r="A275" s="1" t="n">
+        <v>275</v>
+      </c>
+      <c r="B275" t="n">
+        <v>302</v>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>CHTR</t>
+        </is>
+      </c>
+      <c r="D275" s="2" t="n">
+        <v>45583.16485706018</v>
+      </c>
+      <c r="E275" t="n">
+        <v>328.87</v>
+      </c>
+      <c r="F275" t="n">
+        <v>2959.83</v>
+      </c>
+      <c r="G275" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="H275" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I275" t="inlineStr"/>
+      <c r="J275" t="n">
+        <v>0</v>
+      </c>
+      <c r="K275" t="n">
+        <v>0</v>
+      </c>
+      <c r="L275" t="n">
+        <v>9</v>
+      </c>
+      <c r="M275" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N275" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O275" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P275" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q275" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="R275" t="n">
+        <v>0</v>
+      </c>
+      <c r="S275" t="inlineStr">
+        <is>
+          <t>FA19A1B7270C7B2000</t>
+        </is>
+      </c>
+      <c r="T275" t="inlineStr"/>
+      <c r="U275" t="inlineStr"/>
+      <c r="V275" t="inlineStr"/>
+      <c r="W275" t="inlineStr"/>
+      <c r="X275" t="inlineStr">
+        <is>
+          <t>1230</t>
+        </is>
+      </c>
+      <c r="Y275" t="inlineStr">
+        <is>
+          <t>mv :3.49, mv_2m:0.07,      mv_5m : 0.03, mv_30m : 0.88, mv_60m: 0.35</t>
+        </is>
+      </c>
+      <c r="Z275" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA275" t="inlineStr"/>
+    </row>
+    <row r="276">
+      <c r="A276" s="1" t="n">
+        <v>276</v>
+      </c>
+      <c r="B276" t="n">
+        <v>303</v>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>AMAT</t>
+        </is>
+      </c>
+      <c r="D276" s="2" t="n">
+        <v>45583.27386659722</v>
+      </c>
+      <c r="E276" t="n">
+        <v>203.21</v>
+      </c>
+      <c r="F276" t="n">
+        <v>3251.36</v>
+      </c>
+      <c r="G276" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H276" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I276" t="inlineStr"/>
+      <c r="J276" t="n">
+        <v>0</v>
+      </c>
+      <c r="K276" t="n">
+        <v>0</v>
+      </c>
+      <c r="L276" t="n">
+        <v>16</v>
+      </c>
+      <c r="M276" t="inlineStr">
+        <is>
+          <t>placed</t>
+        </is>
+      </c>
+      <c r="N276" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="O276" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P276" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q276" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="R276" t="n">
+        <v>0</v>
+      </c>
+      <c r="S276" t="inlineStr">
+        <is>
+          <t>FA19A1DB14AABB2000</t>
+        </is>
+      </c>
+      <c r="T276" t="inlineStr"/>
+      <c r="U276" t="inlineStr"/>
+      <c r="V276" t="inlineStr"/>
+      <c r="W276" t="inlineStr"/>
+      <c r="X276" t="inlineStr">
+        <is>
+          <t>speed_norm100</t>
+        </is>
+      </c>
+      <c r="Y276" t="inlineStr">
+        <is>
+          <t>mv :0.16, mv_2m:-0.29,      mv_5m : -0.02, mv_30m : -1.16, mv_60m: -0.20</t>
+        </is>
+      </c>
+      <c r="Z276" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA276" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added MA50_MA5 condition and stock exclusion
</commit_message>
<xml_diff>
--- a/db/real_trade_db.xlsx
+++ b/db/real_trade_db.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA820"/>
+  <dimension ref="A1:AA828"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27940,7 +27940,7 @@
         <v>1.006</v>
       </c>
       <c r="Q291" t="n">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="R291" t="n">
         <v>0</v>
@@ -71787,21 +71787,23 @@
         <v>1.03</v>
       </c>
       <c r="H817" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I817" t="inlineStr"/>
+        <v>45741.06419210648</v>
+      </c>
+      <c r="I817" t="n">
+        <v>264.97</v>
+      </c>
       <c r="J817" t="n">
-        <v>0</v>
+        <v>3179.64</v>
       </c>
       <c r="K817" t="n">
-        <v>0</v>
+        <v>1.13</v>
       </c>
       <c r="L817" t="n">
         <v>12</v>
       </c>
       <c r="M817" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N817" t="n">
@@ -71811,13 +71813,13 @@
         <v>1.005</v>
       </c>
       <c r="P817" t="n">
-        <v>1.006</v>
+        <v>1.0075</v>
       </c>
       <c r="Q817" t="n">
         <v>0.15</v>
       </c>
       <c r="R817" t="n">
-        <v>0</v>
+        <v>51.24000000000054</v>
       </c>
       <c r="S817" t="inlineStr">
         <is>
@@ -71940,7 +71942,7 @@
     </row>
     <row r="819">
       <c r="A819" s="1" t="n">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B819" t="n">
         <v>4113</v>
@@ -72029,7 +72031,7 @@
     </row>
     <row r="820">
       <c r="A820" s="1" t="n">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B820" t="n">
         <v>4114</v>
@@ -72052,21 +72054,23 @@
         <v>1.02</v>
       </c>
       <c r="H820" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I820" t="inlineStr"/>
+        <v>45741.02655521991</v>
+      </c>
+      <c r="I820" t="n">
+        <v>305.69</v>
+      </c>
       <c r="J820" t="n">
-        <v>0</v>
+        <v>2751.21</v>
       </c>
       <c r="K820" t="n">
-        <v>0</v>
+        <v>1.11</v>
       </c>
       <c r="L820" t="n">
         <v>9</v>
       </c>
       <c r="M820" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N820" t="n">
@@ -72076,13 +72080,13 @@
         <v>1.0001</v>
       </c>
       <c r="P820" t="n">
-        <v>1.006</v>
+        <v>1.0065</v>
       </c>
       <c r="Q820" t="n">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="R820" t="n">
-        <v>0</v>
+        <v>6.13110000000017</v>
       </c>
       <c r="S820" t="inlineStr">
         <is>
@@ -72114,6 +72118,740 @@
       </c>
       <c r="AA820" t="inlineStr"/>
     </row>
+    <row r="821">
+      <c r="A821" s="1" t="n">
+        <v>819</v>
+      </c>
+      <c r="B821" t="n">
+        <v>4115</v>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>CB</t>
+        </is>
+      </c>
+      <c r="D821" s="2" t="n">
+        <v>45741.14519493056</v>
+      </c>
+      <c r="E821" t="n">
+        <v>291.59</v>
+      </c>
+      <c r="F821" t="n">
+        <v>3207.49</v>
+      </c>
+      <c r="G821" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="H821" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I821" t="inlineStr"/>
+      <c r="J821" t="n">
+        <v>0</v>
+      </c>
+      <c r="K821" t="n">
+        <v>0</v>
+      </c>
+      <c r="L821" t="n">
+        <v>11</v>
+      </c>
+      <c r="M821" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N821" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="O821" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P821" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q821" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="R821" t="n">
+        <v>0</v>
+      </c>
+      <c r="S821" t="inlineStr">
+        <is>
+          <t>FA1A6D1BDE37BB2000</t>
+        </is>
+      </c>
+      <c r="T821" t="inlineStr">
+        <is>
+          <t>FA1A6D1C31003B2000</t>
+        </is>
+      </c>
+      <c r="U821" t="inlineStr"/>
+      <c r="V821" t="inlineStr"/>
+      <c r="W821" t="inlineStr">
+        <is>
+          <t>FA1A6D1C9BDC44A000</t>
+        </is>
+      </c>
+      <c r="X821" t="inlineStr">
+        <is>
+          <t>MA60_MA5</t>
+        </is>
+      </c>
+      <c r="Y821" t="inlineStr">
+        <is>
+          <t>mv :-0.92, mv_2m:0.08,      mv_5m : 0.03, mv_30m : -0.05, mv_60m: 0.21</t>
+        </is>
+      </c>
+      <c r="Z821" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA821" t="inlineStr">
+        <is>
+          <t>FA1A6D1C31CAC4A000</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" s="1" t="n">
+        <v>820</v>
+      </c>
+      <c r="B822" t="n">
+        <v>4116</v>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>INTC</t>
+        </is>
+      </c>
+      <c r="D822" s="2" t="n">
+        <v>45741.20273938657</v>
+      </c>
+      <c r="E822" t="n">
+        <v>24.197</v>
+      </c>
+      <c r="F822" t="n">
+        <v>3000.428</v>
+      </c>
+      <c r="G822" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="H822" s="2" t="n">
+        <v>45741.83583892361</v>
+      </c>
+      <c r="I822" t="n">
+        <v>24.1</v>
+      </c>
+      <c r="J822" t="n">
+        <v>2988.4</v>
+      </c>
+      <c r="K822" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="L822" t="n">
+        <v>124</v>
+      </c>
+      <c r="M822" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N822" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="O822" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P822" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q822" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="R822" t="n">
+        <v>-14.84799999999979</v>
+      </c>
+      <c r="S822" t="inlineStr">
+        <is>
+          <t>FA1A6D2ED58A3B2000</t>
+        </is>
+      </c>
+      <c r="T822" t="inlineStr">
+        <is>
+          <t>FA1A6D2F102CBB2000</t>
+        </is>
+      </c>
+      <c r="U822" t="inlineStr"/>
+      <c r="V822" t="inlineStr"/>
+      <c r="W822" t="inlineStr">
+        <is>
+          <t>FA1A6D3F86DF04A000</t>
+        </is>
+      </c>
+      <c r="X822" t="inlineStr">
+        <is>
+          <t>MA60_MA5</t>
+        </is>
+      </c>
+      <c r="Y822" t="inlineStr">
+        <is>
+          <t>mv :-5.16, mv_2m:0.03,      mv_5m : -0.11, mv_30m : -0.18, mv_60m: -3.92</t>
+        </is>
+      </c>
+      <c r="Z822" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA822" t="inlineStr">
+        <is>
+          <t>FA1A6D2F10E984A000</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" s="1" t="n">
+        <v>821</v>
+      </c>
+      <c r="B823" t="n">
+        <v>4117</v>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>LMT</t>
+        </is>
+      </c>
+      <c r="D823" s="2" t="n">
+        <v>45742.01280428241</v>
+      </c>
+      <c r="E823" t="n">
+        <v>432.71</v>
+      </c>
+      <c r="F823" t="n">
+        <v>2596.26</v>
+      </c>
+      <c r="G823" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H823" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I823" t="inlineStr"/>
+      <c r="J823" t="n">
+        <v>0</v>
+      </c>
+      <c r="K823" t="n">
+        <v>0</v>
+      </c>
+      <c r="L823" t="n">
+        <v>6</v>
+      </c>
+      <c r="M823" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N823" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="O823" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="P823" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q823" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="R823" t="n">
+        <v>0</v>
+      </c>
+      <c r="S823" t="inlineStr">
+        <is>
+          <t>FA1A6E39D2E93B2000</t>
+        </is>
+      </c>
+      <c r="T823" t="inlineStr"/>
+      <c r="U823" t="inlineStr"/>
+      <c r="V823" t="inlineStr"/>
+      <c r="W823" t="inlineStr"/>
+      <c r="X823" t="inlineStr">
+        <is>
+          <t>before_market_open_2</t>
+        </is>
+      </c>
+      <c r="Y823" t="inlineStr">
+        <is>
+          <t>mv :-11.10, mv_2m:-0.47,      mv_5m : 1.37, mv_30m : -7.03, mv_60m: -14.15</t>
+        </is>
+      </c>
+      <c r="Z823" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA823" t="inlineStr"/>
+    </row>
+    <row r="824">
+      <c r="A824" s="1" t="n">
+        <v>822</v>
+      </c>
+      <c r="B824" t="n">
+        <v>4119</v>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>ETN</t>
+        </is>
+      </c>
+      <c r="D824" s="2" t="n">
+        <v>45742.19684638889</v>
+      </c>
+      <c r="E824" t="n">
+        <v>299.5</v>
+      </c>
+      <c r="F824" t="n">
+        <v>3294.5</v>
+      </c>
+      <c r="G824" t="inlineStr"/>
+      <c r="H824" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I824" t="inlineStr"/>
+      <c r="J824" t="n">
+        <v>0</v>
+      </c>
+      <c r="K824" t="n">
+        <v>0</v>
+      </c>
+      <c r="L824" t="n">
+        <v>11</v>
+      </c>
+      <c r="M824" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N824" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O824" t="n">
+        <v>1.0001</v>
+      </c>
+      <c r="P824" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q824" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="R824" t="n">
+        <v>0</v>
+      </c>
+      <c r="S824" t="inlineStr">
+        <is>
+          <t>FA1A6E767B017B2000</t>
+        </is>
+      </c>
+      <c r="T824" t="inlineStr"/>
+      <c r="U824" t="inlineStr"/>
+      <c r="V824" t="inlineStr"/>
+      <c r="W824" t="inlineStr"/>
+      <c r="X824" t="inlineStr">
+        <is>
+          <t>1230</t>
+        </is>
+      </c>
+      <c r="Y824" t="inlineStr">
+        <is>
+          <t>mv :-31.71, mv_2m:0.40,      mv_5m : 1.20, mv_30m : -2.38, mv_60m: -3.82</t>
+        </is>
+      </c>
+      <c r="Z824" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA824" t="inlineStr"/>
+    </row>
+    <row r="825">
+      <c r="A825" s="1" t="n">
+        <v>823</v>
+      </c>
+      <c r="B825" t="n">
+        <v>4120</v>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>KLAC</t>
+        </is>
+      </c>
+      <c r="D825" s="2" t="n">
+        <v>45742.26677307871</v>
+      </c>
+      <c r="E825" t="n">
+        <v>720.85</v>
+      </c>
+      <c r="F825" t="n">
+        <v>2883.4</v>
+      </c>
+      <c r="G825" t="n">
+        <v>1</v>
+      </c>
+      <c r="H825" s="2" t="n">
+        <v>45743.07161030093</v>
+      </c>
+      <c r="I825" t="n">
+        <v>712.42</v>
+      </c>
+      <c r="J825" t="n">
+        <v>2849.68</v>
+      </c>
+      <c r="K825" t="n">
+        <v>1.101</v>
+      </c>
+      <c r="L825" t="n">
+        <v>4</v>
+      </c>
+      <c r="M825" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N825" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="O825" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P825" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q825" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="R825" t="n">
+        <v>-35.82100000000025</v>
+      </c>
+      <c r="S825" t="inlineStr">
+        <is>
+          <t>FA1A6E8D876284A000</t>
+        </is>
+      </c>
+      <c r="T825" t="inlineStr">
+        <is>
+          <t>FA1A6E8DD32D04A000</t>
+        </is>
+      </c>
+      <c r="U825" t="inlineStr"/>
+      <c r="V825" t="inlineStr"/>
+      <c r="W825" t="inlineStr">
+        <is>
+          <t>FA1A6E90522904A000</t>
+        </is>
+      </c>
+      <c r="X825" t="inlineStr">
+        <is>
+          <t>MA60_MA5</t>
+        </is>
+      </c>
+      <c r="Y825" t="inlineStr">
+        <is>
+          <t>mv :-37.17, mv_2m:-0.96,      mv_5m : -0.15, mv_30m : 4.66, mv_60m: -7.47</t>
+        </is>
+      </c>
+      <c r="Z825" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA825" t="inlineStr">
+        <is>
+          <t>FA1A6E8DD3D884A000</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" s="1" t="n">
+        <v>824</v>
+      </c>
+      <c r="B826" t="n">
+        <v>4121</v>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>AMAT</t>
+        </is>
+      </c>
+      <c r="D826" s="2" t="n">
+        <v>45743.09739583333</v>
+      </c>
+      <c r="E826" t="n">
+        <v>152.134</v>
+      </c>
+      <c r="F826" t="n">
+        <v>2738.412</v>
+      </c>
+      <c r="G826" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="H826" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I826" t="inlineStr"/>
+      <c r="J826" t="n">
+        <v>0</v>
+      </c>
+      <c r="K826" t="n">
+        <v>0</v>
+      </c>
+      <c r="L826" t="n">
+        <v>18</v>
+      </c>
+      <c r="M826" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N826" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="O826" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P826" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q826" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="R826" t="n">
+        <v>0</v>
+      </c>
+      <c r="S826" t="inlineStr">
+        <is>
+          <t>FA1A6F9F4B8084A000</t>
+        </is>
+      </c>
+      <c r="T826" t="inlineStr">
+        <is>
+          <t>FA1A6F9F948B3B2000</t>
+        </is>
+      </c>
+      <c r="U826" t="inlineStr"/>
+      <c r="V826" t="inlineStr"/>
+      <c r="W826" t="inlineStr">
+        <is>
+          <t>FA1A70D08058BB2000</t>
+        </is>
+      </c>
+      <c r="X826" t="inlineStr">
+        <is>
+          <t>MA60_MA5</t>
+        </is>
+      </c>
+      <c r="Y826" t="inlineStr">
+        <is>
+          <t>mv :-14.76, mv_2m:-1.45,      mv_5m : -2.00, mv_30m : -2.88, mv_60m: -3.09</t>
+        </is>
+      </c>
+      <c r="Z826" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA826" t="inlineStr">
+        <is>
+          <t>FA1A6F9F9544C4A000</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" s="1" t="n">
+        <v>825</v>
+      </c>
+      <c r="B827" t="n">
+        <v>4122</v>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D827" s="2" t="n">
+        <v>45743.09739583333</v>
+      </c>
+      <c r="E827" t="n">
+        <v>72.235</v>
+      </c>
+      <c r="F827" t="n">
+        <v>2744.93</v>
+      </c>
+      <c r="G827" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H827" s="2" t="n">
+        <v>45745.02083980324</v>
+      </c>
+      <c r="I827" t="n">
+        <v>71.6019</v>
+      </c>
+      <c r="J827" t="n">
+        <v>2720.8722</v>
+      </c>
+      <c r="K827" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="L827" t="n">
+        <v>38</v>
+      </c>
+      <c r="M827" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N827" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="O827" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P827" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q827" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="R827" t="n">
+        <v>-26.34780000000005</v>
+      </c>
+      <c r="S827" t="inlineStr">
+        <is>
+          <t>FA1A71253C16FB2000</t>
+        </is>
+      </c>
+      <c r="T827" t="inlineStr">
+        <is>
+          <t>FA1A7135DEE03B2000</t>
+        </is>
+      </c>
+      <c r="U827" t="inlineStr"/>
+      <c r="V827" t="inlineStr"/>
+      <c r="W827" t="inlineStr"/>
+      <c r="X827" t="inlineStr">
+        <is>
+          <t>MA60_MA5</t>
+        </is>
+      </c>
+      <c r="Y827" t="inlineStr"/>
+      <c r="Z827" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA827" t="inlineStr">
+        <is>
+          <t>FA1A6F9F9544C4A000</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" s="1" t="n">
+        <v>826</v>
+      </c>
+      <c r="B828" t="n">
+        <v>4123</v>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>MRK</t>
+        </is>
+      </c>
+      <c r="D828" s="2" t="n">
+        <v>45745.1103808449</v>
+      </c>
+      <c r="E828" t="n">
+        <v>89.48909999999999</v>
+      </c>
+      <c r="F828" t="n">
+        <v>2774.1621</v>
+      </c>
+      <c r="G828" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="H828" s="2" t="n">
+        <v>45745.32922364584</v>
+      </c>
+      <c r="I828" t="n">
+        <v>89.23099999999999</v>
+      </c>
+      <c r="J828" t="n">
+        <v>2766.161</v>
+      </c>
+      <c r="K828" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="L828" t="n">
+        <v>31</v>
+      </c>
+      <c r="M828" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N828" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="O828" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P828" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q828" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="R828" t="n">
+        <v>-10.25109999999995</v>
+      </c>
+      <c r="S828" t="inlineStr">
+        <is>
+          <t>FA1A7236C0D3BB2000</t>
+        </is>
+      </c>
+      <c r="T828" t="inlineStr">
+        <is>
+          <t>FA1A723701C184A000</t>
+        </is>
+      </c>
+      <c r="U828" t="inlineStr"/>
+      <c r="V828" t="inlineStr"/>
+      <c r="W828" t="inlineStr">
+        <is>
+          <t>FA1A723A168F04A000</t>
+        </is>
+      </c>
+      <c r="X828" t="inlineStr">
+        <is>
+          <t>MA60_MA5</t>
+        </is>
+      </c>
+      <c r="Y828" t="inlineStr">
+        <is>
+          <t>mv :-20.66, mv_2m:-0.04,      mv_5m : 0.56, mv_30m : 12.41, mv_60m: 6.03, md_60m: 1</t>
+        </is>
+      </c>
+      <c r="Z828" t="inlineStr">
+        <is>
+          <t>Сиднейское время (лето)</t>
+        </is>
+      </c>
+      <c r="AA828" t="inlineStr">
+        <is>
+          <t>FA1A72370281BB2000</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
last working state for MACD model
</commit_message>
<xml_diff>
--- a/db/real_trade_db.xlsx
+++ b/db/real_trade_db.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA574"/>
+  <dimension ref="A1:AA597"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -54517,21 +54517,23 @@
         <v>1.01</v>
       </c>
       <c r="H569" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I569" t="inlineStr"/>
+        <v>45834.01851332176</v>
+      </c>
+      <c r="I569" t="n">
+        <v>221.84</v>
+      </c>
       <c r="J569" t="n">
-        <v>0</v>
+        <v>1996.56</v>
       </c>
       <c r="K569" t="n">
-        <v>0</v>
+        <v>1.03</v>
       </c>
       <c r="L569" t="n">
         <v>9</v>
       </c>
       <c r="M569" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N569" t="n">
@@ -54544,10 +54546,10 @@
         <v>1.006</v>
       </c>
       <c r="Q569" t="n">
-        <v>2.99</v>
+        <v>0.05</v>
       </c>
       <c r="R569" t="n">
-        <v>0</v>
+        <v>33.77999999999994</v>
       </c>
       <c r="S569" t="inlineStr">
         <is>
@@ -54592,41 +54594,43 @@
         <v>568</v>
       </c>
       <c r="B570" t="n">
-        <v>4364</v>
+        <v>4365</v>
       </c>
       <c r="C570" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>PLD</t>
         </is>
       </c>
       <c r="D570" s="2" t="n">
-        <v>45831.97983489584</v>
+        <v>45831.98380289352</v>
       </c>
       <c r="E570" t="n">
-        <v>10.56</v>
+        <v>106.18</v>
       </c>
       <c r="F570" t="n">
-        <v>1995.84</v>
+        <v>1911.24</v>
       </c>
       <c r="G570" t="n">
-        <v>1.111</v>
+        <v>1.04</v>
       </c>
       <c r="H570" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I570" t="inlineStr"/>
+        <v>45832.0296459838</v>
+      </c>
+      <c r="I570" t="n">
+        <v>105.86</v>
+      </c>
       <c r="J570" t="n">
-        <v>0</v>
+        <v>1905.48</v>
       </c>
       <c r="K570" t="n">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="L570" t="n">
-        <v>189</v>
+        <v>18</v>
       </c>
       <c r="M570" t="inlineStr">
         <is>
-          <t>placed</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N570" t="n">
@@ -54639,20 +54643,28 @@
         <v>1.006</v>
       </c>
       <c r="Q570" t="n">
-        <v>0.45</v>
+        <v>0.3</v>
       </c>
       <c r="R570" t="n">
-        <v>0</v>
+        <v>-7.849999999999991</v>
       </c>
       <c r="S570" t="inlineStr">
         <is>
-          <t>FA1AE21BC69FCAD000</t>
-        </is>
-      </c>
-      <c r="T570" t="inlineStr"/>
+          <t>FA1AE21D156DCAD000</t>
+        </is>
+      </c>
+      <c r="T570" t="inlineStr">
+        <is>
+          <t>FA1AE21DD37D4AD000</t>
+        </is>
+      </c>
       <c r="U570" t="inlineStr"/>
       <c r="V570" t="inlineStr"/>
-      <c r="W570" t="inlineStr"/>
+      <c r="W570" t="inlineStr">
+        <is>
+          <t>FA1AE21DD53F4AD000</t>
+        </is>
+      </c>
       <c r="X570" t="inlineStr">
         <is>
           <t>MA50_MA5</t>
@@ -54660,7 +54672,7 @@
       </c>
       <c r="Y570" t="inlineStr">
         <is>
-          <t>mv :-0.35, mv_2m:0.72,mv_5m : -0.09, mv_30m : 0.68, mv_60m: 0.32, md_60m: -5c1: 0, c2: 1</t>
+          <t>mv :-0.09, mv_2m:0.07,mv_5m : -2.58, mv_30m : -0.68, mv_60m: -0.79, md_60m: -4c1: 1, c2: 0</t>
         </is>
       </c>
       <c r="Z570" t="inlineStr">
@@ -54668,46 +54680,50 @@
           <t>Сиднейское время (зима)</t>
         </is>
       </c>
-      <c r="AA570" t="inlineStr"/>
+      <c r="AA570" t="inlineStr">
+        <is>
+          <t>FA1AE21DD41057C000</t>
+        </is>
+      </c>
     </row>
     <row r="571">
       <c r="A571" s="1" t="n">
         <v>569</v>
       </c>
       <c r="B571" t="n">
-        <v>4365</v>
+        <v>4370</v>
       </c>
       <c r="C571" t="inlineStr">
         <is>
-          <t>PLD</t>
+          <t>MCHP</t>
         </is>
       </c>
       <c r="D571" s="2" t="n">
-        <v>45831.98380289352</v>
+        <v>45831.98543841435</v>
       </c>
       <c r="E571" t="n">
-        <v>106.18</v>
+        <v>69.64619999999999</v>
       </c>
       <c r="F571" t="n">
-        <v>1911.24</v>
+        <v>1532.2164</v>
       </c>
       <c r="G571" t="n">
-        <v>1.04</v>
+        <v>1.06</v>
       </c>
       <c r="H571" s="2" t="n">
-        <v>45832.0296459838</v>
+        <v>45832.11033256944</v>
       </c>
       <c r="I571" t="n">
-        <v>105.86</v>
+        <v>69.51000000000001</v>
       </c>
       <c r="J571" t="n">
-        <v>1905.48</v>
+        <v>1529.22</v>
       </c>
       <c r="K571" t="n">
-        <v>1.05</v>
+        <v>1.07</v>
       </c>
       <c r="L571" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="M571" t="inlineStr">
         <is>
@@ -54724,26 +54740,26 @@
         <v>1.006</v>
       </c>
       <c r="Q571" t="n">
-        <v>0.3</v>
+        <v>0.01</v>
       </c>
       <c r="R571" t="n">
-        <v>-7.849999999999991</v>
+        <v>-5.126399999999995</v>
       </c>
       <c r="S571" t="inlineStr">
         <is>
-          <t>FA1AE21D156DCAD000</t>
+          <t>FA1AE21D9F6D97C000</t>
         </is>
       </c>
       <c r="T571" t="inlineStr">
         <is>
-          <t>FA1AE21DD37D4AD000</t>
+          <t>FA1AE21F0D3357C000</t>
         </is>
       </c>
       <c r="U571" t="inlineStr"/>
       <c r="V571" t="inlineStr"/>
       <c r="W571" t="inlineStr">
         <is>
-          <t>FA1AE21DD53F4AD000</t>
+          <t>FA1AE21F0EDE57C000</t>
         </is>
       </c>
       <c r="X571" t="inlineStr">
@@ -54753,7 +54769,7 @@
       </c>
       <c r="Y571" t="inlineStr">
         <is>
-          <t>mv :-0.09, mv_2m:0.07,mv_5m : -2.58, mv_30m : -0.68, mv_60m: -0.79, md_60m: -4c1: 1, c2: 0</t>
+          <t>mv :3.85, mv_2m:4.28,mv_5m : 4.85, mv_30m : 7.73, mv_60m: 8.53, md_60m: -5c1: 1, c2: 0</t>
         </is>
       </c>
       <c r="Z571" t="inlineStr">
@@ -54763,7 +54779,7 @@
       </c>
       <c r="AA571" t="inlineStr">
         <is>
-          <t>FA1AE21DD41057C000</t>
+          <t>FA1AE21F0DC34AD000</t>
         </is>
       </c>
     </row>
@@ -54772,41 +54788,43 @@
         <v>570</v>
       </c>
       <c r="B572" t="n">
-        <v>4366</v>
+        <v>4371</v>
       </c>
       <c r="C572" t="inlineStr">
         <is>
-          <t>FI</t>
+          <t>INTU</t>
         </is>
       </c>
       <c r="D572" s="2" t="n">
-        <v>45831.98405833334</v>
+        <v>45831.99085085648</v>
       </c>
       <c r="E572" t="n">
-        <v>169.1</v>
+        <v>760.92</v>
       </c>
       <c r="F572" t="n">
-        <v>1521.9</v>
+        <v>1521.84</v>
       </c>
       <c r="G572" t="n">
-        <v>1.111</v>
+        <v>0.99</v>
       </c>
       <c r="H572" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I572" t="inlineStr"/>
+        <v>45832.07748671297</v>
+      </c>
+      <c r="I572" t="n">
+        <v>762.3</v>
+      </c>
       <c r="J572" t="n">
-        <v>0</v>
+        <v>1524.6</v>
       </c>
       <c r="K572" t="n">
-        <v>0</v>
+        <v>1.01</v>
       </c>
       <c r="L572" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="M572" t="inlineStr">
         <is>
-          <t>placed</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N572" t="n">
@@ -54819,20 +54837,28 @@
         <v>1.006</v>
       </c>
       <c r="Q572" t="n">
-        <v>0.45</v>
+        <v>0.3</v>
       </c>
       <c r="R572" t="n">
-        <v>0</v>
+        <v>0.7599999999999909</v>
       </c>
       <c r="S572" t="inlineStr">
         <is>
-          <t>FA1AE21D2AFA57C000</t>
-        </is>
-      </c>
-      <c r="T572" t="inlineStr"/>
+          <t>FA1AE21F681ACAD000</t>
+        </is>
+      </c>
+      <c r="T572" t="inlineStr">
+        <is>
+          <t>FA1AE21FB0528AD000</t>
+        </is>
+      </c>
       <c r="U572" t="inlineStr"/>
       <c r="V572" t="inlineStr"/>
-      <c r="W572" t="inlineStr"/>
+      <c r="W572" t="inlineStr">
+        <is>
+          <t>FA1AE21FB1FDCAD000</t>
+        </is>
+      </c>
       <c r="X572" t="inlineStr">
         <is>
           <t>MA50_MA5</t>
@@ -54840,7 +54866,7 @@
       </c>
       <c r="Y572" t="inlineStr">
         <is>
-          <t>mv :1.09, mv_2m:1.25,mv_5m : -2.46, mv_30m : 2.00, mv_60m: 1.40, md_60m: -3c1: 1, c2: 0</t>
+          <t>mv :-2.37, mv_2m:-1.00,mv_5m : -3.08, mv_30m : 8.83, mv_60m: 7.90, md_60m: -6c1: 0, c2: 1</t>
         </is>
       </c>
       <c r="Z572" t="inlineStr">
@@ -54848,48 +54874,54 @@
           <t>Сиднейское время (зима)</t>
         </is>
       </c>
-      <c r="AA572" t="inlineStr"/>
+      <c r="AA572" t="inlineStr">
+        <is>
+          <t>FA1AE21FB0E0CAD000</t>
+        </is>
+      </c>
     </row>
     <row r="573">
       <c r="A573" s="1" t="n">
         <v>571</v>
       </c>
       <c r="B573" t="n">
-        <v>4370</v>
+        <v>4372</v>
       </c>
       <c r="C573" t="inlineStr">
         <is>
-          <t>MCHP</t>
+          <t>APH</t>
         </is>
       </c>
       <c r="D573" s="2" t="n">
-        <v>45831.98543841435</v>
+        <v>45832.03896349537</v>
       </c>
       <c r="E573" t="n">
-        <v>69.64619999999999</v>
+        <v>93.9492</v>
       </c>
       <c r="F573" t="n">
-        <v>1532.2164</v>
+        <v>1878.984</v>
       </c>
       <c r="G573" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="H573" s="2" t="n">
+        <v>45832.13798946759</v>
+      </c>
+      <c r="I573" t="n">
+        <v>93.67</v>
+      </c>
+      <c r="J573" t="n">
+        <v>1873.4</v>
+      </c>
+      <c r="K573" t="n">
         <v>1.06</v>
       </c>
-      <c r="H573" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I573" t="inlineStr"/>
-      <c r="J573" t="n">
-        <v>0</v>
-      </c>
-      <c r="K573" t="n">
-        <v>0</v>
-      </c>
       <c r="L573" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M573" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N573" t="n">
@@ -54902,26 +54934,26 @@
         <v>1.006</v>
       </c>
       <c r="Q573" t="n">
-        <v>2.99</v>
+        <v>0.01</v>
       </c>
       <c r="R573" t="n">
-        <v>0</v>
+        <v>-7.693999999999832</v>
       </c>
       <c r="S573" t="inlineStr">
         <is>
-          <t>FA1AE21D9F6D97C000</t>
+          <t>FA1AE22F439FCAD000</t>
         </is>
       </c>
       <c r="T573" t="inlineStr">
         <is>
-          <t>FA1AE21F0D3357C000</t>
+          <t>FA1AE230172C97C000</t>
         </is>
       </c>
       <c r="U573" t="inlineStr"/>
       <c r="V573" t="inlineStr"/>
       <c r="W573" t="inlineStr">
         <is>
-          <t>FA1AE21F0EDE57C000</t>
+          <t>FA1AE23018ED4AD000</t>
         </is>
       </c>
       <c r="X573" t="inlineStr">
@@ -54931,7 +54963,7 @@
       </c>
       <c r="Y573" t="inlineStr">
         <is>
-          <t>mv :3.85, mv_2m:4.28,mv_5m : 4.85, mv_30m : 7.73, mv_60m: 8.53, md_60m: -5c1: 1, c2: 0</t>
+          <t>mv :-2.49, mv_2m:-0.95,mv_5m : -1.64, mv_30m : -14.39, mv_60m: -2.86, md_60m: -34c1: 0, c2: 1</t>
         </is>
       </c>
       <c r="Z573" t="inlineStr">
@@ -54941,7 +54973,7 @@
       </c>
       <c r="AA573" t="inlineStr">
         <is>
-          <t>FA1AE21F0DC34AD000</t>
+          <t>FA1AE23017BC4AD000</t>
         </is>
       </c>
     </row>
@@ -54950,41 +54982,43 @@
         <v>572</v>
       </c>
       <c r="B574" t="n">
-        <v>4371</v>
+        <v>4373</v>
       </c>
       <c r="C574" t="inlineStr">
         <is>
-          <t>INTU</t>
+          <t>PANW</t>
         </is>
       </c>
       <c r="D574" s="2" t="n">
-        <v>45831.99085085648</v>
+        <v>45832.07160158565</v>
       </c>
       <c r="E574" t="n">
-        <v>760.92</v>
+        <v>201.95</v>
       </c>
       <c r="F574" t="n">
-        <v>1521.84</v>
+        <v>1413.65</v>
       </c>
       <c r="G574" t="n">
-        <v>0.99</v>
+        <v>1.01</v>
       </c>
       <c r="H574" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I574" t="inlineStr"/>
+        <v>45832.12611210648</v>
+      </c>
+      <c r="I574" t="n">
+        <v>201.33</v>
+      </c>
       <c r="J574" t="n">
-        <v>0</v>
+        <v>1409.31</v>
       </c>
       <c r="K574" t="n">
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="L574" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M574" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N574" t="n">
@@ -54997,26 +55031,26 @@
         <v>1.006</v>
       </c>
       <c r="Q574" t="n">
-        <v>0.3</v>
+        <v>0.01</v>
       </c>
       <c r="R574" t="n">
-        <v>0</v>
+        <v>-6.369999999999918</v>
       </c>
       <c r="S574" t="inlineStr">
         <is>
-          <t>FA1AE21F681ACAD000</t>
+          <t>FA1AE23A056B17C000</t>
         </is>
       </c>
       <c r="T574" t="inlineStr">
         <is>
-          <t>FA1AE21FB0528AD000</t>
+          <t>FA1AE23A6C6B17C000</t>
         </is>
       </c>
       <c r="U574" t="inlineStr"/>
       <c r="V574" t="inlineStr"/>
       <c r="W574" t="inlineStr">
         <is>
-          <t>FA1AE21FB1FDCAD000</t>
+          <t>FA1AE23A6E550AD000</t>
         </is>
       </c>
       <c r="X574" t="inlineStr">
@@ -55026,7 +55060,7 @@
       </c>
       <c r="Y574" t="inlineStr">
         <is>
-          <t>mv :-2.37, mv_2m:-1.00,mv_5m : -3.08, mv_30m : 8.83, mv_60m: 7.90, md_60m: -6c1: 0, c2: 1</t>
+          <t>mv :-6.42, mv_2m:-1.83,mv_5m : -4.87, mv_30m : -6.79, mv_60m: -18.57, md_60m: -42c1: 0, c2: 1</t>
         </is>
       </c>
       <c r="Z574" t="inlineStr">
@@ -55036,7 +55070,2240 @@
       </c>
       <c r="AA574" t="inlineStr">
         <is>
-          <t>FA1AE21FB0E0CAD000</t>
+          <t>FA1AE23A6D074AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" s="1" t="n">
+        <v>573</v>
+      </c>
+      <c r="B575" t="n">
+        <v>4374</v>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>PANW</t>
+        </is>
+      </c>
+      <c r="D575" s="2" t="n">
+        <v>45832.08828190972</v>
+      </c>
+      <c r="E575" t="n">
+        <v>201.29</v>
+      </c>
+      <c r="F575" t="n">
+        <v>1409.03</v>
+      </c>
+      <c r="G575" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H575" s="2" t="n">
+        <v>45832.14130105324</v>
+      </c>
+      <c r="I575" t="n">
+        <v>200.67</v>
+      </c>
+      <c r="J575" t="n">
+        <v>1404.69</v>
+      </c>
+      <c r="K575" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L575" t="n">
+        <v>7</v>
+      </c>
+      <c r="M575" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N575" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O575" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P575" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q575" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R575" t="n">
+        <v>-6.370000000000145</v>
+      </c>
+      <c r="S575" t="inlineStr">
+        <is>
+          <t>FA1AE23F84D18AD000</t>
+        </is>
+      </c>
+      <c r="T575" t="inlineStr">
+        <is>
+          <t>FA1AE23FD8748AD000</t>
+        </is>
+      </c>
+      <c r="U575" t="inlineStr"/>
+      <c r="V575" t="inlineStr"/>
+      <c r="W575" t="inlineStr">
+        <is>
+          <t>FA1AE23FDA324AD000</t>
+        </is>
+      </c>
+      <c r="X575" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y575" t="inlineStr">
+        <is>
+          <t>mv :-1.23, mv_2m:-0.28,mv_5m : 0.59, mv_30m : -8.61, mv_60m: -11.09, md_60m: -38c1: 0, c2: 1</t>
+        </is>
+      </c>
+      <c r="Z575" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA575" t="inlineStr">
+        <is>
+          <t>FA1AE23FD911D7C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" s="1" t="n">
+        <v>574</v>
+      </c>
+      <c r="B576" t="n">
+        <v>4375</v>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>GD</t>
+        </is>
+      </c>
+      <c r="D576" s="2" t="n">
+        <v>45832.09940652778</v>
+      </c>
+      <c r="E576" t="n">
+        <v>283.23</v>
+      </c>
+      <c r="F576" t="n">
+        <v>1982.61</v>
+      </c>
+      <c r="G576" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H576" s="2" t="n">
+        <v>45832.1489422801</v>
+      </c>
+      <c r="I576" t="n">
+        <v>281.92</v>
+      </c>
+      <c r="J576" t="n">
+        <v>1973.44</v>
+      </c>
+      <c r="K576" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L576" t="n">
+        <v>7</v>
+      </c>
+      <c r="M576" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N576" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O576" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P576" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q576" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R576" t="n">
+        <v>-11.19999999999984</v>
+      </c>
+      <c r="S576" t="inlineStr">
+        <is>
+          <t>FA1AE2432F7417C000</t>
+        </is>
+      </c>
+      <c r="T576" t="inlineStr">
+        <is>
+          <t>FA1AE243F3BDCAD000</t>
+        </is>
+      </c>
+      <c r="U576" t="inlineStr"/>
+      <c r="V576" t="inlineStr"/>
+      <c r="W576" t="inlineStr">
+        <is>
+          <t>FA1AE243F5710AD000</t>
+        </is>
+      </c>
+      <c r="X576" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y576" t="inlineStr">
+        <is>
+          <t>mv :-3.06, mv_2m:-0.63,mv_5m : -2.43, mv_30m : -7.49, mv_60m: -17.54, md_60m: -69c1: 0, c2: 1</t>
+        </is>
+      </c>
+      <c r="Z576" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA576" t="inlineStr">
+        <is>
+          <t>FA1AE243F44BCAD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" s="1" t="n">
+        <v>575</v>
+      </c>
+      <c r="B577" t="n">
+        <v>4376</v>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>TXN</t>
+        </is>
+      </c>
+      <c r="D577" s="2" t="n">
+        <v>45832.10264516203</v>
+      </c>
+      <c r="E577" t="n">
+        <v>199.78</v>
+      </c>
+      <c r="F577" t="n">
+        <v>1398.46</v>
+      </c>
+      <c r="G577" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H577" s="2" t="n">
+        <v>45832.14625863426</v>
+      </c>
+      <c r="I577" t="n">
+        <v>199.15</v>
+      </c>
+      <c r="J577" t="n">
+        <v>1394.05</v>
+      </c>
+      <c r="K577" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L577" t="n">
+        <v>7</v>
+      </c>
+      <c r="M577" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N577" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O577" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P577" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q577" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R577" t="n">
+        <v>-6.440000000000081</v>
+      </c>
+      <c r="S577" t="inlineStr">
+        <is>
+          <t>FA1AE24440B857C000</t>
+        </is>
+      </c>
+      <c r="T577" t="inlineStr">
+        <is>
+          <t>FA1AE2449895D7C000</t>
+        </is>
+      </c>
+      <c r="U577" t="inlineStr"/>
+      <c r="V577" t="inlineStr"/>
+      <c r="W577" t="inlineStr">
+        <is>
+          <t>FA1AE2449A52D7C000</t>
+        </is>
+      </c>
+      <c r="X577" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y577" t="inlineStr">
+        <is>
+          <t>mv :-6.98, mv_2m:-2.58,mv_5m : -6.64, mv_30m : -9.45, mv_60m: -17.65, md_60m: -48c1: 0, c2: 1</t>
+        </is>
+      </c>
+      <c r="Z577" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA577" t="inlineStr">
+        <is>
+          <t>FA1AE2449930D7C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" s="1" t="n">
+        <v>576</v>
+      </c>
+      <c r="B578" t="n">
+        <v>4377</v>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>MPC</t>
+        </is>
+      </c>
+      <c r="D578" s="2" t="n">
+        <v>45832.10769884259</v>
+      </c>
+      <c r="E578" t="n">
+        <v>170.2</v>
+      </c>
+      <c r="F578" t="n">
+        <v>1361.6</v>
+      </c>
+      <c r="G578" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H578" s="2" t="n">
+        <v>45832.14946236111</v>
+      </c>
+      <c r="I578" t="n">
+        <v>169.3475</v>
+      </c>
+      <c r="J578" t="n">
+        <v>1354.78</v>
+      </c>
+      <c r="K578" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L578" t="n">
+        <v>8</v>
+      </c>
+      <c r="M578" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N578" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O578" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P578" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q578" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R578" t="n">
+        <v>-8.849999999999936</v>
+      </c>
+      <c r="S578" t="inlineStr">
+        <is>
+          <t>FA1AE245EB1D57C000</t>
+        </is>
+      </c>
+      <c r="T578" t="inlineStr">
+        <is>
+          <t>FA1AE2465AD54AD000</t>
+        </is>
+      </c>
+      <c r="U578" t="inlineStr"/>
+      <c r="V578" t="inlineStr"/>
+      <c r="W578" t="inlineStr">
+        <is>
+          <t>FA1AE2465C954AD000</t>
+        </is>
+      </c>
+      <c r="X578" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y578" t="inlineStr">
+        <is>
+          <t>mv :-11.91, mv_2m:-0.90,mv_5m : -2.69, mv_30m : -7.39, mv_60m: -11.89, md_60m: -24c1: 0, c2: 1</t>
+        </is>
+      </c>
+      <c r="Z578" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA578" t="inlineStr">
+        <is>
+          <t>FA1AE2465B654AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" s="1" t="n">
+        <v>577</v>
+      </c>
+      <c r="B579" t="n">
+        <v>4378</v>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>NOC</t>
+        </is>
+      </c>
+      <c r="D579" s="2" t="n">
+        <v>45832.11023432871</v>
+      </c>
+      <c r="E579" t="n">
+        <v>507.31</v>
+      </c>
+      <c r="F579" t="n">
+        <v>1521.93</v>
+      </c>
+      <c r="G579" t="n">
+        <v>1</v>
+      </c>
+      <c r="H579" s="2" t="n">
+        <v>45832.15380416666</v>
+      </c>
+      <c r="I579" t="n">
+        <v>504.5827</v>
+      </c>
+      <c r="J579" t="n">
+        <v>1513.7481</v>
+      </c>
+      <c r="K579" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="L579" t="n">
+        <v>3</v>
+      </c>
+      <c r="M579" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N579" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O579" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P579" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q579" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R579" t="n">
+        <v>-10.19190000000004</v>
+      </c>
+      <c r="S579" t="inlineStr">
+        <is>
+          <t>FA1AE246C1110AD000</t>
+        </is>
+      </c>
+      <c r="T579" t="inlineStr">
+        <is>
+          <t>FA1AE247084197C000</t>
+        </is>
+      </c>
+      <c r="U579" t="inlineStr"/>
+      <c r="V579" t="inlineStr"/>
+      <c r="W579" t="inlineStr">
+        <is>
+          <t>FA1AE24709EC57C000</t>
+        </is>
+      </c>
+      <c r="X579" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y579" t="inlineStr">
+        <is>
+          <t>mv :-0.90, mv_2m:0.10,mv_5m : -7.85, mv_30m : -24.21, mv_60m: -36.49, md_60m: -67c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z579" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA579" t="inlineStr">
+        <is>
+          <t>FA1AE24708D797C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" s="1" t="n">
+        <v>578</v>
+      </c>
+      <c r="B580" t="n">
+        <v>4379</v>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>GD</t>
+        </is>
+      </c>
+      <c r="D580" s="2" t="n">
+        <v>45832.1123775926</v>
+      </c>
+      <c r="E580" t="n">
+        <v>281.91</v>
+      </c>
+      <c r="F580" t="n">
+        <v>1691.46</v>
+      </c>
+      <c r="G580" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H580" s="2" t="n">
+        <v>45832.17586607639</v>
+      </c>
+      <c r="I580" t="n">
+        <v>281.16</v>
+      </c>
+      <c r="J580" t="n">
+        <v>1686.96</v>
+      </c>
+      <c r="K580" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L580" t="n">
+        <v>6</v>
+      </c>
+      <c r="M580" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N580" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O580" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P580" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q580" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R580" t="n">
+        <v>-6.529999999999999</v>
+      </c>
+      <c r="S580" t="inlineStr">
+        <is>
+          <t>FA1AE24775E30AD000</t>
+        </is>
+      </c>
+      <c r="T580" t="inlineStr">
+        <is>
+          <t>FA1AE248357C17C000</t>
+        </is>
+      </c>
+      <c r="U580" t="inlineStr"/>
+      <c r="V580" t="inlineStr"/>
+      <c r="W580" t="inlineStr">
+        <is>
+          <t>FA1AE24837364AD000</t>
+        </is>
+      </c>
+      <c r="X580" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y580" t="inlineStr">
+        <is>
+          <t>mv :1.83, mv_2m:2.88,mv_5m : 6.73, mv_30m : -20.82, mv_60m: -31.71, md_60m: -77c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z580" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA580" t="inlineStr">
+        <is>
+          <t>FA1AE248360D97C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" s="1" t="n">
+        <v>579</v>
+      </c>
+      <c r="B581" t="n">
+        <v>4380</v>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>TXN</t>
+        </is>
+      </c>
+      <c r="D581" s="2" t="n">
+        <v>45832.11567224537</v>
+      </c>
+      <c r="E581" t="n">
+        <v>199.97</v>
+      </c>
+      <c r="F581" t="n">
+        <v>1599.76</v>
+      </c>
+      <c r="G581" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H581" s="2" t="n">
+        <v>45832.15595979166</v>
+      </c>
+      <c r="I581" t="n">
+        <v>199.1701</v>
+      </c>
+      <c r="J581" t="n">
+        <v>1593.3608</v>
+      </c>
+      <c r="K581" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L581" t="n">
+        <v>8</v>
+      </c>
+      <c r="M581" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N581" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O581" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P581" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q581" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R581" t="n">
+        <v>-8.429200000000064</v>
+      </c>
+      <c r="S581" t="inlineStr">
+        <is>
+          <t>FA1AE2488BDD57C000</t>
+        </is>
+      </c>
+      <c r="T581" t="inlineStr">
+        <is>
+          <t>FA1AE248E2B557C000</t>
+        </is>
+      </c>
+      <c r="U581" t="inlineStr"/>
+      <c r="V581" t="inlineStr"/>
+      <c r="W581" t="inlineStr">
+        <is>
+          <t>FA1AE248E4698AD000</t>
+        </is>
+      </c>
+      <c r="X581" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y581" t="inlineStr">
+        <is>
+          <t>mv :8.47, mv_2m:1.45,mv_5m : 6.29, mv_30m : -6.32, mv_60m: -9.38, md_60m: -42c1: 0, c2: 1</t>
+        </is>
+      </c>
+      <c r="Z581" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA581" t="inlineStr">
+        <is>
+          <t>FA1AE248E343CAD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" s="1" t="n">
+        <v>580</v>
+      </c>
+      <c r="B582" t="n">
+        <v>4381</v>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>NOC</t>
+        </is>
+      </c>
+      <c r="D582" s="2" t="n">
+        <v>45832.11796085648</v>
+      </c>
+      <c r="E582" t="n">
+        <v>503.76</v>
+      </c>
+      <c r="F582" t="n">
+        <v>1511.28</v>
+      </c>
+      <c r="G582" t="n">
+        <v>1</v>
+      </c>
+      <c r="H582" s="2" t="n">
+        <v>45832.1749002662</v>
+      </c>
+      <c r="I582" t="n">
+        <v>501.15</v>
+      </c>
+      <c r="J582" t="n">
+        <v>1503.45</v>
+      </c>
+      <c r="K582" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="L582" t="n">
+        <v>3</v>
+      </c>
+      <c r="M582" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N582" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O582" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P582" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q582" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R582" t="n">
+        <v>-9.840000000000154</v>
+      </c>
+      <c r="S582" t="inlineStr">
+        <is>
+          <t>FA1AE2494CF797C000</t>
+        </is>
+      </c>
+      <c r="T582" t="inlineStr">
+        <is>
+          <t>FA1AE24A184A4AD000</t>
+        </is>
+      </c>
+      <c r="U582" t="inlineStr"/>
+      <c r="V582" t="inlineStr"/>
+      <c r="W582" t="inlineStr">
+        <is>
+          <t>FA1AE24A19EECAD000</t>
+        </is>
+      </c>
+      <c r="X582" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y582" t="inlineStr">
+        <is>
+          <t>mv :5.55, mv_2m:-3.15,mv_5m : -1.13, mv_30m : -10.55, mv_60m: -14.82, md_60m: -57c1: 0, c2: 1</t>
+        </is>
+      </c>
+      <c r="Z582" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA582" t="inlineStr">
+        <is>
+          <t>FA1AE24A18D8CAD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" s="1" t="n">
+        <v>581</v>
+      </c>
+      <c r="B583" t="n">
+        <v>4382</v>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>ADSK</t>
+        </is>
+      </c>
+      <c r="D583" s="2" t="n">
+        <v>45832.13613508102</v>
+      </c>
+      <c r="E583" t="n">
+        <v>297.8</v>
+      </c>
+      <c r="F583" t="n">
+        <v>1489</v>
+      </c>
+      <c r="G583" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H583" s="2" t="n">
+        <v>45834.26896150463</v>
+      </c>
+      <c r="I583" t="n">
+        <v>303.31</v>
+      </c>
+      <c r="J583" t="n">
+        <v>1516.55</v>
+      </c>
+      <c r="K583" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L583" t="n">
+        <v>5</v>
+      </c>
+      <c r="M583" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N583" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O583" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P583" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q583" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R583" t="n">
+        <v>25.51999999999995</v>
+      </c>
+      <c r="S583" t="inlineStr">
+        <is>
+          <t>FA1AE24F4A69CAD000</t>
+        </is>
+      </c>
+      <c r="T583" t="inlineStr">
+        <is>
+          <t>FA1AE2501D1C57C000</t>
+        </is>
+      </c>
+      <c r="U583" t="inlineStr"/>
+      <c r="V583" t="inlineStr"/>
+      <c r="W583" t="inlineStr">
+        <is>
+          <t>FA1AE2501ECD4AD000</t>
+        </is>
+      </c>
+      <c r="X583" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y583" t="inlineStr">
+        <is>
+          <t>mv :1.37, mv_2m:-0.66,mv_5m : 0.41, mv_30m : -1.28, mv_60m: -17.18, md_60m: -60c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z583" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA583" t="inlineStr">
+        <is>
+          <t>FA1AE2501DBA97C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" s="1" t="n">
+        <v>582</v>
+      </c>
+      <c r="B584" t="n">
+        <v>4383</v>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>TXN</t>
+        </is>
+      </c>
+      <c r="D584" s="2" t="n">
+        <v>45832.13753571759</v>
+      </c>
+      <c r="E584" t="n">
+        <v>200.06</v>
+      </c>
+      <c r="F584" t="n">
+        <v>1800.54</v>
+      </c>
+      <c r="G584" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="H584" s="2" t="n">
+        <v>45834.0848187963</v>
+      </c>
+      <c r="I584" t="n">
+        <v>203.8381</v>
+      </c>
+      <c r="J584" t="n">
+        <v>1834.5429</v>
+      </c>
+      <c r="K584" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="L584" t="n">
+        <v>9</v>
+      </c>
+      <c r="M584" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N584" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O584" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P584" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q584" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R584" t="n">
+        <v>31.95289999999995</v>
+      </c>
+      <c r="S584" t="inlineStr">
+        <is>
+          <t>FA1AE24FC0994AD000</t>
+        </is>
+      </c>
+      <c r="T584" t="inlineStr">
+        <is>
+          <t>FA1AE250164457C000</t>
+        </is>
+      </c>
+      <c r="U584" t="inlineStr"/>
+      <c r="V584" t="inlineStr"/>
+      <c r="W584" t="inlineStr">
+        <is>
+          <t>FA1AE25017E597C000</t>
+        </is>
+      </c>
+      <c r="X584" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y584" t="inlineStr">
+        <is>
+          <t>mv :3.66, mv_2m:2.37,mv_5m : 2.66, mv_30m : 3.11, mv_60m: -9.06, md_60m: -38c1: 0, c2: 1</t>
+        </is>
+      </c>
+      <c r="Z584" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA584" t="inlineStr">
+        <is>
+          <t>FA1AE25016D297C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" s="1" t="n">
+        <v>583</v>
+      </c>
+      <c r="B585" t="n">
+        <v>4384</v>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>MDT</t>
+        </is>
+      </c>
+      <c r="D585" s="2" t="n">
+        <v>45833.99691318287</v>
+      </c>
+      <c r="E585" t="n">
+        <v>85.74639999999999</v>
+      </c>
+      <c r="F585" t="n">
+        <v>1972.1672</v>
+      </c>
+      <c r="G585" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="H585" s="2" t="n">
+        <v>45834.06785967592</v>
+      </c>
+      <c r="I585" t="n">
+        <v>85.6801</v>
+      </c>
+      <c r="J585" t="n">
+        <v>1970.6423</v>
+      </c>
+      <c r="K585" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="L585" t="n">
+        <v>23</v>
+      </c>
+      <c r="M585" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N585" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O585" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P585" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q585" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="R585" t="n">
+        <v>-3.654900000000116</v>
+      </c>
+      <c r="S585" t="inlineStr">
+        <is>
+          <t>FA1AE4B4959717C000</t>
+        </is>
+      </c>
+      <c r="T585" t="inlineStr">
+        <is>
+          <t>FA1AE4B4D5FB8AD000</t>
+        </is>
+      </c>
+      <c r="U585" t="inlineStr"/>
+      <c r="V585" t="inlineStr"/>
+      <c r="W585" t="inlineStr">
+        <is>
+          <t>FA1AE4B4D7C88AD000</t>
+        </is>
+      </c>
+      <c r="X585" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y585" t="inlineStr">
+        <is>
+          <t>mv :-2.74, mv_2m:0.64,mv_5m : -1.33, mv_30m : -15.87, mv_60m: -17.67, md_60m: -40c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z585" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA585" t="inlineStr">
+        <is>
+          <t>FA1AE4B4D69A57C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" s="1" t="n">
+        <v>584</v>
+      </c>
+      <c r="B586" t="n">
+        <v>4385</v>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>MDT</t>
+        </is>
+      </c>
+      <c r="D586" s="2" t="n">
+        <v>45834.04817767361</v>
+      </c>
+      <c r="E586" t="n">
+        <v>85.58969999999999</v>
+      </c>
+      <c r="F586" t="n">
+        <v>1968.5631</v>
+      </c>
+      <c r="G586" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="H586" s="2" t="n">
+        <v>45834.19123069444</v>
+      </c>
+      <c r="I586" t="n">
+        <v>86.0501</v>
+      </c>
+      <c r="J586" t="n">
+        <v>1979.1523</v>
+      </c>
+      <c r="K586" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="L586" t="n">
+        <v>23</v>
+      </c>
+      <c r="M586" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N586" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O586" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P586" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q586" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="R586" t="n">
+        <v>8.459199999999891</v>
+      </c>
+      <c r="S586" t="inlineStr">
+        <is>
+          <t>FA1AE4C57AFE17C000</t>
+        </is>
+      </c>
+      <c r="T586" t="inlineStr">
+        <is>
+          <t>FA1AE4C5BDC897C000</t>
+        </is>
+      </c>
+      <c r="U586" t="inlineStr"/>
+      <c r="V586" t="inlineStr"/>
+      <c r="W586" t="inlineStr">
+        <is>
+          <t>FA1AE4C5BF8BCAD000</t>
+        </is>
+      </c>
+      <c r="X586" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y586" t="inlineStr">
+        <is>
+          <t>mv :-4.51, mv_2m:-0.25,mv_5m : -1.88, mv_30m : -4.42, mv_60m: -2.09, md_60m: -32c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z586" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA586" t="inlineStr">
+        <is>
+          <t>FA1AE4C5BE6797C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" s="1" t="n">
+        <v>585</v>
+      </c>
+      <c r="B587" t="n">
+        <v>4386</v>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>GILD</t>
+        </is>
+      </c>
+      <c r="D587" s="2" t="n">
+        <v>45834.23053396991</v>
+      </c>
+      <c r="E587" t="n">
+        <v>105.9881</v>
+      </c>
+      <c r="F587" t="n">
+        <v>1907.7858</v>
+      </c>
+      <c r="G587" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="H587" s="2" t="n">
+        <v>45835.02306469907</v>
+      </c>
+      <c r="I587" t="n">
+        <v>106.53</v>
+      </c>
+      <c r="J587" t="n">
+        <v>1917.54</v>
+      </c>
+      <c r="K587" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="L587" t="n">
+        <v>18</v>
+      </c>
+      <c r="M587" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N587" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O587" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P587" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q587" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="R587" t="n">
+        <v>7.644199999999856</v>
+      </c>
+      <c r="S587" t="inlineStr">
+        <is>
+          <t>FA1AE501955DCAD000</t>
+        </is>
+      </c>
+      <c r="T587" t="inlineStr">
+        <is>
+          <t>FA1AE501F40757C000</t>
+        </is>
+      </c>
+      <c r="U587" t="inlineStr"/>
+      <c r="V587" t="inlineStr"/>
+      <c r="W587" t="inlineStr">
+        <is>
+          <t>FA1AE501F5B70AD000</t>
+        </is>
+      </c>
+      <c r="X587" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y587" t="inlineStr">
+        <is>
+          <t>mv :1.91, mv_2m:-0.97,mv_5m : -3.27, mv_30m : 0.46, mv_60m: 7.90, md_60m: -3c1: 0, c2: 1</t>
+        </is>
+      </c>
+      <c r="Z587" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA587" t="inlineStr">
+        <is>
+          <t>FA1AE501F49517C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" s="1" t="n">
+        <v>586</v>
+      </c>
+      <c r="B588" t="n">
+        <v>4387</v>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>HCA</t>
+        </is>
+      </c>
+      <c r="D588" s="2" t="n">
+        <v>45835.0375524074</v>
+      </c>
+      <c r="E588" t="n">
+        <v>381.18</v>
+      </c>
+      <c r="F588" t="n">
+        <v>1905.9</v>
+      </c>
+      <c r="G588" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H588" s="2" t="n">
+        <v>45840.28536775463</v>
+      </c>
+      <c r="I588" t="n">
+        <v>389.69</v>
+      </c>
+      <c r="J588" t="n">
+        <v>1948.45</v>
+      </c>
+      <c r="K588" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L588" t="n">
+        <v>5</v>
+      </c>
+      <c r="M588" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N588" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O588" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P588" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q588" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R588" t="n">
+        <v>40.51999999999995</v>
+      </c>
+      <c r="S588" t="inlineStr">
+        <is>
+          <t>FA1AE60B918717C000</t>
+        </is>
+      </c>
+      <c r="T588" t="inlineStr">
+        <is>
+          <t>FA1AE60C1339CAD000</t>
+        </is>
+      </c>
+      <c r="U588" t="inlineStr"/>
+      <c r="V588" t="inlineStr"/>
+      <c r="W588" t="inlineStr">
+        <is>
+          <t>FA1AE60C1500D7C000</t>
+        </is>
+      </c>
+      <c r="X588" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y588" t="inlineStr">
+        <is>
+          <t>mv :2.52, mv_2m:0.43,mv_5m : 1.26, mv_30m : 2.96, mv_60m: 1.80, md_60m: -2c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z588" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA588" t="inlineStr">
+        <is>
+          <t>FA1AE60C13CB0AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" s="1" t="n">
+        <v>587</v>
+      </c>
+      <c r="B589" t="n">
+        <v>4388</v>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="D589" s="2" t="n">
+        <v>45835.08217371528</v>
+      </c>
+      <c r="E589" t="n">
+        <v>100.39</v>
+      </c>
+      <c r="F589" t="n">
+        <v>1907.41</v>
+      </c>
+      <c r="G589" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="H589" s="2" t="n">
+        <v>45836.18839013889</v>
+      </c>
+      <c r="I589" t="n">
+        <v>101.305</v>
+      </c>
+      <c r="J589" t="n">
+        <v>1924.795</v>
+      </c>
+      <c r="K589" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="L589" t="n">
+        <v>19</v>
+      </c>
+      <c r="M589" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N589" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O589" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P589" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q589" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R589" t="n">
+        <v>15.27499999999999</v>
+      </c>
+      <c r="S589" t="inlineStr">
+        <is>
+          <t>FA1AE61A46744AD000</t>
+        </is>
+      </c>
+      <c r="T589" t="inlineStr">
+        <is>
+          <t>FA1AE61AA3CB0AD000</t>
+        </is>
+      </c>
+      <c r="U589" t="inlineStr"/>
+      <c r="V589" t="inlineStr"/>
+      <c r="W589" t="inlineStr">
+        <is>
+          <t>FA1AE61AA5928AD000</t>
+        </is>
+      </c>
+      <c r="X589" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y589" t="inlineStr">
+        <is>
+          <t>mv :-3.81, mv_2m:0.73,mv_5m : 0.51, mv_30m : -2.92, mv_60m: -7.62, md_60m: -32c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z589" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA589" t="inlineStr">
+        <is>
+          <t>FA1AE61AA45997C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" s="1" t="n">
+        <v>588</v>
+      </c>
+      <c r="B590" t="n">
+        <v>4389</v>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>ROK</t>
+        </is>
+      </c>
+      <c r="D590" s="2" t="n">
+        <v>45835.08902726852</v>
+      </c>
+      <c r="E590" t="n">
+        <v>324.64</v>
+      </c>
+      <c r="F590" t="n">
+        <v>1623.2</v>
+      </c>
+      <c r="G590" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H590" s="2" t="n">
+        <v>45836.19656328703</v>
+      </c>
+      <c r="I590" t="n">
+        <v>329.17</v>
+      </c>
+      <c r="J590" t="n">
+        <v>1645.85</v>
+      </c>
+      <c r="K590" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L590" t="n">
+        <v>5</v>
+      </c>
+      <c r="M590" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N590" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O590" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P590" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q590" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R590" t="n">
+        <v>20.62000000000009</v>
+      </c>
+      <c r="S590" t="inlineStr">
+        <is>
+          <t>FA1AE61C88B40AD000</t>
+        </is>
+      </c>
+      <c r="T590" t="inlineStr">
+        <is>
+          <t>FA1AE61D3F3B97C000</t>
+        </is>
+      </c>
+      <c r="U590" t="inlineStr"/>
+      <c r="V590" t="inlineStr"/>
+      <c r="W590" t="inlineStr">
+        <is>
+          <t>FA1AE61D4119D7C000</t>
+        </is>
+      </c>
+      <c r="X590" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y590" t="inlineStr">
+        <is>
+          <t>mv :-1.59, mv_2m:-0.19,mv_5m : 1.55, mv_30m : 0.34, mv_60m: -5.66, md_60m: -47c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z590" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA590" t="inlineStr">
+        <is>
+          <t>FA1AE61D3FC8D7C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" s="1" t="n">
+        <v>589</v>
+      </c>
+      <c r="B591" t="n">
+        <v>4390</v>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>FDX</t>
+        </is>
+      </c>
+      <c r="D591" s="2" t="n">
+        <v>45836.15316915509</v>
+      </c>
+      <c r="E591" t="n">
+        <v>227.8</v>
+      </c>
+      <c r="F591" t="n">
+        <v>1822.4</v>
+      </c>
+      <c r="G591" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H591" s="2" t="n">
+        <v>45840.27049047454</v>
+      </c>
+      <c r="I591" t="n">
+        <v>235.0518</v>
+      </c>
+      <c r="J591" t="n">
+        <v>1880.4144</v>
+      </c>
+      <c r="K591" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L591" t="n">
+        <v>8</v>
+      </c>
+      <c r="M591" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N591" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O591" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P591" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q591" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R591" t="n">
+        <v>55.98439999999979</v>
+      </c>
+      <c r="S591" t="inlineStr">
+        <is>
+          <t>FA1AE77B43A44AD000</t>
+        </is>
+      </c>
+      <c r="T591" t="inlineStr">
+        <is>
+          <t>FA1AE77BDF4BD7C000</t>
+        </is>
+      </c>
+      <c r="U591" t="inlineStr"/>
+      <c r="V591" t="inlineStr"/>
+      <c r="W591" t="inlineStr">
+        <is>
+          <t>FA1AE77BE11F17C000</t>
+        </is>
+      </c>
+      <c r="X591" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y591" t="inlineStr">
+        <is>
+          <t>mv :0.03, mv_2m:-0.00,mv_5m : 0.09, mv_30m : -0.58, mv_60m: -0.73, md_60m: -1c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z591" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA591" t="inlineStr">
+        <is>
+          <t>FA1AE77BDFD9D7C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" s="1" t="n">
+        <v>590</v>
+      </c>
+      <c r="B592" t="n">
+        <v>4391</v>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>MCK</t>
+        </is>
+      </c>
+      <c r="D592" s="2" t="n">
+        <v>45836.15778747686</v>
+      </c>
+      <c r="E592" t="n">
+        <v>731.75</v>
+      </c>
+      <c r="F592" t="n">
+        <v>1463.5</v>
+      </c>
+      <c r="G592" t="n">
+        <v>1</v>
+      </c>
+      <c r="H592" s="2" t="n">
+        <v>45840.10964957176</v>
+      </c>
+      <c r="I592" t="n">
+        <v>717.5700000000001</v>
+      </c>
+      <c r="J592" t="n">
+        <v>1435.14</v>
+      </c>
+      <c r="K592" t="n">
+        <v>1.101</v>
+      </c>
+      <c r="L592" t="n">
+        <v>2</v>
+      </c>
+      <c r="M592" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N592" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O592" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P592" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q592" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="R592" t="n">
+        <v>-30.4609999999999</v>
+      </c>
+      <c r="S592" t="inlineStr">
+        <is>
+          <t>FA1AE77CC9500AD000</t>
+        </is>
+      </c>
+      <c r="T592" t="inlineStr">
+        <is>
+          <t>FA1AE77DFEAA17C000</t>
+        </is>
+      </c>
+      <c r="U592" t="inlineStr"/>
+      <c r="V592" t="inlineStr"/>
+      <c r="W592" t="inlineStr">
+        <is>
+          <t>FA1AE77E00498AD000</t>
+        </is>
+      </c>
+      <c r="X592" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y592" t="inlineStr">
+        <is>
+          <t>mv :-4.85, mv_2m:-2.94,mv_5m : -6.58, mv_30m : -6.10, mv_60m: -10.08, md_60m: -31c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z592" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA592" t="inlineStr">
+        <is>
+          <t>FA1AE77DFF39D7C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" s="1" t="n">
+        <v>591</v>
+      </c>
+      <c r="B593" t="n">
+        <v>4392</v>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>AMT</t>
+        </is>
+      </c>
+      <c r="D593" s="2" t="n">
+        <v>45840.1147853588</v>
+      </c>
+      <c r="E593" t="n">
+        <v>223.34</v>
+      </c>
+      <c r="F593" t="n">
+        <v>1563.38</v>
+      </c>
+      <c r="G593" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H593" s="2" t="n">
+        <v>45841.02754986111</v>
+      </c>
+      <c r="I593" t="n">
+        <v>223.5</v>
+      </c>
+      <c r="J593" t="n">
+        <v>1564.5</v>
+      </c>
+      <c r="K593" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L593" t="n">
+        <v>7</v>
+      </c>
+      <c r="M593" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N593" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O593" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P593" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q593" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R593" t="n">
+        <v>-0.9100000000001092</v>
+      </c>
+      <c r="S593" t="inlineStr">
+        <is>
+          <t>FA1AEC94F8F24AD000</t>
+        </is>
+      </c>
+      <c r="T593" t="inlineStr">
+        <is>
+          <t>FA1AEC958E14CAD000</t>
+        </is>
+      </c>
+      <c r="U593" t="inlineStr"/>
+      <c r="V593" t="inlineStr"/>
+      <c r="W593" t="inlineStr">
+        <is>
+          <t>FA1AEC958FEA97C000</t>
+        </is>
+      </c>
+      <c r="X593" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y593" t="inlineStr">
+        <is>
+          <t>mv :32.32, mv_2m:-0.31,mv_5m : -1.14, mv_30m : -2.64, mv_60m: -0.91, md_60m: -2c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z593" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA593" t="inlineStr">
+        <is>
+          <t>FA1AEC958EB20AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" s="1" t="n">
+        <v>592</v>
+      </c>
+      <c r="B594" t="n">
+        <v>4393</v>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D594" s="2" t="n">
+        <v>45840.23921135416</v>
+      </c>
+      <c r="E594" t="n">
+        <v>57.8987</v>
+      </c>
+      <c r="F594" t="n">
+        <v>1968.5558</v>
+      </c>
+      <c r="G594" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="H594" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I594" t="inlineStr"/>
+      <c r="J594" t="n">
+        <v>0</v>
+      </c>
+      <c r="K594" t="n">
+        <v>0</v>
+      </c>
+      <c r="L594" t="n">
+        <v>34</v>
+      </c>
+      <c r="M594" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N594" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O594" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P594" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q594" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="R594" t="n">
+        <v>0</v>
+      </c>
+      <c r="S594" t="inlineStr">
+        <is>
+          <t>FA1AECBDFB5B97C000</t>
+        </is>
+      </c>
+      <c r="T594" t="inlineStr">
+        <is>
+          <t>FA1AECBE57078AD000</t>
+        </is>
+      </c>
+      <c r="U594" t="inlineStr"/>
+      <c r="V594" t="inlineStr"/>
+      <c r="W594" t="inlineStr">
+        <is>
+          <t>FA1AECBE58F3CAD000</t>
+        </is>
+      </c>
+      <c r="X594" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y594" t="inlineStr">
+        <is>
+          <t>mv :37.83, mv_2m:0.48,mv_5m : 2.78, mv_30m : 3.20, mv_60m: 0.35, md_60m: -34c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z594" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA594" t="inlineStr">
+        <is>
+          <t>FA1AECBE5797D7C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" s="1" t="n">
+        <v>593</v>
+      </c>
+      <c r="B595" t="n">
+        <v>4394</v>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>ADM</t>
+        </is>
+      </c>
+      <c r="D595" s="2" t="n">
+        <v>45840.24952729166</v>
+      </c>
+      <c r="E595" t="n">
+        <v>54.3597</v>
+      </c>
+      <c r="F595" t="n">
+        <v>1956.9492</v>
+      </c>
+      <c r="G595" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H595" s="2" t="n">
+        <v>45841.26957667824</v>
+      </c>
+      <c r="I595" t="n">
+        <v>55.6818</v>
+      </c>
+      <c r="J595" t="n">
+        <v>2004.5448</v>
+      </c>
+      <c r="K595" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="L595" t="n">
+        <v>36</v>
+      </c>
+      <c r="M595" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N595" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O595" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P595" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q595" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R595" t="n">
+        <v>45.3856000000001</v>
+      </c>
+      <c r="S595" t="inlineStr">
+        <is>
+          <t>FA1AECC161C40AD000</t>
+        </is>
+      </c>
+      <c r="T595" t="inlineStr">
+        <is>
+          <t>FA1AECC268C817C000</t>
+        </is>
+      </c>
+      <c r="U595" t="inlineStr"/>
+      <c r="V595" t="inlineStr"/>
+      <c r="W595" t="inlineStr">
+        <is>
+          <t>FA1AECC26A9197C000</t>
+        </is>
+      </c>
+      <c r="X595" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y595" t="inlineStr">
+        <is>
+          <t>mv :35.14, mv_2m:-2.74,mv_5m : 1.00, mv_30m : -7.26, mv_60m: -8.95, md_60m: -53c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z595" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA595" t="inlineStr">
+        <is>
+          <t>FA1AECC269604AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" s="1" t="n">
+        <v>594</v>
+      </c>
+      <c r="B596" t="n">
+        <v>4395</v>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>XOM</t>
+        </is>
+      </c>
+      <c r="D596" s="2" t="n">
+        <v>45841.003339375</v>
+      </c>
+      <c r="E596" t="n">
+        <v>109.29</v>
+      </c>
+      <c r="F596" t="n">
+        <v>1530.06</v>
+      </c>
+      <c r="G596" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="H596" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I596" t="inlineStr"/>
+      <c r="J596" t="n">
+        <v>0</v>
+      </c>
+      <c r="K596" t="n">
+        <v>0</v>
+      </c>
+      <c r="L596" t="n">
+        <v>14</v>
+      </c>
+      <c r="M596" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N596" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O596" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P596" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q596" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="R596" t="n">
+        <v>0</v>
+      </c>
+      <c r="S596" t="inlineStr">
+        <is>
+          <t>FA1AEDB9D4A74AD000</t>
+        </is>
+      </c>
+      <c r="T596" t="inlineStr">
+        <is>
+          <t>FA1AEDBAE42257C000</t>
+        </is>
+      </c>
+      <c r="U596" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="V596" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="W596" t="inlineStr">
+        <is>
+          <t>FA1AEDBAE6048AD000</t>
+        </is>
+      </c>
+      <c r="X596" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y596" t="inlineStr">
+        <is>
+          <t>mv :-5.85, mv_2m:0.59,mv_5m : 1.15, mv_30m : 3.58, mv_60m: -6.65, md_60m: -13c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z596" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA596" t="inlineStr">
+        <is>
+          <t>FA1AEDBAE4B10AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" s="1" t="n">
+        <v>595</v>
+      </c>
+      <c r="B597" t="n">
+        <v>4396</v>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>FI</t>
+        </is>
+      </c>
+      <c r="D597" s="2" t="n">
+        <v>45842.07413511574</v>
+      </c>
+      <c r="E597" t="n">
+        <v>174.64</v>
+      </c>
+      <c r="F597" t="n">
+        <v>1921.04</v>
+      </c>
+      <c r="G597" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="H597" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I597" t="inlineStr"/>
+      <c r="J597" t="n">
+        <v>0</v>
+      </c>
+      <c r="K597" t="n">
+        <v>0</v>
+      </c>
+      <c r="L597" t="n">
+        <v>11</v>
+      </c>
+      <c r="M597" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N597" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O597" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P597" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q597" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="R597" t="n">
+        <v>0</v>
+      </c>
+      <c r="S597" t="inlineStr">
+        <is>
+          <t>FA1AEF1AC1130AD000</t>
+        </is>
+      </c>
+      <c r="T597" t="inlineStr">
+        <is>
+          <t>FA1AEF1B521497C000</t>
+        </is>
+      </c>
+      <c r="U597" t="inlineStr"/>
+      <c r="V597" t="inlineStr"/>
+      <c r="W597" t="inlineStr">
+        <is>
+          <t>FA1AEF1B54364AD000</t>
+        </is>
+      </c>
+      <c r="X597" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y597" t="inlineStr">
+        <is>
+          <t>mv :27.43, mv_2m:0.39,mv_5m : 0.77, mv_30m : 0.17, mv_60m: 1.17, md_60m: -4c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z597" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA597" t="inlineStr">
+        <is>
+          <t>FA1AEF1B52F497C000</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
improved buy and sell conditions
</commit_message>
<xml_diff>
--- a/db/real_trade_db.xlsx
+++ b/db/real_trade_db.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA597"/>
+  <dimension ref="A1:AA618"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -56942,21 +56942,23 @@
         <v>1.09</v>
       </c>
       <c r="H594" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I594" t="inlineStr"/>
+        <v>45847.01809327547</v>
+      </c>
+      <c r="I594" t="n">
+        <v>57.17</v>
+      </c>
       <c r="J594" t="n">
-        <v>0</v>
+        <v>1943.78</v>
       </c>
       <c r="K594" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="L594" t="n">
         <v>34</v>
       </c>
       <c r="M594" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N594" t="n">
@@ -56969,10 +56971,10 @@
         <v>1.006</v>
       </c>
       <c r="Q594" t="n">
-        <v>2.99</v>
+        <v>0.3</v>
       </c>
       <c r="R594" t="n">
-        <v>0</v>
+        <v>-26.96580000000012</v>
       </c>
       <c r="S594" t="inlineStr">
         <is>
@@ -57134,21 +57136,23 @@
         <v>1.03</v>
       </c>
       <c r="H596" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I596" t="inlineStr"/>
+        <v>45846.01879324074</v>
+      </c>
+      <c r="I596" t="n">
+        <v>111.12</v>
+      </c>
       <c r="J596" t="n">
-        <v>0</v>
+        <v>1555.68</v>
       </c>
       <c r="K596" t="n">
-        <v>0</v>
+        <v>1.04</v>
       </c>
       <c r="L596" t="n">
         <v>14</v>
       </c>
       <c r="M596" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N596" t="n">
@@ -57161,10 +57165,10 @@
         <v>1.006</v>
       </c>
       <c r="Q596" t="n">
-        <v>2.99</v>
+        <v>0.05</v>
       </c>
       <c r="R596" t="n">
-        <v>0</v>
+        <v>23.55000000000012</v>
       </c>
       <c r="S596" t="inlineStr">
         <is>
@@ -57176,16 +57180,8 @@
           <t>FA1AEDBAE42257C000</t>
         </is>
       </c>
-      <c r="U596" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="V596" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="U596" t="inlineStr"/>
+      <c r="V596" t="inlineStr"/>
       <c r="W596" t="inlineStr">
         <is>
           <t>FA1AEDBAE6048AD000</t>
@@ -57237,21 +57233,23 @@
         <v>1.02</v>
       </c>
       <c r="H597" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I597" t="inlineStr"/>
+        <v>45847.03790008102</v>
+      </c>
+      <c r="I597" t="n">
+        <v>171.02</v>
+      </c>
       <c r="J597" t="n">
-        <v>0</v>
+        <v>1881.22</v>
       </c>
       <c r="K597" t="n">
-        <v>0</v>
+        <v>1.03</v>
       </c>
       <c r="L597" t="n">
         <v>11</v>
       </c>
       <c r="M597" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N597" t="n">
@@ -57267,7 +57265,7 @@
         <v>2.99</v>
       </c>
       <c r="R597" t="n">
-        <v>0</v>
+        <v>-41.86999999999994</v>
       </c>
       <c r="S597" t="inlineStr">
         <is>
@@ -57304,6 +57302,2043 @@
       <c r="AA597" t="inlineStr">
         <is>
           <t>FA1AEF1B52F497C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" s="1" t="n">
+        <v>596</v>
+      </c>
+      <c r="B598" t="n">
+        <v>4397</v>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>PANW</t>
+        </is>
+      </c>
+      <c r="D598" s="2" t="n">
+        <v>45845.99309769676</v>
+      </c>
+      <c r="E598" t="n">
+        <v>200.61</v>
+      </c>
+      <c r="F598" t="n">
+        <v>1604.88</v>
+      </c>
+      <c r="G598" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H598" s="2" t="n">
+        <v>45846.19576506945</v>
+      </c>
+      <c r="I598" t="n">
+        <v>200.45</v>
+      </c>
+      <c r="J598" t="n">
+        <v>1603.6</v>
+      </c>
+      <c r="K598" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L598" t="n">
+        <v>8</v>
+      </c>
+      <c r="M598" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N598" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O598" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P598" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q598" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="R598" t="n">
+        <v>-3.3100000000002</v>
+      </c>
+      <c r="S598" t="inlineStr">
+        <is>
+          <t>FA1AF42667934AD000</t>
+        </is>
+      </c>
+      <c r="T598" t="inlineStr">
+        <is>
+          <t>FA1AF427589C97C000</t>
+        </is>
+      </c>
+      <c r="U598" t="inlineStr"/>
+      <c r="V598" t="inlineStr"/>
+      <c r="W598" t="inlineStr">
+        <is>
+          <t>FA1AF4275A5D57C000</t>
+        </is>
+      </c>
+      <c r="X598" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y598" t="inlineStr">
+        <is>
+          <t>mv :-6.32, mv_2m:0.23,mv_5m : -1.72, mv_30m : -1.89, mv_60m: -1.62, md_60m: -8c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z598" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA598" t="inlineStr">
+        <is>
+          <t>FA1AF427593257C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" s="1" t="n">
+        <v>597</v>
+      </c>
+      <c r="B599" t="n">
+        <v>4398</v>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>WELL</t>
+        </is>
+      </c>
+      <c r="D599" s="2" t="n">
+        <v>45846.18907966435</v>
+      </c>
+      <c r="E599" t="n">
+        <v>153.117</v>
+      </c>
+      <c r="F599" t="n">
+        <v>1684.287</v>
+      </c>
+      <c r="G599" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="H599" s="2" t="n">
+        <v>45847.04139300926</v>
+      </c>
+      <c r="I599" t="n">
+        <v>153.395</v>
+      </c>
+      <c r="J599" t="n">
+        <v>1687.345</v>
+      </c>
+      <c r="K599" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="L599" t="n">
+        <v>11</v>
+      </c>
+      <c r="M599" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N599" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O599" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P599" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q599" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R599" t="n">
+        <v>1.007999999999993</v>
+      </c>
+      <c r="S599" t="inlineStr">
+        <is>
+          <t>FA1AF466FF9097C000</t>
+        </is>
+      </c>
+      <c r="T599" t="inlineStr">
+        <is>
+          <t>FA1AF467B0F94AD000</t>
+        </is>
+      </c>
+      <c r="U599" t="inlineStr"/>
+      <c r="V599" t="inlineStr"/>
+      <c r="W599" t="inlineStr">
+        <is>
+          <t>FA1AF467B2BC0AD000</t>
+        </is>
+      </c>
+      <c r="X599" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y599" t="inlineStr">
+        <is>
+          <t>mv :-35.45, mv_2m:-0.15,mv_5m : -5.85, mv_30m : -27.63, mv_60m: -30.83, md_60m: -94c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z599" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA599" t="inlineStr">
+        <is>
+          <t>FA1AF467B1990AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" s="1" t="n">
+        <v>598</v>
+      </c>
+      <c r="B600" t="n">
+        <v>4399</v>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>INTC</t>
+        </is>
+      </c>
+      <c r="D600" s="2" t="n">
+        <v>45847.0857991088</v>
+      </c>
+      <c r="E600" t="n">
+        <v>23.2097</v>
+      </c>
+      <c r="F600" t="n">
+        <v>1996.0342</v>
+      </c>
+      <c r="G600" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="H600" s="2" t="n">
+        <v>45848.01828075232</v>
+      </c>
+      <c r="I600" t="n">
+        <v>23.4003</v>
+      </c>
+      <c r="J600" t="n">
+        <v>2012.4258</v>
+      </c>
+      <c r="K600" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="L600" t="n">
+        <v>86</v>
+      </c>
+      <c r="M600" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N600" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O600" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P600" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q600" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R600" t="n">
+        <v>13.88160000000015</v>
+      </c>
+      <c r="S600" t="inlineStr">
+        <is>
+          <t>FA1AF58E8BA44AD000</t>
+        </is>
+      </c>
+      <c r="T600" t="inlineStr">
+        <is>
+          <t>FA1AF58F091B4AD000</t>
+        </is>
+      </c>
+      <c r="U600" t="inlineStr"/>
+      <c r="V600" t="inlineStr"/>
+      <c r="W600" t="inlineStr">
+        <is>
+          <t>FA1AF58F0AD617C000</t>
+        </is>
+      </c>
+      <c r="X600" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y600" t="inlineStr">
+        <is>
+          <t>mv :-7.21, mv_2m:-0.26,mv_5m : -0.26, mv_30m : -2.24, mv_60m: -2.56, md_60m: -5c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z600" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA600" t="inlineStr">
+        <is>
+          <t>FA1AF58F09AED7C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" s="1" t="n">
+        <v>599</v>
+      </c>
+      <c r="B601" t="n">
+        <v>4400</v>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>MCHP</t>
+        </is>
+      </c>
+      <c r="D601" s="2" t="n">
+        <v>45847.09491254629</v>
+      </c>
+      <c r="E601" t="n">
+        <v>74.2594</v>
+      </c>
+      <c r="F601" t="n">
+        <v>1930.7444</v>
+      </c>
+      <c r="G601" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="H601" s="2" t="n">
+        <v>45848.05264450231</v>
+      </c>
+      <c r="I601" t="n">
+        <v>74.6208</v>
+      </c>
+      <c r="J601" t="n">
+        <v>1940.1408</v>
+      </c>
+      <c r="K601" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="L601" t="n">
+        <v>26</v>
+      </c>
+      <c r="M601" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N601" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O601" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P601" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q601" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R601" t="n">
+        <v>7.246400000000085</v>
+      </c>
+      <c r="S601" t="inlineStr">
+        <is>
+          <t>FA1AF5918C9617C000</t>
+        </is>
+      </c>
+      <c r="T601" t="inlineStr">
+        <is>
+          <t>FA1AF591C6590AD000</t>
+        </is>
+      </c>
+      <c r="U601" t="inlineStr"/>
+      <c r="V601" t="inlineStr"/>
+      <c r="W601" t="inlineStr">
+        <is>
+          <t>FA1AF591C80D8AD000</t>
+        </is>
+      </c>
+      <c r="X601" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y601" t="inlineStr">
+        <is>
+          <t>mv :-11.02, mv_2m:0.43,mv_5m : -0.07, mv_30m : -7.95, mv_60m: -16.71, md_60m: -47c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z601" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA601" t="inlineStr">
+        <is>
+          <t>FA1AF591C6ED17C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" s="1" t="n">
+        <v>600</v>
+      </c>
+      <c r="B602" t="n">
+        <v>4401</v>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>LLY</t>
+        </is>
+      </c>
+      <c r="D602" s="2" t="n">
+        <v>45847.09697940973</v>
+      </c>
+      <c r="E602" t="n">
+        <v>789.95</v>
+      </c>
+      <c r="F602" t="n">
+        <v>1579.9</v>
+      </c>
+      <c r="G602" t="n">
+        <v>1</v>
+      </c>
+      <c r="H602" s="2" t="n">
+        <v>45847.16724581018</v>
+      </c>
+      <c r="I602" t="n">
+        <v>773.38</v>
+      </c>
+      <c r="J602" t="n">
+        <v>1546.76</v>
+      </c>
+      <c r="K602" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="L602" t="n">
+        <v>2</v>
+      </c>
+      <c r="M602" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N602" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O602" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P602" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q602" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="R602" t="n">
+        <v>-35.1500000000001</v>
+      </c>
+      <c r="S602" t="inlineStr">
+        <is>
+          <t>FA1AF5923AF94AD000</t>
+        </is>
+      </c>
+      <c r="T602" t="inlineStr">
+        <is>
+          <t>FA1AF592EC0FCAD000</t>
+        </is>
+      </c>
+      <c r="U602" t="inlineStr"/>
+      <c r="V602" t="inlineStr"/>
+      <c r="W602" t="inlineStr">
+        <is>
+          <t>FA1AF592EDCF97C000</t>
+        </is>
+      </c>
+      <c r="X602" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y602" t="inlineStr">
+        <is>
+          <t>mv :-9.55, mv_2m:1.10,mv_5m : 3.04, mv_30m : -8.56, mv_60m: -14.32, md_60m: -43c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z602" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA602" t="inlineStr">
+        <is>
+          <t>FA1AF592ECAE0AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" s="1" t="n">
+        <v>601</v>
+      </c>
+      <c r="B603" t="n">
+        <v>4402</v>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>SBUX</t>
+        </is>
+      </c>
+      <c r="D603" s="2" t="n">
+        <v>45847.13725704861</v>
+      </c>
+      <c r="E603" t="n">
+        <v>94.9293</v>
+      </c>
+      <c r="F603" t="n">
+        <v>1518.8688</v>
+      </c>
+      <c r="G603" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="H603" s="2" t="n">
+        <v>45847.28520521991</v>
+      </c>
+      <c r="I603" t="n">
+        <v>95.0111</v>
+      </c>
+      <c r="J603" t="n">
+        <v>1520.1776</v>
+      </c>
+      <c r="K603" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="L603" t="n">
+        <v>16</v>
+      </c>
+      <c r="M603" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N603" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O603" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P603" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q603" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R603" t="n">
+        <v>-0.7811999999999808</v>
+      </c>
+      <c r="S603" t="inlineStr">
+        <is>
+          <t>FA1AF59F815CD7C000</t>
+        </is>
+      </c>
+      <c r="T603" t="inlineStr">
+        <is>
+          <t>FA1AF59FBD71CAD000</t>
+        </is>
+      </c>
+      <c r="U603" t="inlineStr"/>
+      <c r="V603" t="inlineStr"/>
+      <c r="W603" t="inlineStr">
+        <is>
+          <t>FA1AF59FBF2397C000</t>
+        </is>
+      </c>
+      <c r="X603" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y603" t="inlineStr">
+        <is>
+          <t>mv :-7.96, mv_2m:-1.95,mv_5m : 1.60, mv_30m : -4.28, mv_60m: -2.63, md_60m: -29c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z603" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA603" t="inlineStr">
+        <is>
+          <t>FA1AF59FBE028AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" s="1" t="n">
+        <v>602</v>
+      </c>
+      <c r="B604" t="n">
+        <v>4403</v>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>INTC</t>
+        </is>
+      </c>
+      <c r="D604" s="2" t="n">
+        <v>45847.99162548611</v>
+      </c>
+      <c r="E604" t="n">
+        <v>23.4589</v>
+      </c>
+      <c r="F604" t="n">
+        <v>1994.0065</v>
+      </c>
+      <c r="G604" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="H604" s="2" t="n">
+        <v>45848.03354096065</v>
+      </c>
+      <c r="I604" t="n">
+        <v>23.3803</v>
+      </c>
+      <c r="J604" t="n">
+        <v>1987.3255</v>
+      </c>
+      <c r="K604" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="L604" t="n">
+        <v>85</v>
+      </c>
+      <c r="M604" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N604" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O604" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P604" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q604" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R604" t="n">
+        <v>-9.19100000000004</v>
+      </c>
+      <c r="S604" t="inlineStr">
+        <is>
+          <t>FA1AF6B9194DCAD000</t>
+        </is>
+      </c>
+      <c r="T604" t="inlineStr">
+        <is>
+          <t>FA1AF6B9A0B1D7C000</t>
+        </is>
+      </c>
+      <c r="U604" t="inlineStr"/>
+      <c r="V604" t="inlineStr"/>
+      <c r="W604" t="inlineStr">
+        <is>
+          <t>FA1AF6B9A27B17C000</t>
+        </is>
+      </c>
+      <c r="X604" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y604" t="inlineStr">
+        <is>
+          <t>mv :1.72, mv_2m:0.16,mv_5m : 0.25, mv_30m : -0.27, mv_60m: 0.40, md_60m: -1c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z604" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA604" t="inlineStr">
+        <is>
+          <t>FA1AF6B9A1564AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" s="1" t="n">
+        <v>603</v>
+      </c>
+      <c r="B605" t="n">
+        <v>4404</v>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>RTX</t>
+        </is>
+      </c>
+      <c r="D605" s="2" t="n">
+        <v>45848.13101875</v>
+      </c>
+      <c r="E605" t="n">
+        <v>145.92</v>
+      </c>
+      <c r="F605" t="n">
+        <v>1896.96</v>
+      </c>
+      <c r="G605" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="H605" s="2" t="n">
+        <v>45849.02554996528</v>
+      </c>
+      <c r="I605" t="n">
+        <v>145.92</v>
+      </c>
+      <c r="J605" t="n">
+        <v>1896.96</v>
+      </c>
+      <c r="K605" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="L605" t="n">
+        <v>13</v>
+      </c>
+      <c r="M605" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N605" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O605" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P605" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q605" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R605" t="n">
+        <v>-2.070000000000228</v>
+      </c>
+      <c r="S605" t="inlineStr">
+        <is>
+          <t>FA1AF6E70A784AD000</t>
+        </is>
+      </c>
+      <c r="T605" t="inlineStr">
+        <is>
+          <t>FA1AF6E7701357C000</t>
+        </is>
+      </c>
+      <c r="U605" t="inlineStr"/>
+      <c r="V605" t="inlineStr"/>
+      <c r="W605" t="inlineStr">
+        <is>
+          <t>FA1AF6E771EBD7C000</t>
+        </is>
+      </c>
+      <c r="X605" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y605" t="inlineStr">
+        <is>
+          <t>mv :1.88, mv_2m:0.16,mv_5m : -0.14, mv_30m : 3.55, mv_60m: 2.12, md_60m: -17c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z605" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA605" t="inlineStr">
+        <is>
+          <t>FA1AF6E770BC17C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" s="1" t="n">
+        <v>604</v>
+      </c>
+      <c r="B606" t="n">
+        <v>4405</v>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
+      <c r="D606" s="2" t="n">
+        <v>45848.18197834491</v>
+      </c>
+      <c r="E606" t="n">
+        <v>250.0283</v>
+      </c>
+      <c r="F606" t="n">
+        <v>1750.1981</v>
+      </c>
+      <c r="G606" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H606" s="2" t="n">
+        <v>45848.23518974537</v>
+      </c>
+      <c r="I606" t="n">
+        <v>249.7954</v>
+      </c>
+      <c r="J606" t="n">
+        <v>1748.5678</v>
+      </c>
+      <c r="K606" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L606" t="n">
+        <v>7</v>
+      </c>
+      <c r="M606" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N606" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O606" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P606" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q606" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R606" t="n">
+        <v>-3.660300000000034</v>
+      </c>
+      <c r="S606" t="inlineStr">
+        <is>
+          <t>FA1AF6F7D62217C000</t>
+        </is>
+      </c>
+      <c r="T606" t="inlineStr">
+        <is>
+          <t>FA1AF6F83B4DD7C000</t>
+        </is>
+      </c>
+      <c r="U606" t="inlineStr"/>
+      <c r="V606" t="inlineStr"/>
+      <c r="W606" t="inlineStr">
+        <is>
+          <t>FA1AF6F83D1B97C000</t>
+        </is>
+      </c>
+      <c r="X606" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y606" t="inlineStr">
+        <is>
+          <t>mv :-1.35, mv_2m:-0.64,mv_5m : -0.34, mv_30m : -0.41, mv_60m: -0.01, md_60m: -14c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z606" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA606" t="inlineStr">
+        <is>
+          <t>FA1AF6F83BE197C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" s="1" t="n">
+        <v>605</v>
+      </c>
+      <c r="B607" t="n">
+        <v>4406</v>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="D607" s="2" t="n">
+        <v>45848.23129435186</v>
+      </c>
+      <c r="E607" t="n">
+        <v>139.0177</v>
+      </c>
+      <c r="F607" t="n">
+        <v>1946.2478</v>
+      </c>
+      <c r="G607" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="H607" s="2" t="n">
+        <v>45848.28271886574</v>
+      </c>
+      <c r="I607" t="n">
+        <v>138.3102</v>
+      </c>
+      <c r="J607" t="n">
+        <v>1936.3428</v>
+      </c>
+      <c r="K607" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="L607" t="n">
+        <v>14</v>
+      </c>
+      <c r="M607" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N607" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O607" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P607" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q607" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R607" t="n">
+        <v>-11.97499999999997</v>
+      </c>
+      <c r="S607" t="inlineStr">
+        <is>
+          <t>FA1AF708172D57C000</t>
+        </is>
+      </c>
+      <c r="T607" t="inlineStr">
+        <is>
+          <t>FA1AF7089BC757C000</t>
+        </is>
+      </c>
+      <c r="U607" t="inlineStr"/>
+      <c r="V607" t="inlineStr"/>
+      <c r="W607" t="inlineStr">
+        <is>
+          <t>FA1AF7089D9F57C000</t>
+        </is>
+      </c>
+      <c r="X607" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y607" t="inlineStr">
+        <is>
+          <t>mv :-0.39, mv_2m:0.21,mv_5m : -0.04, mv_30m : 1.28, mv_60m: 2.84, md_60m: -1c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z607" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA607" t="inlineStr">
+        <is>
+          <t>FA1AF7089C6117C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" s="1" t="n">
+        <v>606</v>
+      </c>
+      <c r="B608" t="n">
+        <v>4407</v>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="D608" s="2" t="n">
+        <v>45849.03112979166</v>
+      </c>
+      <c r="E608" t="n">
+        <v>178.235</v>
+      </c>
+      <c r="F608" t="n">
+        <v>1960.585</v>
+      </c>
+      <c r="G608" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="H608" s="2" t="n">
+        <v>45849.07687009259</v>
+      </c>
+      <c r="I608" t="n">
+        <v>178.15</v>
+      </c>
+      <c r="J608" t="n">
+        <v>1959.65</v>
+      </c>
+      <c r="K608" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="L608" t="n">
+        <v>11</v>
+      </c>
+      <c r="M608" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N608" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O608" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P608" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q608" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R608" t="n">
+        <v>-2.984999999999945</v>
+      </c>
+      <c r="S608" t="inlineStr">
+        <is>
+          <t>FA1AF80FB5914AD000</t>
+        </is>
+      </c>
+      <c r="T608" t="inlineStr">
+        <is>
+          <t>FA1AF81008170AD000</t>
+        </is>
+      </c>
+      <c r="U608" t="inlineStr"/>
+      <c r="V608" t="inlineStr"/>
+      <c r="W608" t="inlineStr">
+        <is>
+          <t>FA1AF81009E997C000</t>
+        </is>
+      </c>
+      <c r="X608" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y608" t="inlineStr">
+        <is>
+          <t>mv :0.48, mv_2m:0.45,mv_5m : 2.59, mv_30m : 9.13, mv_60m: 24.48, md_60m: 20c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z608" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA608" t="inlineStr">
+        <is>
+          <t>FA1AF81008AB57C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" s="1" t="n">
+        <v>607</v>
+      </c>
+      <c r="B609" t="n">
+        <v>4408</v>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="D609" s="2" t="n">
+        <v>45849.06373532407</v>
+      </c>
+      <c r="E609" t="n">
+        <v>144.0489</v>
+      </c>
+      <c r="F609" t="n">
+        <v>1872.6357</v>
+      </c>
+      <c r="G609" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="H609" s="2" t="n">
+        <v>45849.2310037963</v>
+      </c>
+      <c r="I609" t="n">
+        <v>143.8601</v>
+      </c>
+      <c r="J609" t="n">
+        <v>1870.1813</v>
+      </c>
+      <c r="K609" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="L609" t="n">
+        <v>13</v>
+      </c>
+      <c r="M609" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N609" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O609" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P609" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q609" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R609" t="n">
+        <v>-4.524400000000306</v>
+      </c>
+      <c r="S609" t="inlineStr">
+        <is>
+          <t>FA1AF81A74A997C000</t>
+        </is>
+      </c>
+      <c r="T609" t="inlineStr">
+        <is>
+          <t>FA1AF81AF1884AD000</t>
+        </is>
+      </c>
+      <c r="U609" t="inlineStr"/>
+      <c r="V609" t="inlineStr"/>
+      <c r="W609" t="inlineStr">
+        <is>
+          <t>FA1AF81AF34717C000</t>
+        </is>
+      </c>
+      <c r="X609" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y609" t="inlineStr">
+        <is>
+          <t>mv :2.81, mv_2m:0.32,mv_5m : 0.49, mv_30m : 0.54, mv_60m: 3.65, md_60m: 3c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z609" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA609" t="inlineStr">
+        <is>
+          <t>FA1AF81AF21D0AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" s="1" t="n">
+        <v>608</v>
+      </c>
+      <c r="B610" t="n">
+        <v>4409</v>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>MDT</t>
+        </is>
+      </c>
+      <c r="D610" s="2" t="n">
+        <v>45849.07251065972</v>
+      </c>
+      <c r="E610" t="n">
+        <v>90.0287</v>
+      </c>
+      <c r="F610" t="n">
+        <v>1980.6314</v>
+      </c>
+      <c r="G610" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="H610" s="2" t="n">
+        <v>45849.23012575231</v>
+      </c>
+      <c r="I610" t="n">
+        <v>89.8203</v>
+      </c>
+      <c r="J610" t="n">
+        <v>1976.0466</v>
+      </c>
+      <c r="K610" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="L610" t="n">
+        <v>22</v>
+      </c>
+      <c r="M610" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N610" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O610" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P610" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q610" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R610" t="n">
+        <v>-6.71479999999986</v>
+      </c>
+      <c r="S610" t="inlineStr">
+        <is>
+          <t>FA1AF81D591497C000</t>
+        </is>
+      </c>
+      <c r="T610" t="inlineStr">
+        <is>
+          <t>FA1AF81D9C568AD000</t>
+        </is>
+      </c>
+      <c r="U610" t="inlineStr"/>
+      <c r="V610" t="inlineStr"/>
+      <c r="W610" t="inlineStr">
+        <is>
+          <t>FA1AF81D9E16D7C000</t>
+        </is>
+      </c>
+      <c r="X610" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y610" t="inlineStr">
+        <is>
+          <t>mv :0.40, mv_2m:0.58,mv_5m : -0.28, mv_30m : -0.96, mv_60m: -0.47, md_60m: -21c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z610" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA610" t="inlineStr">
+        <is>
+          <t>FA1AF81D9CF8CAD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" s="1" t="n">
+        <v>609</v>
+      </c>
+      <c r="B611" t="n">
+        <v>4410</v>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>ABT</t>
+        </is>
+      </c>
+      <c r="D611" s="2" t="n">
+        <v>45849.07408901621</v>
+      </c>
+      <c r="E611" t="n">
+        <v>134.38</v>
+      </c>
+      <c r="F611" t="n">
+        <v>1612.56</v>
+      </c>
+      <c r="G611" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="H611" s="2" t="n">
+        <v>45849.12419916667</v>
+      </c>
+      <c r="I611" t="n">
+        <v>134.273</v>
+      </c>
+      <c r="J611" t="n">
+        <v>1611.276</v>
+      </c>
+      <c r="K611" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="L611" t="n">
+        <v>12</v>
+      </c>
+      <c r="M611" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N611" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O611" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P611" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q611" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R611" t="n">
+        <v>-3.354000000000106</v>
+      </c>
+      <c r="S611" t="inlineStr">
+        <is>
+          <t>FA1AF81DDE3FD7C000</t>
+        </is>
+      </c>
+      <c r="T611" t="inlineStr">
+        <is>
+          <t>FA1AF81E384357C000</t>
+        </is>
+      </c>
+      <c r="U611" t="inlineStr"/>
+      <c r="V611" t="inlineStr"/>
+      <c r="W611" t="inlineStr">
+        <is>
+          <t>FA1AF81E3A0D0AD000</t>
+        </is>
+      </c>
+      <c r="X611" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y611" t="inlineStr">
+        <is>
+          <t>mv :0.24, mv_2m:-0.14,mv_5m : 0.19, mv_30m : -2.96, mv_60m: 0.78, md_60m: -19c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z611" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA611" t="inlineStr">
+        <is>
+          <t>FA1AF81E38D6D7C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" s="1" t="n">
+        <v>610</v>
+      </c>
+      <c r="B612" t="n">
+        <v>4411</v>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>ABBV</t>
+        </is>
+      </c>
+      <c r="D612" s="2" t="n">
+        <v>45849.08576494213</v>
+      </c>
+      <c r="E612" t="n">
+        <v>195.15</v>
+      </c>
+      <c r="F612" t="n">
+        <v>1561.2</v>
+      </c>
+      <c r="G612" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H612" s="2" t="n">
+        <v>45849.2695047338</v>
+      </c>
+      <c r="I612" t="n">
+        <v>195.3911</v>
+      </c>
+      <c r="J612" t="n">
+        <v>1563.1288</v>
+      </c>
+      <c r="K612" t="n">
+        <v>1.101</v>
+      </c>
+      <c r="L612" t="n">
+        <v>8</v>
+      </c>
+      <c r="M612" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N612" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O612" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P612" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q612" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R612" t="n">
+        <v>-0.1822000000000898</v>
+      </c>
+      <c r="S612" t="inlineStr">
+        <is>
+          <t>FA1AF821B76717C000</t>
+        </is>
+      </c>
+      <c r="T612" t="inlineStr">
+        <is>
+          <t>FA1AF8227073CAD000</t>
+        </is>
+      </c>
+      <c r="U612" t="inlineStr"/>
+      <c r="V612" t="inlineStr"/>
+      <c r="W612" t="inlineStr">
+        <is>
+          <t>FA1AF82272488AD000</t>
+        </is>
+      </c>
+      <c r="X612" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y612" t="inlineStr">
+        <is>
+          <t>mv :-1.90, mv_2m:0.97,mv_5m : 1.73, mv_30m : -8.94, mv_60m: -6.41, md_60m: -46c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z612" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA612" t="inlineStr">
+        <is>
+          <t>FA1AF822710A97C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" s="1" t="n">
+        <v>611</v>
+      </c>
+      <c r="B613" t="n">
+        <v>4412</v>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>DHR</t>
+        </is>
+      </c>
+      <c r="D613" s="2" t="n">
+        <v>45849.19834469907</v>
+      </c>
+      <c r="E613" t="n">
+        <v>206.3295</v>
+      </c>
+      <c r="F613" t="n">
+        <v>1856.9655</v>
+      </c>
+      <c r="G613" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="H613" s="2" t="n">
+        <v>45849.24387465278</v>
+      </c>
+      <c r="I613" t="n">
+        <v>205.8</v>
+      </c>
+      <c r="J613" t="n">
+        <v>1852.2</v>
+      </c>
+      <c r="K613" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="L613" t="n">
+        <v>9</v>
+      </c>
+      <c r="M613" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N613" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O613" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P613" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q613" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R613" t="n">
+        <v>-6.825499999999974</v>
+      </c>
+      <c r="S613" t="inlineStr">
+        <is>
+          <t>FA1AF846D249D7C000</t>
+        </is>
+      </c>
+      <c r="T613" t="inlineStr">
+        <is>
+          <t>FA1AF8474C52CAD000</t>
+        </is>
+      </c>
+      <c r="U613" t="inlineStr"/>
+      <c r="V613" t="inlineStr"/>
+      <c r="W613" t="inlineStr">
+        <is>
+          <t>FA1AF8474E1E8AD000</t>
+        </is>
+      </c>
+      <c r="X613" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y613" t="inlineStr">
+        <is>
+          <t>mv :-2.31, mv_2m:-0.10,mv_5m : 0.03, mv_30m : -1.83, mv_60m: -3.24, md_60m: -19c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z613" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA613" t="inlineStr">
+        <is>
+          <t>FA1AF8474CF6CAD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" s="1" t="n">
+        <v>612</v>
+      </c>
+      <c r="B614" t="n">
+        <v>4413</v>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>WELL</t>
+        </is>
+      </c>
+      <c r="D614" s="2" t="n">
+        <v>45849.1993509838</v>
+      </c>
+      <c r="E614" t="n">
+        <v>152.9347</v>
+      </c>
+      <c r="F614" t="n">
+        <v>1988.1511</v>
+      </c>
+      <c r="G614" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="H614" s="2" t="n">
+        <v>45849.28267967593</v>
+      </c>
+      <c r="I614" t="n">
+        <v>152.7</v>
+      </c>
+      <c r="J614" t="n">
+        <v>1985.1</v>
+      </c>
+      <c r="K614" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="L614" t="n">
+        <v>13</v>
+      </c>
+      <c r="M614" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N614" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O614" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P614" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q614" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="R614" t="n">
+        <v>-5.121100000000133</v>
+      </c>
+      <c r="S614" t="inlineStr">
+        <is>
+          <t>FA1AF8472731D7C000</t>
+        </is>
+      </c>
+      <c r="T614" t="inlineStr">
+        <is>
+          <t>FA1AF847DF0D0AD000</t>
+        </is>
+      </c>
+      <c r="U614" t="inlineStr"/>
+      <c r="V614" t="inlineStr"/>
+      <c r="W614" t="inlineStr">
+        <is>
+          <t>FA1AF847E0C797C000</t>
+        </is>
+      </c>
+      <c r="X614" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y614" t="inlineStr">
+        <is>
+          <t>mv :-3.92, mv_2m:-1.70,mv_5m : -2.71, mv_30m : -5.31, mv_60m: -7.71, md_60m: -68c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z614" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA614" t="inlineStr">
+        <is>
+          <t>FA1AF847DFA017C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" s="1" t="n">
+        <v>613</v>
+      </c>
+      <c r="B615" t="n">
+        <v>4414</v>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>CMG</t>
+        </is>
+      </c>
+      <c r="D615" s="2" t="n">
+        <v>45849.21469648148</v>
+      </c>
+      <c r="E615" t="n">
+        <v>56.6888</v>
+      </c>
+      <c r="F615" t="n">
+        <v>1927.4192</v>
+      </c>
+      <c r="G615" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="H615" s="2" t="n">
+        <v>45849.27384170139</v>
+      </c>
+      <c r="I615" t="n">
+        <v>56.5502</v>
+      </c>
+      <c r="J615" t="n">
+        <v>1922.7068</v>
+      </c>
+      <c r="K615" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="L615" t="n">
+        <v>34</v>
+      </c>
+      <c r="M615" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N615" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O615" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P615" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q615" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R615" t="n">
+        <v>-6.902400000000116</v>
+      </c>
+      <c r="S615" t="inlineStr">
+        <is>
+          <t>FA1AF84C35F48AD000</t>
+        </is>
+      </c>
+      <c r="T615" t="inlineStr">
+        <is>
+          <t>FA1AF84CCD4117C000</t>
+        </is>
+      </c>
+      <c r="U615" t="inlineStr"/>
+      <c r="V615" t="inlineStr"/>
+      <c r="W615" t="inlineStr">
+        <is>
+          <t>FA1AF84CCEF497C000</t>
+        </is>
+      </c>
+      <c r="X615" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y615" t="inlineStr">
+        <is>
+          <t>mv :-4.85, mv_2m:0.09,mv_5m : 0.35, mv_30m : 1.06, mv_60m: 0.93, md_60m: 0c1: 1, c2: 0</t>
+        </is>
+      </c>
+      <c r="Z615" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA615" t="inlineStr">
+        <is>
+          <t>FA1AF84CCDD597C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" s="1" t="n">
+        <v>614</v>
+      </c>
+      <c r="B616" t="n">
+        <v>4415</v>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>RTX</t>
+        </is>
+      </c>
+      <c r="D616" s="2" t="n">
+        <v>45850.04046799769</v>
+      </c>
+      <c r="E616" t="n">
+        <v>146.5387</v>
+      </c>
+      <c r="F616" t="n">
+        <v>1905.0031</v>
+      </c>
+      <c r="G616" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="H616" s="2" t="n">
+        <v>45850.11751971065</v>
+      </c>
+      <c r="I616" t="n">
+        <v>146.1705</v>
+      </c>
+      <c r="J616" t="n">
+        <v>1900.2165</v>
+      </c>
+      <c r="K616" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="L616" t="n">
+        <v>13</v>
+      </c>
+      <c r="M616" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N616" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O616" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P616" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q616" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R616" t="n">
+        <v>-6.856599999999908</v>
+      </c>
+      <c r="S616" t="inlineStr">
+        <is>
+          <t>FA1AF95C606A97C000</t>
+        </is>
+      </c>
+      <c r="T616" t="inlineStr">
+        <is>
+          <t>FA1AF95D0AA18AD000</t>
+        </is>
+      </c>
+      <c r="U616" t="inlineStr"/>
+      <c r="V616" t="inlineStr"/>
+      <c r="W616" t="inlineStr">
+        <is>
+          <t>FA1AF95D0CA08AD000</t>
+        </is>
+      </c>
+      <c r="X616" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y616" t="inlineStr">
+        <is>
+          <t>mv :-0.14, mv_2m:0.91,mv_5m : 0.68, mv_30m : -1.41, mv_60m: 3.57, md_60m: 0c1: 1, c2: 0, c9: 1</t>
+        </is>
+      </c>
+      <c r="Z616" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA616" t="inlineStr">
+        <is>
+          <t>FA1AF95D0B34D7C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" s="1" t="n">
+        <v>615</v>
+      </c>
+      <c r="B617" t="n">
+        <v>4416</v>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>WMB</t>
+        </is>
+      </c>
+      <c r="D617" s="2" t="n">
+        <v>45850.04144208333</v>
+      </c>
+      <c r="E617" t="n">
+        <v>58.3998</v>
+      </c>
+      <c r="F617" t="n">
+        <v>1985.5932</v>
+      </c>
+      <c r="G617" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="H617" s="2" t="n">
+        <v>45850.28306538195</v>
+      </c>
+      <c r="I617" t="n">
+        <v>58.1409</v>
+      </c>
+      <c r="J617" t="n">
+        <v>1976.7906</v>
+      </c>
+      <c r="K617" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="L617" t="n">
+        <v>34</v>
+      </c>
+      <c r="M617" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N617" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O617" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P617" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q617" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R617" t="n">
+        <v>-10.99259999999998</v>
+      </c>
+      <c r="S617" t="inlineStr">
+        <is>
+          <t>FA1AF95CB2994AD000</t>
+        </is>
+      </c>
+      <c r="T617" t="inlineStr">
+        <is>
+          <t>FA1AF95DA376CAD000</t>
+        </is>
+      </c>
+      <c r="U617" t="inlineStr"/>
+      <c r="V617" t="inlineStr"/>
+      <c r="W617" t="inlineStr">
+        <is>
+          <t>FA1AF95DA5344AD000</t>
+        </is>
+      </c>
+      <c r="X617" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y617" t="inlineStr">
+        <is>
+          <t>mv :-0.01, mv_2m:1.05,mv_5m : 5.15, mv_30m : -2.42, mv_60m: 11.38, md_60m: -5c1: 1, c2: 0, c9: 1</t>
+        </is>
+      </c>
+      <c r="Z617" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA617" t="inlineStr">
+        <is>
+          <t>FA1AF95DA40957C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" s="1" t="n">
+        <v>616</v>
+      </c>
+      <c r="B618" t="n">
+        <v>4417</v>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>NSC</t>
+        </is>
+      </c>
+      <c r="D618" s="2" t="n">
+        <v>45850.05836446759</v>
+      </c>
+      <c r="E618" t="n">
+        <v>267.26</v>
+      </c>
+      <c r="F618" t="n">
+        <v>1336.3</v>
+      </c>
+      <c r="G618" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H618" s="2" t="n">
+        <v>45850.21847697916</v>
+      </c>
+      <c r="I618" t="n">
+        <v>265.974</v>
+      </c>
+      <c r="J618" t="n">
+        <v>1329.87</v>
+      </c>
+      <c r="K618" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L618" t="n">
+        <v>5</v>
+      </c>
+      <c r="M618" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N618" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O618" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P618" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q618" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R618" t="n">
+        <v>-8.460000000000063</v>
+      </c>
+      <c r="S618" t="inlineStr">
+        <is>
+          <t>FA1AF962466E57C000</t>
+        </is>
+      </c>
+      <c r="T618" t="inlineStr">
+        <is>
+          <t>FA1AF9628316D7C000</t>
+        </is>
+      </c>
+      <c r="U618" t="inlineStr"/>
+      <c r="V618" t="inlineStr"/>
+      <c r="W618" t="inlineStr">
+        <is>
+          <t>FA1AF96284D4CAD000</t>
+        </is>
+      </c>
+      <c r="X618" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y618" t="inlineStr">
+        <is>
+          <t>mv :-1.00, mv_2m:1.18,mv_5m : 4.42, mv_30m : -1.07, mv_60m: -7.87, md_60m: -55c1: 1, c2: 0, c9: 1</t>
+        </is>
+      </c>
+      <c r="Z618" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA618" t="inlineStr">
+        <is>
+          <t>FA1AF96283AA57C000</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
before modify before market open condition
</commit_message>
<xml_diff>
--- a/db/real_trade_db.xlsx
+++ b/db/real_trade_db.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA850"/>
+  <dimension ref="A1:AA866"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -80765,41 +80765,41 @@
         <v>838</v>
       </c>
       <c r="B840" t="n">
-        <v>4667</v>
+        <v>4669</v>
       </c>
       <c r="C840" t="inlineStr">
         <is>
-          <t>SCHW</t>
+          <t>NEE</t>
         </is>
       </c>
       <c r="D840" s="2" t="n">
-        <v>45920.08007607639</v>
+        <v>45920.09996373842</v>
       </c>
       <c r="E840" t="n">
-        <v>93.39</v>
+        <v>70.92</v>
       </c>
       <c r="F840" t="n">
-        <v>2428.14</v>
-      </c>
-      <c r="G840" t="n">
-        <v>1.111</v>
-      </c>
+        <v>2482.2</v>
+      </c>
+      <c r="G840" t="inlineStr"/>
       <c r="H840" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I840" t="inlineStr"/>
+        <v>45920.15402466435</v>
+      </c>
+      <c r="I840" t="n">
+        <v>70.7303</v>
+      </c>
       <c r="J840" t="n">
-        <v>0</v>
+        <v>2475.5605</v>
       </c>
       <c r="K840" t="n">
-        <v>0</v>
+        <v>1.11</v>
       </c>
       <c r="L840" t="n">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="M840" t="inlineStr">
         <is>
-          <t>cancelled</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N840" t="n">
@@ -80812,20 +80812,26 @@
         <v>1.006</v>
       </c>
       <c r="Q840" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="R840" t="n">
-        <v>0</v>
-      </c>
+        <v>0.05</v>
+      </c>
+      <c r="R840" t="inlineStr"/>
       <c r="S840" t="inlineStr">
         <is>
-          <t>FA1B5388B86B8AD000</t>
-        </is>
-      </c>
-      <c r="T840" t="inlineStr"/>
+          <t>FA1B538F46714AD000</t>
+        </is>
+      </c>
+      <c r="T840" t="inlineStr">
+        <is>
+          <t>FA1B53909B0C4AD000</t>
+        </is>
+      </c>
       <c r="U840" t="inlineStr"/>
       <c r="V840" t="inlineStr"/>
-      <c r="W840" t="inlineStr"/>
+      <c r="W840" t="inlineStr">
+        <is>
+          <t>FA1B53909D23D7C000</t>
+        </is>
+      </c>
       <c r="X840" t="inlineStr">
         <is>
           <t>MA50_MA5</t>
@@ -80833,8 +80839,8 @@
       </c>
       <c r="Y840" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:1,  df['MACD'].iloc[-1]: -0.131, df['MACD'].iloc[-2]: -0.173,  df['MACD_hist'].iloc[-1]: 0.462, df['MACD_hist'].iloc[-2]: 0.448,  delta_MA50_M120.iloc[-1]: -1.656, delta_MA50_M120.iloc[-2]: -1.706,\ 
-  df['MA30_RSI10'].iloc[-1]: 43.920, df['MA30_RSI10'].iloc[-2]: 43.363  delta_MA50_MA120_1m.iloc[-1]: 0.170, delta_MA50_MA120_1m.iloc[-2]: 0.165  df_1m['MA30_RSI10'].iloc[-1]: 61.524, df_1m['MA30_RSI10'].iloc[-2]: 61.122  df_1m['MACD'].iloc[-1]: 0.065, df_1m['MACD'].iloc[-2]: 0.063  df_1m['MACD_hist'].iloc[-1]: 0.006, df_1m['MACD_hist'].iloc[-2]: 0.001  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.029 (more than 1.07 is good),  MACD_hist_max_amp: 0.457, MACD_hist_max_amp_1m: 0.041  </t>
+          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.137, df['MACD'].iloc[-2]: -0.152,  df['MACD_hist'].iloc[-1]: 0.048, df['MACD_hist'].iloc[-2]: 0.025,  delta_MA50_M120.iloc[-1]: -0.589, delta_MA50_M120.iloc[-2]: -0.640,\ 
+  df['MA30_RSI10'].iloc[-1]: 45.014, df['MA30_RSI10'].iloc[-2]: 44.970  delta_MA50_MA120_1m.iloc[-1]: 0.169, delta_MA50_MA120_1m.iloc[-2]: 0.163  df_1m['MA30_RSI10'].iloc[-1]: 60.226, df_1m['MA30_RSI10'].iloc[-2]: 59.701  df_1m['MACD'].iloc[-1]: 0.053, df_1m['MACD'].iloc[-2]: 0.053  df_1m['MACD_hist'].iloc[-1]: 0.006, df_1m['MACD_hist'].iloc[-2]: 0.006  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.912 (more than 1.07 is good),  MACD_hist_max_amp: 0.493, MACD_hist_max_amp_1m: 0.057  </t>
         </is>
       </c>
       <c r="Z840" t="inlineStr">
@@ -80842,48 +80848,54 @@
           <t>Сиднейское время (зима)</t>
         </is>
       </c>
-      <c r="AA840" t="inlineStr"/>
+      <c r="AA840" t="inlineStr">
+        <is>
+          <t>FA1B53909BB7D7C000</t>
+        </is>
+      </c>
     </row>
     <row r="841">
       <c r="A841" s="1" t="n">
         <v>839</v>
       </c>
       <c r="B841" t="n">
-        <v>4668</v>
+        <v>4671</v>
       </c>
       <c r="C841" t="inlineStr">
         <is>
-          <t>ASML</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="D841" s="2" t="n">
-        <v>45920.08635392361</v>
+        <v>45920.11251706019</v>
       </c>
       <c r="E841" t="n">
-        <v>932.39</v>
+        <v>477.11</v>
       </c>
       <c r="F841" t="n">
-        <v>1864.78</v>
+        <v>2385.55</v>
       </c>
       <c r="G841" t="n">
-        <v>1.111</v>
+        <v>1.01</v>
       </c>
       <c r="H841" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I841" t="inlineStr"/>
+        <v>45923.01961702546</v>
+      </c>
+      <c r="I841" t="n">
+        <v>477.7</v>
+      </c>
       <c r="J841" t="n">
-        <v>0</v>
+        <v>2388.5</v>
       </c>
       <c r="K841" t="n">
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="L841" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M841" t="inlineStr">
         <is>
-          <t>cancelled</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N841" t="n">
@@ -80896,20 +80908,28 @@
         <v>1.006</v>
       </c>
       <c r="Q841" t="n">
-        <v>0.45</v>
+        <v>0.05</v>
       </c>
       <c r="R841" t="n">
-        <v>0</v>
+        <v>0.9199999999998181</v>
       </c>
       <c r="S841" t="inlineStr">
         <is>
-          <t>FA1B538ACA240AD000</t>
-        </is>
-      </c>
-      <c r="T841" t="inlineStr"/>
+          <t>FA1B539369AB97C000</t>
+        </is>
+      </c>
+      <c r="T841" t="inlineStr">
+        <is>
+          <t>FA1B5393CDD217C000</t>
+        </is>
+      </c>
       <c r="U841" t="inlineStr"/>
       <c r="V841" t="inlineStr"/>
-      <c r="W841" t="inlineStr"/>
+      <c r="W841" t="inlineStr">
+        <is>
+          <t>FA1B5393CFDD0AD000</t>
+        </is>
+      </c>
       <c r="X841" t="inlineStr">
         <is>
           <t>MA50_MA5</t>
@@ -80917,8 +80937,8 @@
       </c>
       <c r="Y841" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:False, cond_b5:False  cond_RSI:0, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:1,  df['MACD'].iloc[-1]: 30.742, df['MACD'].iloc[-2]: 30.464,  df['MACD_hist'].iloc[-1]: 6.514, df['MACD_hist'].iloc[-2]: 6.960,  delta_MA50_M120.iloc[-1]: 6.844, delta_MA50_M120.iloc[-2]: 6.697,\ 
-  df['MA30_RSI10'].iloc[-1]: 80.614, df['MA30_RSI10'].iloc[-2]: 81.261  delta_MA50_MA120_1m.iloc[-1]: -0.041, delta_MA50_MA120_1m.iloc[-2]: -0.042  df_1m['MA30_RSI10'].iloc[-1]: 62.226, df_1m['MA30_RSI10'].iloc[-2]: 60.572  df_1m['MACD'].iloc[-1]: 0.607, df_1m['MACD'].iloc[-2]: 0.543  df_1m['MACD_hist'].iloc[-1]: 0.513, df_1m['MACD_hist'].iloc[-2]: 0.465  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 0.936 (more than 1.07 is good),  MACD_hist_max_amp: 9.659, MACD_hist_max_amp_1m: 0.716  </t>
+          <t xml:space="preserve">cond_b1:True, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 0.136, df['MACD'].iloc[-2]: 0.105,  df['MACD_hist'].iloc[-1]: 0.057, df['MACD_hist'].iloc[-2]: 0.004,  delta_MA50_M120.iloc[-1]: 0.191, delta_MA50_M120.iloc[-2]: 0.162,\ 
+  df['MA30_RSI10'].iloc[-1]: 44.005, df['MA30_RSI10'].iloc[-2]: 43.985  delta_MA50_MA120_1m.iloc[-1]: 0.051, delta_MA50_MA120_1m.iloc[-2]: 0.044  df_1m['MA30_RSI10'].iloc[-1]: 56.951, df_1m['MA30_RSI10'].iloc[-2]: 55.968  df_1m['MACD'].iloc[-1]: 0.199, df_1m['MACD'].iloc[-2]: 0.188  df_1m['MACD_hist'].iloc[-1]: 0.066, df_1m['MACD_hist'].iloc[-2]: 0.054  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 15.296 (more than 1.07 is good),  MACD_hist_max_amp: 2.510, MACD_hist_max_amp_1m: 0.132  </t>
         </is>
       </c>
       <c r="Z841" t="inlineStr">
@@ -80926,44 +80946,50 @@
           <t>Сиднейское время (зима)</t>
         </is>
       </c>
-      <c r="AA841" t="inlineStr"/>
+      <c r="AA841" t="inlineStr">
+        <is>
+          <t>FA1B5393CE7997C000</t>
+        </is>
+      </c>
     </row>
     <row r="842">
       <c r="A842" s="1" t="n">
         <v>840</v>
       </c>
       <c r="B842" t="n">
-        <v>4669</v>
+        <v>4672</v>
       </c>
       <c r="C842" t="inlineStr">
         <is>
-          <t>NEE</t>
+          <t>TMO</t>
         </is>
       </c>
       <c r="D842" s="2" t="n">
-        <v>45920.09996373842</v>
+        <v>45920.12814253472</v>
       </c>
       <c r="E842" t="n">
-        <v>70.92</v>
+        <v>481.93</v>
       </c>
       <c r="F842" t="n">
-        <v>2482.2</v>
-      </c>
-      <c r="G842" t="inlineStr"/>
+        <v>2409.65</v>
+      </c>
+      <c r="G842" t="n">
+        <v>1.01</v>
+      </c>
       <c r="H842" s="2" t="n">
-        <v>45920.15402466435</v>
+        <v>45920.19588012731</v>
       </c>
       <c r="I842" t="n">
-        <v>70.7303</v>
+        <v>480.435</v>
       </c>
       <c r="J842" t="n">
-        <v>2475.5605</v>
+        <v>2402.175</v>
       </c>
       <c r="K842" t="n">
-        <v>1.11</v>
+        <v>1.02</v>
       </c>
       <c r="L842" t="n">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="M842" t="inlineStr">
         <is>
@@ -80982,22 +81008,24 @@
       <c r="Q842" t="n">
         <v>0.05</v>
       </c>
-      <c r="R842" t="inlineStr"/>
+      <c r="R842" t="n">
+        <v>-9.504999999999908</v>
+      </c>
       <c r="S842" t="inlineStr">
         <is>
-          <t>FA1B538F46714AD000</t>
+          <t>FA1B5398900A57C000</t>
         </is>
       </c>
       <c r="T842" t="inlineStr">
         <is>
-          <t>FA1B53909B0C4AD000</t>
+          <t>FA1B5398E2050AD000</t>
         </is>
       </c>
       <c r="U842" t="inlineStr"/>
       <c r="V842" t="inlineStr"/>
       <c r="W842" t="inlineStr">
         <is>
-          <t>FA1B53909D23D7C000</t>
+          <t>FA1B5398E41497C000</t>
         </is>
       </c>
       <c r="X842" t="inlineStr">
@@ -81007,8 +81035,8 @@
       </c>
       <c r="Y842" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.137, df['MACD'].iloc[-2]: -0.152,  df['MACD_hist'].iloc[-1]: 0.048, df['MACD_hist'].iloc[-2]: 0.025,  delta_MA50_M120.iloc[-1]: -0.589, delta_MA50_M120.iloc[-2]: -0.640,\ 
-  df['MA30_RSI10'].iloc[-1]: 45.014, df['MA30_RSI10'].iloc[-2]: 44.970  delta_MA50_MA120_1m.iloc[-1]: 0.169, delta_MA50_MA120_1m.iloc[-2]: 0.163  df_1m['MA30_RSI10'].iloc[-1]: 60.226, df_1m['MA30_RSI10'].iloc[-2]: 59.701  df_1m['MACD'].iloc[-1]: 0.053, df_1m['MACD'].iloc[-2]: 0.053  df_1m['MACD_hist'].iloc[-1]: 0.006, df_1m['MACD_hist'].iloc[-2]: 0.006  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.912 (more than 1.07 is good),  MACD_hist_max_amp: 0.493, MACD_hist_max_amp_1m: 0.057  </t>
+          <t xml:space="preserve">cond_b1:True, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -1.004, df['MACD'].iloc[-2]: -1.149,  df['MACD_hist'].iloc[-1]: 1.212, df['MACD_hist'].iloc[-2]: 1.110,  delta_MA50_M120.iloc[-1]: -0.749, delta_MA50_M120.iloc[-2]: -0.756,\ 
+  df['MA30_RSI10'].iloc[-1]: 46.644, df['MA30_RSI10'].iloc[-2]: 45.815  delta_MA50_MA120_1m.iloc[-1]: 0.151, delta_MA50_MA120_1m.iloc[-2]: 0.143  df_1m['MA30_RSI10'].iloc[-1]: 51.542, df_1m['MA30_RSI10'].iloc[-2]: 51.309  df_1m['MACD'].iloc[-1]: 0.169, df_1m['MACD'].iloc[-2]: 0.162  df_1m['MACD_hist'].iloc[-1]: -0.038, df_1m['MACD_hist'].iloc[-2]: -0.058  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.092 (more than 1.07 is good),  MACD_hist_max_amp: 2.151, MACD_hist_max_amp_1m: 0.486  </t>
         </is>
       </c>
       <c r="Z842" t="inlineStr">
@@ -81018,7 +81046,7 @@
       </c>
       <c r="AA842" t="inlineStr">
         <is>
-          <t>FA1B53909BB7D7C000</t>
+          <t>FA1B5398E2B80AD000</t>
         </is>
       </c>
     </row>
@@ -81027,41 +81055,43 @@
         <v>841</v>
       </c>
       <c r="B843" t="n">
-        <v>4670</v>
+        <v>4675</v>
       </c>
       <c r="C843" t="inlineStr">
         <is>
-          <t>WFC</t>
+          <t>CME</t>
         </is>
       </c>
       <c r="D843" s="2" t="n">
-        <v>45920.10874604167</v>
+        <v>45920.16000833333</v>
       </c>
       <c r="E843" t="n">
-        <v>84.27</v>
+        <v>262.225</v>
       </c>
       <c r="F843" t="n">
-        <v>2443.83</v>
+        <v>2360.025</v>
       </c>
       <c r="G843" t="n">
-        <v>1.111</v>
+        <v>1.02</v>
       </c>
       <c r="H843" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I843" t="inlineStr"/>
+        <v>45920.26251295139</v>
+      </c>
+      <c r="I843" t="n">
+        <v>261.6732</v>
+      </c>
       <c r="J843" t="n">
-        <v>0</v>
+        <v>2355.0588</v>
       </c>
       <c r="K843" t="n">
-        <v>0</v>
+        <v>1.03</v>
       </c>
       <c r="L843" t="n">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="M843" t="inlineStr">
         <is>
-          <t>cancelled</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N843" t="n">
@@ -81074,20 +81104,28 @@
         <v>1.006</v>
       </c>
       <c r="Q843" t="n">
-        <v>0.45</v>
+        <v>0.05</v>
       </c>
       <c r="R843" t="n">
-        <v>0</v>
+        <v>-7.016199999999844</v>
       </c>
       <c r="S843" t="inlineStr">
         <is>
-          <t>FA1B53922B72D7C000</t>
-        </is>
-      </c>
-      <c r="T843" t="inlineStr"/>
+          <t>FA1B53A310B0CAD000</t>
+        </is>
+      </c>
+      <c r="T843" t="inlineStr">
+        <is>
+          <t>FA1B53A375474AD000</t>
+        </is>
+      </c>
       <c r="U843" t="inlineStr"/>
       <c r="V843" t="inlineStr"/>
-      <c r="W843" t="inlineStr"/>
+      <c r="W843" t="inlineStr">
+        <is>
+          <t>FA1B53A37761D7C000</t>
+        </is>
+      </c>
       <c r="X843" t="inlineStr">
         <is>
           <t>MA50_MA5</t>
@@ -81095,8 +81133,8 @@
       </c>
       <c r="Y843" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 0.670, df['MACD'].iloc[-2]: 0.623,  df['MACD_hist'].iloc[-1]: 0.425, df['MACD_hist'].iloc[-2]: 0.397,  delta_MA50_M120.iloc[-1]: 0.384, delta_MA50_M120.iloc[-2]: 0.325,\ 
-  df['MA30_RSI10'].iloc[-1]: 60.489, df['MA30_RSI10'].iloc[-2]: 59.761  delta_MA50_MA120_1m.iloc[-1]: 0.243, delta_MA50_MA120_1m.iloc[-2]: 0.240  df_1m['MA30_RSI10'].iloc[-1]: 60.786, df_1m['MA30_RSI10'].iloc[-2]: 60.393  df_1m['MACD'].iloc[-1]: 0.084, df_1m['MACD'].iloc[-2]: 0.083  df_1m['MACD_hist'].iloc[-1]: 0.013, df_1m['MACD_hist'].iloc[-2]: 0.013  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.072 (more than 1.07 is good),  MACD_hist_max_amp: 0.357, MACD_hist_max_amp_1m: 0.029  </t>
+          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.280, df['MACD'].iloc[-2]: -0.324,  df['MACD_hist'].iloc[-1]: 0.258, df['MACD_hist'].iloc[-2]: 0.209,  delta_MA50_M120.iloc[-1]: -0.929, delta_MA50_M120.iloc[-2]: -0.970,\ 
+  df['MA30_RSI10'].iloc[-1]: 48.994, df['MA30_RSI10'].iloc[-2]: 48.913  delta_MA50_MA120_1m.iloc[-1]: 0.095, delta_MA50_MA120_1m.iloc[-2]: 0.091  df_1m['MA30_RSI10'].iloc[-1]: 59.162, df_1m['MA30_RSI10'].iloc[-2]: 59.051  df_1m['MACD'].iloc[-1]: 0.150, df_1m['MACD'].iloc[-2]: 0.140  df_1m['MACD_hist'].iloc[-1]: 0.033, df_1m['MACD_hist'].iloc[-2]: 0.017  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.234 (more than 1.07 is good),  MACD_hist_max_amp: 0.742, MACD_hist_max_amp_1m: 0.098  </t>
         </is>
       </c>
       <c r="Z843" t="inlineStr">
@@ -81104,48 +81142,54 @@
           <t>Сиднейское время (зима)</t>
         </is>
       </c>
-      <c r="AA843" t="inlineStr"/>
+      <c r="AA843" t="inlineStr">
+        <is>
+          <t>FA1B53A376030AD000</t>
+        </is>
+      </c>
     </row>
     <row r="844">
       <c r="A844" s="1" t="n">
         <v>842</v>
       </c>
       <c r="B844" t="n">
-        <v>4671</v>
+        <v>4676</v>
       </c>
       <c r="C844" t="inlineStr">
         <is>
-          <t>LIN</t>
+          <t>ADM</t>
         </is>
       </c>
       <c r="D844" s="2" t="n">
-        <v>45920.11251706019</v>
+        <v>45920.1621208912</v>
       </c>
       <c r="E844" t="n">
-        <v>477.11</v>
+        <v>61.349</v>
       </c>
       <c r="F844" t="n">
-        <v>2385.55</v>
+        <v>2453.96</v>
       </c>
       <c r="G844" t="n">
-        <v>1.01</v>
+        <v>1.11</v>
       </c>
       <c r="H844" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I844" t="inlineStr"/>
+        <v>45923.01881101852</v>
+      </c>
+      <c r="I844" t="n">
+        <v>61.11</v>
+      </c>
       <c r="J844" t="n">
-        <v>0</v>
+        <v>2444.4</v>
       </c>
       <c r="K844" t="n">
-        <v>0</v>
+        <v>1.12</v>
       </c>
       <c r="L844" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="M844" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N844" t="n">
@@ -81161,23 +81205,23 @@
         <v>1.25</v>
       </c>
       <c r="R844" t="n">
-        <v>0</v>
+        <v>-11.78999999999994</v>
       </c>
       <c r="S844" t="inlineStr">
         <is>
-          <t>FA1B539369AB97C000</t>
+          <t>FA1B53A3C2EECAD000</t>
         </is>
       </c>
       <c r="T844" t="inlineStr">
         <is>
-          <t>FA1B5393CDD217C000</t>
+          <t>FA1B53A500E1D7C000</t>
         </is>
       </c>
       <c r="U844" t="inlineStr"/>
       <c r="V844" t="inlineStr"/>
       <c r="W844" t="inlineStr">
         <is>
-          <t>FA1B5393CFDD0AD000</t>
+          <t>FA1B53A503098AD000</t>
         </is>
       </c>
       <c r="X844" t="inlineStr">
@@ -81187,8 +81231,8 @@
       </c>
       <c r="Y844" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:True, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 0.136, df['MACD'].iloc[-2]: 0.105,  df['MACD_hist'].iloc[-1]: 0.057, df['MACD_hist'].iloc[-2]: 0.004,  delta_MA50_M120.iloc[-1]: 0.191, delta_MA50_M120.iloc[-2]: 0.162,\ 
-  df['MA30_RSI10'].iloc[-1]: 44.005, df['MA30_RSI10'].iloc[-2]: 43.985  delta_MA50_MA120_1m.iloc[-1]: 0.051, delta_MA50_MA120_1m.iloc[-2]: 0.044  df_1m['MA30_RSI10'].iloc[-1]: 56.951, df_1m['MA30_RSI10'].iloc[-2]: 55.968  df_1m['MACD'].iloc[-1]: 0.199, df_1m['MACD'].iloc[-2]: 0.188  df_1m['MACD_hist'].iloc[-1]: 0.066, df_1m['MACD_hist'].iloc[-2]: 0.054  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 15.296 (more than 1.07 is good),  MACD_hist_max_amp: 2.510, MACD_hist_max_amp_1m: 0.132  </t>
+          <t xml:space="preserve">cond_b1:True, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:False  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.118, df['MACD'].iloc[-2]: -0.131,  df['MACD_hist'].iloc[-1]: -0.009, df['MACD_hist'].iloc[-2]: -0.036,  delta_MA50_M120.iloc[-1]: -0.771, delta_MA50_M120.iloc[-2]: -0.814,\ 
+  df['MA30_RSI10'].iloc[-1]: 47.113, df['MA30_RSI10'].iloc[-2]: 46.524  delta_MA50_MA120_1m.iloc[-1]: 0.149, delta_MA50_MA120_1m.iloc[-2]: 0.142  df_1m['MA30_RSI10'].iloc[-1]: 63.496, df_1m['MA30_RSI10'].iloc[-2]: 62.859  df_1m['MACD'].iloc[-1]: 0.054, df_1m['MACD'].iloc[-2]: 0.053  df_1m['MACD_hist'].iloc[-1]: 0.010, df_1m['MACD_hist'].iloc[-2]: 0.010  cond_a1:0, cond_a2:1, cond_a3:0, cond_a4:0  MACD_hist_speed: 0.242 (more than 1.07 is good),  MACD_hist_max_amp: 0.262, MACD_hist_max_amp_1m: 0.039  </t>
         </is>
       </c>
       <c r="Z844" t="inlineStr">
@@ -81198,7 +81242,7 @@
       </c>
       <c r="AA844" t="inlineStr">
         <is>
-          <t>FA1B5393CE7997C000</t>
+          <t>FA1B53A5019F97C000</t>
         </is>
       </c>
     </row>
@@ -81207,33 +81251,33 @@
         <v>843</v>
       </c>
       <c r="B845" t="n">
-        <v>4672</v>
+        <v>4677</v>
       </c>
       <c r="C845" t="inlineStr">
         <is>
-          <t>TMO</t>
+          <t>CAT</t>
         </is>
       </c>
       <c r="D845" s="2" t="n">
-        <v>45920.12814253472</v>
+        <v>45920.22675645833</v>
       </c>
       <c r="E845" t="n">
-        <v>481.93</v>
+        <v>466.14</v>
       </c>
       <c r="F845" t="n">
-        <v>2409.65</v>
+        <v>2330.7</v>
       </c>
       <c r="G845" t="n">
         <v>1.01</v>
       </c>
       <c r="H845" s="2" t="n">
-        <v>45920.19588012731</v>
+        <v>45920.28659583334</v>
       </c>
       <c r="I845" t="n">
-        <v>480.435</v>
+        <v>466.28</v>
       </c>
       <c r="J845" t="n">
-        <v>2402.175</v>
+        <v>2331.4</v>
       </c>
       <c r="K845" t="n">
         <v>1.02</v>
@@ -81256,26 +81300,26 @@
         <v>1.006</v>
       </c>
       <c r="Q845" t="n">
-        <v>0.05</v>
+        <v>1.25</v>
       </c>
       <c r="R845" t="n">
-        <v>-9.504999999999908</v>
+        <v>-1.330000000000182</v>
       </c>
       <c r="S845" t="inlineStr">
         <is>
-          <t>FA1B5398900A57C000</t>
+          <t>FA1B53B9108A0AD000</t>
         </is>
       </c>
       <c r="T845" t="inlineStr">
         <is>
-          <t>FA1B5398E2050AD000</t>
+          <t>FA1B53BB40D90AD000</t>
         </is>
       </c>
       <c r="U845" t="inlineStr"/>
       <c r="V845" t="inlineStr"/>
       <c r="W845" t="inlineStr">
         <is>
-          <t>FA1B5398E41497C000</t>
+          <t>FA1B53BB42E50AD000</t>
         </is>
       </c>
       <c r="X845" t="inlineStr">
@@ -81285,8 +81329,8 @@
       </c>
       <c r="Y845" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:True, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -1.004, df['MACD'].iloc[-2]: -1.149,  df['MACD_hist'].iloc[-1]: 1.212, df['MACD_hist'].iloc[-2]: 1.110,  delta_MA50_M120.iloc[-1]: -0.749, delta_MA50_M120.iloc[-2]: -0.756,\ 
-  df['MA30_RSI10'].iloc[-1]: 46.644, df['MA30_RSI10'].iloc[-2]: 45.815  delta_MA50_MA120_1m.iloc[-1]: 0.151, delta_MA50_MA120_1m.iloc[-2]: 0.143  df_1m['MA30_RSI10'].iloc[-1]: 51.542, df_1m['MA30_RSI10'].iloc[-2]: 51.309  df_1m['MACD'].iloc[-1]: 0.169, df_1m['MACD'].iloc[-2]: 0.162  df_1m['MACD_hist'].iloc[-1]: -0.038, df_1m['MACD_hist'].iloc[-2]: -0.058  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.092 (more than 1.07 is good),  MACD_hist_max_amp: 2.151, MACD_hist_max_amp_1m: 0.486  </t>
+          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:False, cond_b5:False  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:1,  df['MACD'].iloc[-1]: 9.368, df['MACD'].iloc[-2]: 9.306,  df['MACD_hist'].iloc[-1]: 2.546, df['MACD_hist'].iloc[-2]: 2.814,  delta_MA50_M120.iloc[-1]: 2.949, delta_MA50_M120.iloc[-2]: 2.830,\ 
+  df['MA30_RSI10'].iloc[-1]: 77.810, df['MA30_RSI10'].iloc[-2]: 77.466  delta_MA50_MA120_1m.iloc[-1]: -0.016, delta_MA50_MA120_1m.iloc[-2]: -0.022  df_1m['MA30_RSI10'].iloc[-1]: 68.711, df_1m['MA30_RSI10'].iloc[-2]: 68.130  df_1m['MACD'].iloc[-1]: 0.276, df_1m['MACD'].iloc[-2]: 0.258  df_1m['MACD_hist'].iloc[-1]: 0.139, df_1m['MACD_hist'].iloc[-2]: 0.124  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 0.905 (more than 1.07 is good),  MACD_hist_max_amp: 4.329, MACD_hist_max_amp_1m: 0.298  </t>
         </is>
       </c>
       <c r="Z845" t="inlineStr">
@@ -81296,7 +81340,7 @@
       </c>
       <c r="AA845" t="inlineStr">
         <is>
-          <t>FA1B5398E2B80AD000</t>
+          <t>FA1B53BB418457C000</t>
         </is>
       </c>
     </row>
@@ -81305,41 +81349,41 @@
         <v>844</v>
       </c>
       <c r="B846" t="n">
-        <v>4673</v>
+        <v>4681</v>
       </c>
       <c r="C846" t="inlineStr">
         <is>
-          <t>MAR</t>
+          <t>HIG</t>
         </is>
       </c>
       <c r="D846" s="2" t="n">
-        <v>45920.13579047454</v>
+        <v>45923.05715646991</v>
       </c>
       <c r="E846" t="n">
-        <v>266.19</v>
+        <v>130.9714</v>
       </c>
       <c r="F846" t="n">
-        <v>2395.71</v>
-      </c>
-      <c r="G846" t="n">
-        <v>1.111</v>
-      </c>
+        <v>2488.4566</v>
+      </c>
+      <c r="G846" t="inlineStr"/>
       <c r="H846" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I846" t="inlineStr"/>
+        <v>45923.10328150463</v>
+      </c>
+      <c r="I846" t="n">
+        <v>130.65</v>
+      </c>
       <c r="J846" t="n">
-        <v>0</v>
+        <v>2482.35</v>
       </c>
       <c r="K846" t="n">
-        <v>0</v>
+        <v>1.06</v>
       </c>
       <c r="L846" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="M846" t="inlineStr">
         <is>
-          <t>cancelled</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N846" t="n">
@@ -81352,20 +81396,26 @@
         <v>1.006</v>
       </c>
       <c r="Q846" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="R846" t="n">
-        <v>0</v>
-      </c>
+        <v>0.05</v>
+      </c>
+      <c r="R846" t="inlineStr"/>
       <c r="S846" t="inlineStr">
         <is>
-          <t>FA1B539B154E4AD000</t>
-        </is>
-      </c>
-      <c r="T846" t="inlineStr"/>
+          <t>FA1B575DEF9117C000</t>
+        </is>
+      </c>
+      <c r="T846" t="inlineStr">
+        <is>
+          <t>FA1B575E36E357C000</t>
+        </is>
+      </c>
       <c r="U846" t="inlineStr"/>
       <c r="V846" t="inlineStr"/>
-      <c r="W846" t="inlineStr"/>
+      <c r="W846" t="inlineStr">
+        <is>
+          <t>FA1B575E390B0AD000</t>
+        </is>
+      </c>
       <c r="X846" t="inlineStr">
         <is>
           <t>MA50_MA5</t>
@@ -81373,8 +81423,8 @@
       </c>
       <c r="Y846" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:True, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:False  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.292, df['MACD'].iloc[-2]: -0.364,  df['MACD_hist'].iloc[-1]: 0.094, df['MACD_hist'].iloc[-2]: -0.036,  delta_MA50_M120.iloc[-1]: -0.286, delta_MA50_M120.iloc[-2]: -0.311,\ 
-  df['MA30_RSI10'].iloc[-1]: 47.815, df['MA30_RSI10'].iloc[-2]: 47.514  delta_MA50_MA120_1m.iloc[-1]: 0.129, delta_MA50_MA120_1m.iloc[-2]: 0.125  df_1m['MA30_RSI10'].iloc[-1]: 60.062, df_1m['MA30_RSI10'].iloc[-2]: 59.077  df_1m['MACD'].iloc[-1]: 0.168, df_1m['MACD'].iloc[-2]: 0.157  df_1m['MACD_hist'].iloc[-1]: 0.035, df_1m['MACD_hist'].iloc[-2]: 0.018  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: -2.563 (more than 1.07 is good),  MACD_hist_max_amp: 0.772, MACD_hist_max_amp_1m: 0.217  </t>
+          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:True, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.229, df['MACD'].iloc[-2]: -0.237,  df['MACD_hist'].iloc[-1]: 0.034, df['MACD_hist'].iloc[-2]: 0.023,  delta_MA50_M120.iloc[-1]: -0.304, delta_MA50_M120.iloc[-2]: -0.304,\ 
+  df['MA30_RSI10'].iloc[-1]: 43.132, df['MA30_RSI10'].iloc[-2]: 42.602  delta_MA50_MA120_1m.iloc[-1]: 0.019, delta_MA50_MA120_1m.iloc[-2]: 0.018  df_1m['MA30_RSI10'].iloc[-1]: 45.150, df_1m['MA30_RSI10'].iloc[-2]: 44.605  df_1m['MACD'].iloc[-1]: -0.020, df_1m['MACD'].iloc[-2]: -0.025  df_1m['MACD_hist'].iloc[-1]: 0.008, df_1m['MACD_hist'].iloc[-2]: -0.002  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.464 (more than 1.07 is good),  MACD_hist_max_amp: 0.515, MACD_hist_max_amp_1m: 0.047  </t>
         </is>
       </c>
       <c r="Z846" t="inlineStr">
@@ -81382,48 +81432,54 @@
           <t>Сиднейское время (зима)</t>
         </is>
       </c>
-      <c r="AA846" t="inlineStr"/>
+      <c r="AA846" t="inlineStr">
+        <is>
+          <t>FA1B575E37A0CAD000</t>
+        </is>
+      </c>
     </row>
     <row r="847">
       <c r="A847" s="1" t="n">
         <v>845</v>
       </c>
       <c r="B847" t="n">
-        <v>4674</v>
+        <v>4682</v>
       </c>
       <c r="C847" t="inlineStr">
         <is>
-          <t>CME</t>
+          <t>MCHP</t>
         </is>
       </c>
       <c r="D847" s="2" t="n">
-        <v>45920.14876416667</v>
+        <v>45923.07307094907</v>
       </c>
       <c r="E847" t="n">
-        <v>261.5</v>
+        <v>65.94</v>
       </c>
       <c r="F847" t="n">
-        <v>2353.5</v>
+        <v>2439.78</v>
       </c>
       <c r="G847" t="n">
-        <v>1.111</v>
+        <v>1.1</v>
       </c>
       <c r="H847" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I847" t="inlineStr"/>
+        <v>45923.15305194444</v>
+      </c>
+      <c r="I847" t="n">
+        <v>65.5615</v>
+      </c>
       <c r="J847" t="n">
-        <v>0</v>
+        <v>2425.7755</v>
       </c>
       <c r="K847" t="n">
-        <v>0</v>
+        <v>1.11</v>
       </c>
       <c r="L847" t="n">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="M847" t="inlineStr">
         <is>
-          <t>cancelled</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N847" t="n">
@@ -81436,20 +81492,28 @@
         <v>1.006</v>
       </c>
       <c r="Q847" t="n">
-        <v>0.45</v>
+        <v>0.05</v>
       </c>
       <c r="R847" t="n">
-        <v>0</v>
+        <v>-16.21450000000046</v>
       </c>
       <c r="S847" t="inlineStr">
         <is>
-          <t>FA1B539F5BF817C000</t>
-        </is>
-      </c>
-      <c r="T847" t="inlineStr"/>
+          <t>FA1B57632E610AD000</t>
+        </is>
+      </c>
+      <c r="T847" t="inlineStr">
+        <is>
+          <t>FA1B5763642CCAD000</t>
+        </is>
+      </c>
       <c r="U847" t="inlineStr"/>
       <c r="V847" t="inlineStr"/>
-      <c r="W847" t="inlineStr"/>
+      <c r="W847" t="inlineStr">
+        <is>
+          <t>FA1B5763664CCAD000</t>
+        </is>
+      </c>
       <c r="X847" t="inlineStr">
         <is>
           <t>MA50_MA5</t>
@@ -81457,8 +81521,8 @@
       </c>
       <c r="Y847" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.288, df['MACD'].iloc[-2]: -0.324,  df['MACD_hist'].iloc[-1]: 0.243, df['MACD_hist'].iloc[-2]: 0.209,  delta_MA50_M120.iloc[-1]: -0.930, delta_MA50_M120.iloc[-2]: -0.970,\ 
-  df['MA30_RSI10'].iloc[-1]: 48.942, df['MA30_RSI10'].iloc[-2]: 48.913  delta_MA50_MA120_1m.iloc[-1]: 0.048, delta_MA50_MA120_1m.iloc[-2]: 0.044  df_1m['MA30_RSI10'].iloc[-1]: 60.375, df_1m['MA30_RSI10'].iloc[-2]: 60.070  df_1m['MACD'].iloc[-1]: 0.143, df_1m['MACD'].iloc[-2]: 0.134  df_1m['MACD_hist'].iloc[-1]: 0.061, df_1m['MACD_hist'].iloc[-2]: 0.053  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.162 (more than 1.07 is good),  MACD_hist_max_amp: 0.742, MACD_hist_max_amp_1m: 0.098  </t>
+          <t xml:space="preserve">cond_b1:True, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 0.168, df['MACD'].iloc[-2]: 0.149,  df['MACD_hist'].iloc[-1]: -0.027, df['MACD_hist'].iloc[-2]: -0.068,  delta_MA50_M120.iloc[-1]: 0.161, delta_MA50_M120.iloc[-2]: 0.109,\ 
+  df['MA30_RSI10'].iloc[-1]: 55.611, df['MA30_RSI10'].iloc[-2]: 55.277  delta_MA50_MA120_1m.iloc[-1]: 0.164, delta_MA50_MA120_1m.iloc[-2]: 0.157  df_1m['MA30_RSI10'].iloc[-1]: 53.842, df_1m['MA30_RSI10'].iloc[-2]: 53.593  df_1m['MACD'].iloc[-1]: 0.052, df_1m['MACD'].iloc[-2]: 0.051  df_1m['MACD_hist'].iloc[-1]: -0.007, df_1m['MACD_hist'].iloc[-2]: -0.010  cond_a1:0, cond_a2:1, cond_a3:1, cond_a4:0  MACD_hist_speed: 0.402 (more than 1.07 is good),  MACD_hist_max_amp: 0.642, MACD_hist_max_amp_1m: 0.075  </t>
         </is>
       </c>
       <c r="Z847" t="inlineStr">
@@ -81466,46 +81530,50 @@
           <t>Сиднейское время (зима)</t>
         </is>
       </c>
-      <c r="AA847" t="inlineStr"/>
+      <c r="AA847" t="inlineStr">
+        <is>
+          <t>FA1B576364D757C000</t>
+        </is>
+      </c>
     </row>
     <row r="848">
       <c r="A848" s="1" t="n">
         <v>846</v>
       </c>
       <c r="B848" t="n">
-        <v>4675</v>
+        <v>4683</v>
       </c>
       <c r="C848" t="inlineStr">
         <is>
-          <t>CME</t>
+          <t>ADI</t>
         </is>
       </c>
       <c r="D848" s="2" t="n">
-        <v>45920.16000833333</v>
+        <v>45923.12699020834</v>
       </c>
       <c r="E848" t="n">
-        <v>262.225</v>
+        <v>247.6393</v>
       </c>
       <c r="F848" t="n">
-        <v>2360.025</v>
+        <v>2476.393</v>
       </c>
       <c r="G848" t="n">
         <v>1.02</v>
       </c>
       <c r="H848" s="2" t="n">
-        <v>45920.26251295139</v>
+        <v>45923.25844611111</v>
       </c>
       <c r="I848" t="n">
-        <v>261.6732</v>
+        <v>246.986</v>
       </c>
       <c r="J848" t="n">
-        <v>2355.0588</v>
+        <v>2469.86</v>
       </c>
       <c r="K848" t="n">
         <v>1.03</v>
       </c>
       <c r="L848" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M848" t="inlineStr">
         <is>
@@ -81525,23 +81593,23 @@
         <v>0.05</v>
       </c>
       <c r="R848" t="n">
-        <v>-7.016199999999844</v>
+        <v>-8.583000000000355</v>
       </c>
       <c r="S848" t="inlineStr">
         <is>
-          <t>FA1B53A310B0CAD000</t>
+          <t>FA1B5774F3CC57C000</t>
         </is>
       </c>
       <c r="T848" t="inlineStr">
         <is>
-          <t>FA1B53A375474AD000</t>
+          <t>FA1B5775307BD7C000</t>
         </is>
       </c>
       <c r="U848" t="inlineStr"/>
       <c r="V848" t="inlineStr"/>
       <c r="W848" t="inlineStr">
         <is>
-          <t>FA1B53A37761D7C000</t>
+          <t>FA1B5775328F4AD000</t>
         </is>
       </c>
       <c r="X848" t="inlineStr">
@@ -81551,8 +81619,8 @@
       </c>
       <c r="Y848" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.280, df['MACD'].iloc[-2]: -0.324,  df['MACD_hist'].iloc[-1]: 0.258, df['MACD_hist'].iloc[-2]: 0.209,  delta_MA50_M120.iloc[-1]: -0.929, delta_MA50_M120.iloc[-2]: -0.970,\ 
-  df['MA30_RSI10'].iloc[-1]: 48.994, df['MA30_RSI10'].iloc[-2]: 48.913  delta_MA50_MA120_1m.iloc[-1]: 0.095, delta_MA50_MA120_1m.iloc[-2]: 0.091  df_1m['MA30_RSI10'].iloc[-1]: 59.162, df_1m['MA30_RSI10'].iloc[-2]: 59.051  df_1m['MACD'].iloc[-1]: 0.150, df_1m['MACD'].iloc[-2]: 0.140  df_1m['MACD_hist'].iloc[-1]: 0.033, df_1m['MACD_hist'].iloc[-2]: 0.017  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.234 (more than 1.07 is good),  MACD_hist_max_amp: 0.742, MACD_hist_max_amp_1m: 0.098  </t>
+          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 0.090, df['MACD'].iloc[-2]: 0.060,  df['MACD_hist'].iloc[-1]: 0.116, df['MACD_hist'].iloc[-2]: 0.074,  delta_MA50_M120.iloc[-1]: -0.482, delta_MA50_M120.iloc[-2]: -0.507,\ 
+  df['MA30_RSI10'].iloc[-1]: 51.533, df['MA30_RSI10'].iloc[-2]: 50.622  delta_MA50_MA120_1m.iloc[-1]: -0.165, delta_MA50_MA120_1m.iloc[-2]: -0.167  df_1m['MA30_RSI10'].iloc[-1]: 48.445, df_1m['MA30_RSI10'].iloc[-2]: 47.887  df_1m['MACD'].iloc[-1]: -0.070, df_1m['MACD'].iloc[-2]: -0.079  df_1m['MACD_hist'].iloc[-1]: 0.053, df_1m['MACD_hist'].iloc[-2]: 0.043  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.578 (more than 1.07 is good),  MACD_hist_max_amp: 1.033, MACD_hist_max_amp_1m: 0.196  </t>
         </is>
       </c>
       <c r="Z848" t="inlineStr">
@@ -81562,7 +81630,7 @@
       </c>
       <c r="AA848" t="inlineStr">
         <is>
-          <t>FA1B53A376030AD000</t>
+          <t>FA1B5775312657C000</t>
         </is>
       </c>
     </row>
@@ -81571,41 +81639,43 @@
         <v>847</v>
       </c>
       <c r="B849" t="n">
-        <v>4676</v>
+        <v>4685</v>
       </c>
       <c r="C849" t="inlineStr">
         <is>
-          <t>ADM</t>
+          <t>MCHP</t>
         </is>
       </c>
       <c r="D849" s="2" t="n">
-        <v>45920.1621208912</v>
+        <v>45923.15721479167</v>
       </c>
       <c r="E849" t="n">
-        <v>61.349</v>
+        <v>65.56999999999999</v>
       </c>
       <c r="F849" t="n">
-        <v>2453.96</v>
+        <v>2491.66</v>
       </c>
       <c r="G849" t="n">
-        <v>1.11</v>
+        <v>1.1</v>
       </c>
       <c r="H849" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I849" t="inlineStr"/>
+        <v>45923.22298072917</v>
+      </c>
+      <c r="I849" t="n">
+        <v>65.4619</v>
+      </c>
       <c r="J849" t="n">
-        <v>0</v>
+        <v>2487.5522</v>
       </c>
       <c r="K849" t="n">
-        <v>0</v>
+        <v>1.101</v>
       </c>
       <c r="L849" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M849" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N849" t="n">
@@ -81618,26 +81688,26 @@
         <v>1.006</v>
       </c>
       <c r="Q849" t="n">
-        <v>1.25</v>
+        <v>0.05</v>
       </c>
       <c r="R849" t="n">
-        <v>0</v>
+        <v>-6.30879999999977</v>
       </c>
       <c r="S849" t="inlineStr">
         <is>
-          <t>FA1B53A3C2EECAD000</t>
+          <t>FA1B577EE9FD8AD000</t>
         </is>
       </c>
       <c r="T849" t="inlineStr">
         <is>
-          <t>FA1B53A500E1D7C000</t>
+          <t>FA1B577F304B0AD000</t>
         </is>
       </c>
       <c r="U849" t="inlineStr"/>
       <c r="V849" t="inlineStr"/>
       <c r="W849" t="inlineStr">
         <is>
-          <t>FA1B53A503098AD000</t>
+          <t>FA1B577F32644AD000</t>
         </is>
       </c>
       <c r="X849" t="inlineStr">
@@ -81647,8 +81717,8 @@
       </c>
       <c r="Y849" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:True, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:False  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.118, df['MACD'].iloc[-2]: -0.131,  df['MACD_hist'].iloc[-1]: -0.009, df['MACD_hist'].iloc[-2]: -0.036,  delta_MA50_M120.iloc[-1]: -0.771, delta_MA50_M120.iloc[-2]: -0.814,\ 
-  df['MA30_RSI10'].iloc[-1]: 47.113, df['MA30_RSI10'].iloc[-2]: 46.524  delta_MA50_MA120_1m.iloc[-1]: 0.149, delta_MA50_MA120_1m.iloc[-2]: 0.142  df_1m['MA30_RSI10'].iloc[-1]: 63.496, df_1m['MA30_RSI10'].iloc[-2]: 62.859  df_1m['MACD'].iloc[-1]: 0.054, df_1m['MACD'].iloc[-2]: 0.053  df_1m['MACD_hist'].iloc[-1]: 0.010, df_1m['MACD_hist'].iloc[-2]: 0.010  cond_a1:0, cond_a2:1, cond_a3:0, cond_a4:0  MACD_hist_speed: 0.242 (more than 1.07 is good),  MACD_hist_max_amp: 0.262, MACD_hist_max_amp_1m: 0.039  </t>
+          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:True, cond_b4:False, cond_b5:False  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 0.161, df['MACD'].iloc[-2]: 0.159,  df['MACD_hist'].iloc[-1]: -0.029, df['MACD_hist'].iloc[-2]: -0.036,  delta_MA50_M120.iloc[-1]: 0.260, delta_MA50_M120.iloc[-2]: 0.215,\ 
+  df['MA30_RSI10'].iloc[-1]: 56.334, df['MA30_RSI10'].iloc[-2]: 56.021  delta_MA50_MA120_1m.iloc[-1]: -0.196, delta_MA50_MA120_1m.iloc[-2]: -0.200  df_1m['MA30_RSI10'].iloc[-1]: 53.379, df_1m['MA30_RSI10'].iloc[-2]: 52.835  df_1m['MACD'].iloc[-1]: -0.008, df_1m['MACD'].iloc[-2]: -0.010  df_1m['MACD_hist'].iloc[-1]: 0.019, df_1m['MACD_hist'].iloc[-2]: 0.018  cond_a1:0, cond_a2:1, cond_a3:0, cond_a4:0  MACD_hist_speed: 0.791 (more than 1.07 is good),  MACD_hist_max_amp: 0.642, MACD_hist_max_amp_1m: 0.048  </t>
         </is>
       </c>
       <c r="Z849" t="inlineStr">
@@ -81658,7 +81728,7 @@
       </c>
       <c r="AA849" t="inlineStr">
         <is>
-          <t>FA1B53A5019F97C000</t>
+          <t>FA1B577F30F8D7C000</t>
         </is>
       </c>
     </row>
@@ -81667,39 +81737,39 @@
         <v>848</v>
       </c>
       <c r="B850" t="n">
-        <v>4677</v>
+        <v>4686</v>
       </c>
       <c r="C850" t="inlineStr">
         <is>
-          <t>CAT</t>
+          <t>RMD</t>
         </is>
       </c>
       <c r="D850" s="2" t="n">
-        <v>45920.22675645833</v>
+        <v>45923.18131232639</v>
       </c>
       <c r="E850" t="n">
-        <v>466.14</v>
+        <v>274.31</v>
       </c>
       <c r="F850" t="n">
-        <v>2330.7</v>
+        <v>2468.79</v>
       </c>
       <c r="G850" t="n">
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
       <c r="H850" s="2" t="n">
-        <v>45920.28659583334</v>
+        <v>45924.02071753472</v>
       </c>
       <c r="I850" t="n">
-        <v>466.28</v>
+        <v>274.73</v>
       </c>
       <c r="J850" t="n">
-        <v>2331.4</v>
+        <v>2472.57</v>
       </c>
       <c r="K850" t="n">
-        <v>1.02</v>
+        <v>1.101</v>
       </c>
       <c r="L850" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="M850" t="inlineStr">
         <is>
@@ -81716,57 +81786,1550 @@
         <v>1.006</v>
       </c>
       <c r="Q850" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R850" t="n">
+        <v>1.6590000000002</v>
+      </c>
+      <c r="S850" t="inlineStr">
+        <is>
+          <t>FA1B5786DB3757C000</t>
+        </is>
+      </c>
+      <c r="T850" t="inlineStr">
+        <is>
+          <t>FA1B57870A35CAD000</t>
+        </is>
+      </c>
+      <c r="U850" t="inlineStr"/>
+      <c r="V850" t="inlineStr"/>
+      <c r="W850" t="inlineStr">
+        <is>
+          <t>FA1B57870C350AD000</t>
+        </is>
+      </c>
+      <c r="X850" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y850" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.046, df['MACD'].iloc[-2]: -0.101,  df['MACD_hist'].iloc[-1]: 0.367, df['MACD_hist'].iloc[-2]: 0.314,  delta_MA50_M120.iloc[-1]: -0.378, delta_MA50_M120.iloc[-2]: -0.401,\ 
+  df['MA30_RSI10'].iloc[-1]: 52.732, df['MA30_RSI10'].iloc[-2]: 52.142  delta_MA50_MA120_1m.iloc[-1]: 0.145, delta_MA50_MA120_1m.iloc[-2]: 0.142  df_1m['MA30_RSI10'].iloc[-1]: 52.340, df_1m['MA30_RSI10'].iloc[-2]: 52.018  df_1m['MACD'].iloc[-1]: 0.091, df_1m['MACD'].iloc[-2]: 0.078  df_1m['MACD_hist'].iloc[-1]: -0.017, df_1m['MACD_hist'].iloc[-2]: -0.045  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:1  MACD_hist_speed: 1.170 (more than 1.07 is good),  MACD_hist_max_amp: 0.603, MACD_hist_max_amp_1m: 0.118  </t>
+        </is>
+      </c>
+      <c r="Z850" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA850" t="inlineStr">
+        <is>
+          <t>FA1B57870AE017C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" s="1" t="n">
+        <v>849</v>
+      </c>
+      <c r="B851" t="n">
+        <v>4711</v>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>SO</t>
+        </is>
+      </c>
+      <c r="D851" s="2" t="n">
+        <v>45926.98900717593</v>
+      </c>
+      <c r="E851" t="n">
+        <v>92.4288</v>
+      </c>
+      <c r="F851" t="n">
+        <v>2495.5776</v>
+      </c>
+      <c r="G851" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="H851" s="2" t="n">
+        <v>45927.14355092592</v>
+      </c>
+      <c r="I851" t="n">
+        <v>94.38</v>
+      </c>
+      <c r="J851" t="n">
+        <v>2548.26</v>
+      </c>
+      <c r="K851" t="n">
+        <v>1.101</v>
+      </c>
+      <c r="L851" t="n">
+        <v>27</v>
+      </c>
+      <c r="M851" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N851" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O851" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P851" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q851" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R851" t="n">
+        <v>50.51139999999969</v>
+      </c>
+      <c r="S851" t="inlineStr">
+        <is>
+          <t>FA1B578DC7478AD000</t>
+        </is>
+      </c>
+      <c r="T851" t="inlineStr">
+        <is>
+          <t>FA1B5C6E53648AD000</t>
+        </is>
+      </c>
+      <c r="U851" t="inlineStr"/>
+      <c r="V851" t="inlineStr"/>
+      <c r="W851" t="inlineStr">
+        <is>
+          <t>FA1B5C6E559A8AD000</t>
+        </is>
+      </c>
+      <c r="X851" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y851" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z851" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA851" t="inlineStr">
+        <is>
+          <t>FA1B5C6E541FCAD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" s="1" t="n">
+        <v>850</v>
+      </c>
+      <c r="B852" t="n">
+        <v>4688</v>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>TEL</t>
+        </is>
+      </c>
+      <c r="D852" s="2" t="n">
+        <v>45923.24157341435</v>
+      </c>
+      <c r="E852" t="n">
+        <v>218.4626</v>
+      </c>
+      <c r="F852" t="n">
+        <v>2403.0886</v>
+      </c>
+      <c r="G852" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="H852" s="2" t="n">
+        <v>45924.186171875</v>
+      </c>
+      <c r="I852" t="n">
+        <v>218.7201</v>
+      </c>
+      <c r="J852" t="n">
+        <v>2405.9211</v>
+      </c>
+      <c r="K852" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="L852" t="n">
+        <v>11</v>
+      </c>
+      <c r="M852" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N852" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O852" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P852" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q852" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R852" t="n">
+        <v>0.7824999999999818</v>
+      </c>
+      <c r="S852" t="inlineStr">
+        <is>
+          <t>FA1B579AB7BB4AD000</t>
+        </is>
+      </c>
+      <c r="T852" t="inlineStr">
+        <is>
+          <t>FA1B579AE0954AD000</t>
+        </is>
+      </c>
+      <c r="U852" t="inlineStr"/>
+      <c r="V852" t="inlineStr"/>
+      <c r="W852" t="inlineStr">
+        <is>
+          <t>FA1B579AE2B34AD000</t>
+        </is>
+      </c>
+      <c r="X852" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y852" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 1.711, df['MACD'].iloc[-2]: 1.685,  df['MACD_hist'].iloc[-1]: 0.142, df['MACD_hist'].iloc[-2]: 0.113,  delta_MA50_M120.iloc[-1]: 1.728, delta_MA50_M120.iloc[-2]: 1.726,\ 
+  df['MA30_RSI10'].iloc[-1]: 63.862, df['MA30_RSI10'].iloc[-2]: 63.668  delta_MA50_MA120_1m.iloc[-1]: 0.073, delta_MA50_MA120_1m.iloc[-2]: 0.068  df_1m['MA30_RSI10'].iloc[-1]: 62.761, df_1m['MA30_RSI10'].iloc[-2]: 62.300  df_1m['MACD'].iloc[-1]: 0.124, df_1m['MACD'].iloc[-2]: 0.119  df_1m['MACD_hist'].iloc[-1]: 0.029, df_1m['MACD_hist'].iloc[-2]: 0.024  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:1  MACD_hist_speed: 1.251 (more than 1.07 is good),  MACD_hist_max_amp: 0.892, MACD_hist_max_amp_1m: 0.064  </t>
+        </is>
+      </c>
+      <c r="Z852" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA852" t="inlineStr">
+        <is>
+          <t>FA1B579AE152CAD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" s="1" t="n">
+        <v>851</v>
+      </c>
+      <c r="B853" t="n">
+        <v>4689</v>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>MMC</t>
+        </is>
+      </c>
+      <c r="D853" s="2" t="n">
+        <v>45923.9824696875</v>
+      </c>
+      <c r="E853" t="n">
+        <v>197.39</v>
+      </c>
+      <c r="F853" t="n">
+        <v>2368.68</v>
+      </c>
+      <c r="G853" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="H853" s="2" t="n">
+        <v>45924.06039420139</v>
+      </c>
+      <c r="I853" t="n">
+        <v>196.49</v>
+      </c>
+      <c r="J853" t="n">
+        <v>2357.88</v>
+      </c>
+      <c r="K853" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="L853" t="n">
+        <v>12</v>
+      </c>
+      <c r="M853" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N853" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O853" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P853" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q853" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R853" t="n">
+        <v>-12.86999999999973</v>
+      </c>
+      <c r="S853" t="inlineStr">
+        <is>
+          <t>FA1B588EE8DA4AD000</t>
+        </is>
+      </c>
+      <c r="T853" t="inlineStr">
+        <is>
+          <t>FA1B588F22388AD000</t>
+        </is>
+      </c>
+      <c r="U853" t="inlineStr"/>
+      <c r="V853" t="inlineStr"/>
+      <c r="W853" t="inlineStr">
+        <is>
+          <t>FA1B588F2462CAD000</t>
+        </is>
+      </c>
+      <c r="X853" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y853" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:True, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:False, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.928, df['MACD'].iloc[-2]: -0.967,  df['MACD_hist'].iloc[-1]: 0.349, df['MACD_hist'].iloc[-2]: 0.325,  delta_MA50_M120.iloc[-1]: -1.599, delta_MA50_M120.iloc[-2]: -1.576,\ 
+  df['MA30_RSI10'].iloc[-1]: 44.688, df['MA30_RSI10'].iloc[-2]: 43.917  delta_MA50_MA120_1m.iloc[-1]: 0.100, delta_MA50_MA120_1m.iloc[-2]: 0.096  df_1m['MA30_RSI10'].iloc[-1]: 51.085, df_1m['MA30_RSI10'].iloc[-2]: 51.019  df_1m['MACD'].iloc[-1]: 0.038, df_1m['MACD'].iloc[-2]: 0.035  df_1m['MACD_hist'].iloc[-1]: -0.035, df_1m['MACD_hist'].iloc[-2]: -0.046  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:1  MACD_hist_speed: 1.076 (more than 1.07 is good),  MACD_hist_max_amp: 0.874, MACD_hist_max_amp_1m: 0.100  
+  </t>
+        </is>
+      </c>
+      <c r="Z853" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA853" t="inlineStr">
+        <is>
+          <t>FA1B588F22E5D7C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" s="1" t="n">
+        <v>852</v>
+      </c>
+      <c r="B854" t="n">
+        <v>4693</v>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>AEP</t>
+        </is>
+      </c>
+      <c r="D854" s="2" t="n">
+        <v>45924.06971196759</v>
+      </c>
+      <c r="E854" t="n">
+        <v>107.246547</v>
+      </c>
+      <c r="F854" t="n">
+        <v>2466.670581</v>
+      </c>
+      <c r="G854" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="H854" s="2" t="n">
+        <v>45925.27009060185</v>
+      </c>
+      <c r="I854" t="n">
+        <v>108.9301</v>
+      </c>
+      <c r="J854" t="n">
+        <v>2505.3923</v>
+      </c>
+      <c r="K854" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="L854" t="n">
+        <v>23</v>
+      </c>
+      <c r="M854" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N854" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O854" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P854" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q854" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R854" t="n">
+        <v>36.59171900000012</v>
+      </c>
+      <c r="S854" t="inlineStr">
+        <is>
+          <t>FA1B58ABA9E60AD000</t>
+        </is>
+      </c>
+      <c r="T854" t="inlineStr">
+        <is>
+          <t>FA1B58ABDCA117C000</t>
+        </is>
+      </c>
+      <c r="U854" t="inlineStr"/>
+      <c r="V854" t="inlineStr"/>
+      <c r="W854" t="inlineStr">
+        <is>
+          <t>FA1B58ABDEC98AD000</t>
+        </is>
+      </c>
+      <c r="X854" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y854" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:True, cond_b2:False, cond_b3:False, cond_b4:True, cond_b5:True, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.378, df['MACD'].iloc[-2]: -0.402,  df['MACD_hist'].iloc[-1]: 0.123, df['MACD_hist'].iloc[-2]: 0.094,  delta_MA50_M120.iloc[-1]: -0.808, delta_MA50_M120.iloc[-2]: -0.814,\ 
+  df['MA30_RSI10'].iloc[-1]: 41.990, df['MA30_RSI10'].iloc[-2]: 41.184  delta_MA50_MA120_1m.iloc[-1]: 0.045, delta_MA50_MA120_1m.iloc[-2]: 0.040  df_1m['MA30_RSI10'].iloc[-1]: 48.698, df_1m['MA30_RSI10'].iloc[-2]: 48.434  df_1m['MACD'].iloc[-1]: 0.022, df_1m['MACD'].iloc[-2]: 0.017  df_1m['MACD_hist'].iloc[-1]: 0.023, df_1m['MACD_hist'].iloc[-2]: 0.018  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.302 (more than 1.07 is good),  MACD_hist_max_amp: 0.444, MACD_hist_max_amp_1m: 0.058  
+  </t>
+        </is>
+      </c>
+      <c r="Z854" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA854" t="inlineStr">
+        <is>
+          <t>FA1B58ABDD624AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" s="1" t="n">
+        <v>853</v>
+      </c>
+      <c r="B855" t="n">
+        <v>4702</v>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>HII</t>
+        </is>
+      </c>
+      <c r="D855" s="2" t="n">
+        <v>45925.04084181713</v>
+      </c>
+      <c r="E855" t="n">
+        <v>280.18</v>
+      </c>
+      <c r="F855" t="n">
+        <v>2241.44</v>
+      </c>
+      <c r="G855" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H855" s="2" t="n">
+        <v>45925.11625666667</v>
+      </c>
+      <c r="I855" t="n">
+        <v>277.55</v>
+      </c>
+      <c r="J855" t="n">
+        <v>2220.4</v>
+      </c>
+      <c r="K855" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L855" t="n">
+        <v>8</v>
+      </c>
+      <c r="M855" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N855" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O855" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P855" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q855" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R855" t="n">
+        <v>-23.06999999999996</v>
+      </c>
+      <c r="S855" t="inlineStr">
+        <is>
+          <t>FA1B59EBBD048AD000</t>
+        </is>
+      </c>
+      <c r="T855" t="inlineStr">
+        <is>
+          <t>FA1B59EC3EB297C000</t>
+        </is>
+      </c>
+      <c r="U855" t="inlineStr"/>
+      <c r="V855" t="inlineStr"/>
+      <c r="W855" t="inlineStr">
+        <is>
+          <t>FA1B59EC4093D7C000</t>
+        </is>
+      </c>
+      <c r="X855" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y855" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:True, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:False, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 1.199, df['MACD'].iloc[-2]: 1.063,  df['MACD_hist'].iloc[-1]: 0.587, df['MACD_hist'].iloc[-2]: 0.406,  delta_MA50_M120.iloc[-1]: 0.892, delta_MA50_M120.iloc[-2]: 0.887,\ 
+  df['MA30_RSI10'].iloc[-1]: 55.132, df['MA30_RSI10'].iloc[-2]: 54.273  delta_MA50_MA120_1m.iloc[-1]: 0.357, delta_MA50_MA120_1m.iloc[-2]: 0.343  df_1m['MA30_RSI10'].iloc[-1]: 65.255, df_1m['MA30_RSI10'].iloc[-2]: 64.901  df_1m['MACD'].iloc[-1]: 0.964, df_1m['MACD'].iloc[-2]: 0.960  df_1m['MACD_hist'].iloc[-1]: 0.286, df_1m['MACD_hist'].iloc[-2]: 0.323  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.448 (more than 1.07 is good),  MACD_hist_max_amp: 0.745, MACD_hist_max_amp_1m: 0.460  
+  </t>
+        </is>
+      </c>
+      <c r="Z855" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA855" t="inlineStr">
+        <is>
+          <t>FA1B59EC3F5E57C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" s="1" t="n">
+        <v>854</v>
+      </c>
+      <c r="B856" t="n">
+        <v>4703</v>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>KHC</t>
+        </is>
+      </c>
+      <c r="D856" s="2" t="n">
+        <v>45925.07772570602</v>
+      </c>
+      <c r="E856" t="n">
+        <v>26.7797</v>
+      </c>
+      <c r="F856" t="n">
+        <v>2490.5121</v>
+      </c>
+      <c r="G856" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="H856" s="2" t="n">
+        <v>45925.22933460648</v>
+      </c>
+      <c r="I856" t="n">
+        <v>26.7118</v>
+      </c>
+      <c r="J856" t="n">
+        <v>2484.1974</v>
+      </c>
+      <c r="K856" t="n">
+        <v>1.101</v>
+      </c>
+      <c r="L856" t="n">
+        <v>93</v>
+      </c>
+      <c r="M856" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N856" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O856" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P856" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q856" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R856" t="n">
+        <v>-8.685699999999901</v>
+      </c>
+      <c r="S856" t="inlineStr">
+        <is>
+          <t>FA1B59F7E5174AD000</t>
+        </is>
+      </c>
+      <c r="T856" t="inlineStr">
+        <is>
+          <t>FA1B59F88A31CAD000</t>
+        </is>
+      </c>
+      <c r="U856" t="inlineStr"/>
+      <c r="V856" t="inlineStr"/>
+      <c r="W856" t="inlineStr">
+        <is>
+          <t>FA1B59F88C49D7C000</t>
+        </is>
+      </c>
+      <c r="X856" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y856" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:False, cond_b5:False, cond_b6: False  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 0.075, df['MACD'].iloc[-2]: 0.064,  df['MACD_hist'].iloc[-1]: 0.097, df['MACD_hist'].iloc[-2]: 0.089,  delta_MA50_M120.iloc[-1]: -1.120, delta_MA50_M120.iloc[-2]: -1.206,\ 
+  df['MA30_RSI10'].iloc[-1]: 60.902, df['MA30_RSI10'].iloc[-2]: 60.432  delta_MA50_MA120_1m.iloc[-1]: -0.004, delta_MA50_MA120_1m.iloc[-2]: -0.011  df_1m['MA30_RSI10'].iloc[-1]: 74.106, df_1m['MA30_RSI10'].iloc[-2]: 73.430  df_1m['MACD'].iloc[-1]: 0.037, df_1m['MACD'].iloc[-2]: 0.036  df_1m['MACD_hist'].iloc[-1]: 0.024, df_1m['MACD_hist'].iloc[-2]: 0.026  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:1  MACD_hist_speed: 1.081 (more than 1.07 is good),  MACD_hist_max_amp: 0.145, MACD_hist_max_amp_1m: 0.029  
+  </t>
+        </is>
+      </c>
+      <c r="Z856" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA856" t="inlineStr">
+        <is>
+          <t>FA1B59F88AE097C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" s="1" t="n">
+        <v>855</v>
+      </c>
+      <c r="B857" t="n">
+        <v>4708</v>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>AJG</t>
+        </is>
+      </c>
+      <c r="D857" s="2" t="n">
+        <v>45925.98572012731</v>
+      </c>
+      <c r="E857" t="n">
+        <v>305.81</v>
+      </c>
+      <c r="F857" t="n">
+        <v>2446.48</v>
+      </c>
+      <c r="G857" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H857" s="2" t="n">
+        <v>45926.04974020833</v>
+      </c>
+      <c r="I857" t="n">
+        <v>304.54</v>
+      </c>
+      <c r="J857" t="n">
+        <v>2436.32</v>
+      </c>
+      <c r="K857" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L857" t="n">
+        <v>8</v>
+      </c>
+      <c r="M857" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N857" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O857" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P857" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q857" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R857" t="n">
+        <v>-12.18999999999985</v>
+      </c>
+      <c r="S857" t="inlineStr">
+        <is>
+          <t>FA1B5B232916D7C000</t>
+        </is>
+      </c>
+      <c r="T857" t="inlineStr">
+        <is>
+          <t>FA1B5B24543E97C000</t>
+        </is>
+      </c>
+      <c r="U857" t="inlineStr"/>
+      <c r="V857" t="inlineStr"/>
+      <c r="W857" t="inlineStr">
+        <is>
+          <t>FA1B5B24566F0AD001</t>
+        </is>
+      </c>
+      <c r="X857" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y857" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:True, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 2.186, df['MACD'].iloc[-2]: 2.092,  df['MACD_hist'].iloc[-1]: 1.049, df['MACD_hist'].iloc[-2]: 1.022,  delta_MA50_M120.iloc[-1]: -0.134, delta_MA50_M120.iloc[-2]: -0.238,\ 
+  df['MA30_RSI10'].iloc[-1]: 66.715, df['MA30_RSI10'].iloc[-2]: 66.071  delta_MA50_MA120_1m.iloc[-1]: 0.048, delta_MA50_MA120_1m.iloc[-2]: 0.038  df_1m['MA30_RSI10'].iloc[-1]: 55.752, df_1m['MA30_RSI10'].iloc[-2]: 55.174  df_1m['MACD'].iloc[-1]: 0.355, df_1m['MACD'].iloc[-2]: 0.314  df_1m['MACD_hist'].iloc[-1]: 0.353, df_1m['MACD_hist'].iloc[-2]: 0.326  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.027 (more than 1.07 is good),  MACD_hist_max_amp: 1.584, MACD_hist_max_amp_1m: 0.282  
+  </t>
+        </is>
+      </c>
+      <c r="Z857" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA857" t="inlineStr">
+        <is>
+          <t>FA1B5B2454EA57C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" s="1" t="n">
+        <v>856</v>
+      </c>
+      <c r="B858" t="n">
+        <v>4709</v>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>STZ</t>
+        </is>
+      </c>
+      <c r="D858" s="2" t="n">
+        <v>45926.11206836806</v>
+      </c>
+      <c r="E858" t="n">
+        <v>133.22</v>
+      </c>
+      <c r="F858" t="n">
+        <v>2397.96</v>
+      </c>
+      <c r="G858" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="H858" s="2" t="n">
+        <v>45926.15684761574</v>
+      </c>
+      <c r="I858" t="n">
+        <v>133.05</v>
+      </c>
+      <c r="J858" t="n">
+        <v>2394.9</v>
+      </c>
+      <c r="K858" t="n">
+        <v>1.101</v>
+      </c>
+      <c r="L858" t="n">
+        <v>18</v>
+      </c>
+      <c r="M858" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N858" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O858" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P858" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q858" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R858" t="n">
+        <v>-5.200999999999945</v>
+      </c>
+      <c r="S858" t="inlineStr">
+        <is>
+          <t>FA1B5B4CCDBC17C000</t>
+        </is>
+      </c>
+      <c r="T858" t="inlineStr">
+        <is>
+          <t>FA1B5B4E360257C000</t>
+        </is>
+      </c>
+      <c r="U858" t="inlineStr"/>
+      <c r="V858" t="inlineStr"/>
+      <c r="W858" t="inlineStr">
+        <is>
+          <t>FA1B5B4E3812D7C000</t>
+        </is>
+      </c>
+      <c r="X858" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y858" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:True, cond_b2:True, cond_b3:False, cond_b4:False, cond_b5:True, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -1.194, df['MACD'].iloc[-2]: -1.262,  df['MACD_hist'].iloc[-1]: 0.729, df['MACD_hist'].iloc[-2]: 0.705,  delta_MA50_M120.iloc[-1]: -4.479, delta_MA50_M120.iloc[-2]: -4.571,\ 
+  df['MA30_RSI10'].iloc[-1]: 47.273, df['MA30_RSI10'].iloc[-2]: 46.281  delta_MA50_MA120_1m.iloc[-1]: 0.020, delta_MA50_MA120_1m.iloc[-2]: 0.014  df_1m['MA30_RSI10'].iloc[-1]: 59.422, df_1m['MA30_RSI10'].iloc[-2]: 59.143  df_1m['MACD'].iloc[-1]: 0.111, df_1m['MACD'].iloc[-2]: 0.101  df_1m['MACD_hist'].iloc[-1]: 0.117, df_1m['MACD_hist'].iloc[-2]: 0.115  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.035 (more than 1.07 is good),  MACD_hist_max_amp: 1.023, MACD_hist_max_amp_1m: 0.123  
+  </t>
+        </is>
+      </c>
+      <c r="Z858" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA858" t="inlineStr">
+        <is>
+          <t>FA1B5B4E36AE8AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" s="1" t="n">
+        <v>857</v>
+      </c>
+      <c r="B859" t="n">
+        <v>4715</v>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>CVX</t>
+        </is>
+      </c>
+      <c r="D859" s="2" t="n">
+        <v>45927.02695020833</v>
+      </c>
+      <c r="E859" t="n">
+        <v>160.9791</v>
+      </c>
+      <c r="F859" t="n">
+        <v>2414.6865</v>
+      </c>
+      <c r="G859" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="H859" s="2" t="n">
+        <v>45927.06464710648</v>
+      </c>
+      <c r="I859" t="n">
+        <v>160.4392</v>
+      </c>
+      <c r="J859" t="n">
+        <v>2406.588</v>
+      </c>
+      <c r="K859" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="L859" t="n">
+        <v>15</v>
+      </c>
+      <c r="M859" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N859" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O859" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P859" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q859" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R859" t="n">
+        <v>-10.1884999999996</v>
+      </c>
+      <c r="S859" t="inlineStr">
+        <is>
+          <t>FA1B5C768B830AD000</t>
+        </is>
+      </c>
+      <c r="T859" t="inlineStr"/>
+      <c r="U859" t="inlineStr"/>
+      <c r="V859" t="inlineStr"/>
+      <c r="W859" t="inlineStr"/>
+      <c r="X859" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y859" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z859" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA859" t="inlineStr"/>
+    </row>
+    <row r="860">
+      <c r="A860" s="1" t="n">
+        <v>858</v>
+      </c>
+      <c r="B860" t="n">
+        <v>4717</v>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="D860" s="2" t="n">
+        <v>45927.07422052083</v>
+      </c>
+      <c r="E860" t="n">
+        <v>409.51</v>
+      </c>
+      <c r="F860" t="n">
+        <v>2457.06</v>
+      </c>
+      <c r="G860" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H860" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I860" t="inlineStr"/>
+      <c r="J860" t="n">
+        <v>0</v>
+      </c>
+      <c r="K860" t="n">
+        <v>0</v>
+      </c>
+      <c r="L860" t="n">
+        <v>6</v>
+      </c>
+      <c r="M860" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N860" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O860" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P860" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q860" t="n">
         <v>1.25</v>
       </c>
-      <c r="R850" t="n">
-        <v>-1.330000000000182</v>
-      </c>
-      <c r="S850" t="inlineStr">
-        <is>
-          <t>FA1B53B9108A0AD000</t>
-        </is>
-      </c>
-      <c r="T850" t="inlineStr">
-        <is>
-          <t>FA1B53BB40D90AD000</t>
-        </is>
-      </c>
-      <c r="U850" t="inlineStr">
+      <c r="R860" t="n">
+        <v>0</v>
+      </c>
+      <c r="S860" t="inlineStr">
+        <is>
+          <t>FA1B5C898C300AD000</t>
+        </is>
+      </c>
+      <c r="T860" t="inlineStr">
+        <is>
+          <t>FA1B5C8AECCC57C000</t>
+        </is>
+      </c>
+      <c r="U860" t="inlineStr"/>
+      <c r="V860" t="inlineStr"/>
+      <c r="W860" t="inlineStr">
+        <is>
+          <t>FA1B5C8AEEFF57C000</t>
+        </is>
+      </c>
+      <c r="X860" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y860" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z860" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA860" t="inlineStr">
+        <is>
+          <t>FA1B5C8AED7B17C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" s="1" t="n">
+        <v>859</v>
+      </c>
+      <c r="B861" t="n">
+        <v>4718</v>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>SPG</t>
+        </is>
+      </c>
+      <c r="D861" s="2" t="n">
+        <v>45927.09922373843</v>
+      </c>
+      <c r="E861" t="n">
+        <v>184.5</v>
+      </c>
+      <c r="F861" t="n">
+        <v>2398.5</v>
+      </c>
+      <c r="G861" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="H861" s="2" t="n">
+        <v>45927.26870071759</v>
+      </c>
+      <c r="I861" t="n">
+        <v>184.5585</v>
+      </c>
+      <c r="J861" t="n">
+        <v>2399.2605</v>
+      </c>
+      <c r="K861" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="L861" t="n">
+        <v>13</v>
+      </c>
+      <c r="M861" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N861" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O861" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P861" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q861" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R861" t="n">
+        <v>-1.30949999999968</v>
+      </c>
+      <c r="S861" t="inlineStr">
+        <is>
+          <t>FA1B5C9228F40AD000</t>
+        </is>
+      </c>
+      <c r="T861" t="inlineStr">
+        <is>
+          <t>FA1B5C928A0C8AD000</t>
+        </is>
+      </c>
+      <c r="U861" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="V850" t="inlineStr">
+      <c r="V861" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="W850" t="inlineStr">
-        <is>
-          <t>FA1B53BB42E50AD000</t>
-        </is>
-      </c>
-      <c r="X850" t="inlineStr">
+      <c r="W861" t="inlineStr">
+        <is>
+          <t>FA1B5C928C2A8AD000</t>
+        </is>
+      </c>
+      <c r="X861" t="inlineStr">
         <is>
           <t>MA50_MA5</t>
         </is>
       </c>
-      <c r="Y850" t="inlineStr">
-        <is>
-          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:False, cond_b5:False  cond_RSI:1, cond_grad_MACD:1,  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:1,  df['MACD'].iloc[-1]: 9.368, df['MACD'].iloc[-2]: 9.306,  df['MACD_hist'].iloc[-1]: 2.546, df['MACD_hist'].iloc[-2]: 2.814,  delta_MA50_M120.iloc[-1]: 2.949, delta_MA50_M120.iloc[-2]: 2.830,\ 
-  df['MA30_RSI10'].iloc[-1]: 77.810, df['MA30_RSI10'].iloc[-2]: 77.466  delta_MA50_MA120_1m.iloc[-1]: -0.016, delta_MA50_MA120_1m.iloc[-2]: -0.022  df_1m['MA30_RSI10'].iloc[-1]: 68.711, df_1m['MA30_RSI10'].iloc[-2]: 68.130  df_1m['MACD'].iloc[-1]: 0.276, df_1m['MACD'].iloc[-2]: 0.258  df_1m['MACD_hist'].iloc[-1]: 0.139, df_1m['MACD_hist'].iloc[-2]: 0.124  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 0.905 (more than 1.07 is good),  MACD_hist_max_amp: 4.329, MACD_hist_max_amp_1m: 0.298  </t>
-        </is>
-      </c>
-      <c r="Z850" t="inlineStr">
+      <c r="Y861" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:True, cond_b2:True, cond_b3:False, cond_b4:True, cond_b5:True, cond_b6: False  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 0.535, df['MACD'].iloc[-2]: 0.499,  df['MACD_hist'].iloc[-1]: 0.198, df['MACD_hist'].iloc[-2]: 0.157,  delta_MA50_M120.iloc[-1]: 0.262, delta_MA50_M120.iloc[-2]: 0.259,\ 
+  df['MA30_RSI10'].iloc[-1]: 56.296, df['MA30_RSI10'].iloc[-2]: 55.398  delta_MA50_MA120_1m.iloc[-1]: 0.001, delta_MA50_MA120_1m.iloc[-2]: -0.005  df_1m['MA30_RSI10'].iloc[-1]: 48.385, df_1m['MA30_RSI10'].iloc[-2]: 47.836  df_1m['MACD'].iloc[-1]: 0.015, df_1m['MACD'].iloc[-2]: 0.007  df_1m['MACD_hist'].iloc[-1]: 0.023, df_1m['MACD_hist'].iloc[-2]: 0.010  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:1  MACD_hist_speed: 1.263 (more than 1.07 is good),  MACD_hist_max_amp: 0.711, MACD_hist_max_amp_1m: 0.120  
+  </t>
+        </is>
+      </c>
+      <c r="Z861" t="inlineStr">
         <is>
           <t>Сиднейское время (зима)</t>
         </is>
       </c>
-      <c r="AA850" t="inlineStr">
-        <is>
-          <t>FA1B53BB418457C000</t>
-        </is>
-      </c>
+      <c r="AA861" t="inlineStr">
+        <is>
+          <t>FA1B5C928ACB97C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" s="1" t="n">
+        <v>860</v>
+      </c>
+      <c r="B862" t="n">
+        <v>4719</v>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>CAG</t>
+        </is>
+      </c>
+      <c r="D862" s="2" t="n">
+        <v>45927.10685473379</v>
+      </c>
+      <c r="E862" t="n">
+        <v>18.22</v>
+      </c>
+      <c r="F862" t="n">
+        <v>2496.14</v>
+      </c>
+      <c r="G862" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H862" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I862" t="inlineStr"/>
+      <c r="J862" t="n">
+        <v>0</v>
+      </c>
+      <c r="K862" t="n">
+        <v>0</v>
+      </c>
+      <c r="L862" t="n">
+        <v>137</v>
+      </c>
+      <c r="M862" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N862" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O862" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P862" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q862" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="R862" t="n">
+        <v>0</v>
+      </c>
+      <c r="S862" t="inlineStr">
+        <is>
+          <t>FA1B5C94ACDCD7C000</t>
+        </is>
+      </c>
+      <c r="T862" t="inlineStr"/>
+      <c r="U862" t="inlineStr"/>
+      <c r="V862" t="inlineStr"/>
+      <c r="W862" t="inlineStr"/>
+      <c r="X862" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y862" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:False, cond_b5:True, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.150, df['MACD'].iloc[-2]: -0.154,  df['MACD_hist'].iloc[-1]: 0.018, df['MACD_hist'].iloc[-2]: 0.013,  delta_MA50_M120.iloc[-1]: -2.294, delta_MA50_M120.iloc[-2]: -2.229,\ 
+  df['MA30_RSI10'].iloc[-1]: 38.240, df['MA30_RSI10'].iloc[-2]: 37.385  delta_MA50_MA120_1m.iloc[-1]: -0.064, delta_MA50_MA120_1m.iloc[-2]: -0.071  df_1m['MA30_RSI10'].iloc[-1]: 57.370, df_1m['MA30_RSI10'].iloc[-2]: 56.745  df_1m['MACD'].iloc[-1]: 0.005, df_1m['MACD'].iloc[-2]: 0.004  df_1m['MACD_hist'].iloc[-1]: 0.003, df_1m['MACD_hist'].iloc[-2]: 0.002  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.359 (more than 1.07 is good),  MACD_hist_max_amp: 0.075, MACD_hist_max_amp_1m: 0.010  
+  </t>
+        </is>
+      </c>
+      <c r="Z862" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA862" t="inlineStr"/>
+    </row>
+    <row r="863">
+      <c r="A863" s="1" t="n">
+        <v>861</v>
+      </c>
+      <c r="B863" t="n">
+        <v>4720</v>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>PNC</t>
+        </is>
+      </c>
+      <c r="D863" s="2" t="n">
+        <v>45927.10707041666</v>
+      </c>
+      <c r="E863" t="n">
+        <v>203.13</v>
+      </c>
+      <c r="F863" t="n">
+        <v>2437.56</v>
+      </c>
+      <c r="G863" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H863" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I863" t="inlineStr"/>
+      <c r="J863" t="n">
+        <v>0</v>
+      </c>
+      <c r="K863" t="n">
+        <v>0</v>
+      </c>
+      <c r="L863" t="n">
+        <v>12</v>
+      </c>
+      <c r="M863" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N863" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O863" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P863" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q863" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="R863" t="n">
+        <v>0</v>
+      </c>
+      <c r="S863" t="inlineStr">
+        <is>
+          <t>FA1B5C94BF088AD000</t>
+        </is>
+      </c>
+      <c r="T863" t="inlineStr"/>
+      <c r="U863" t="inlineStr"/>
+      <c r="V863" t="inlineStr"/>
+      <c r="W863" t="inlineStr"/>
+      <c r="X863" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y863" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:True, cond_b2:True, cond_b3:False, cond_b4:True, cond_b5:True, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.091, df['MACD'].iloc[-2]: -0.105,  df['MACD_hist'].iloc[-1]: -0.199, df['MACD_hist'].iloc[-2]: -0.257,  delta_MA50_M120.iloc[-1]: 0.366, delta_MA50_M120.iloc[-2]: 0.363,\ 
+  df['MA30_RSI10'].iloc[-1]: 46.340, df['MA30_RSI10'].iloc[-2]: 46.139  delta_MA50_MA120_1m.iloc[-1]: 0.059, delta_MA50_MA120_1m.iloc[-2]: 0.053  df_1m['MA30_RSI10'].iloc[-1]: 44.932, df_1m['MA30_RSI10'].iloc[-2]: 44.165  df_1m['MACD'].iloc[-1]: 0.041, df_1m['MACD'].iloc[-2]: 0.028  df_1m['MACD_hist'].iloc[-1]: 0.095, df_1m['MACD_hist'].iloc[-2]: 0.084  cond_a1:0, cond_a2:1, cond_a3:1, cond_a4:0  MACD_hist_speed: 0.775 (more than 1.07 is good),  MACD_hist_max_amp: 0.765, MACD_hist_max_amp_1m: 0.211  
+  </t>
+        </is>
+      </c>
+      <c r="Z863" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA863" t="inlineStr"/>
+    </row>
+    <row r="864">
+      <c r="A864" s="1" t="n">
+        <v>862</v>
+      </c>
+      <c r="B864" t="n">
+        <v>4721</v>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>PLD</t>
+        </is>
+      </c>
+      <c r="D864" s="2" t="n">
+        <v>45927.1139700463</v>
+      </c>
+      <c r="E864" t="n">
+        <v>113.64</v>
+      </c>
+      <c r="F864" t="n">
+        <v>2500.08</v>
+      </c>
+      <c r="G864" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H864" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I864" t="inlineStr"/>
+      <c r="J864" t="n">
+        <v>0</v>
+      </c>
+      <c r="K864" t="n">
+        <v>0</v>
+      </c>
+      <c r="L864" t="n">
+        <v>22</v>
+      </c>
+      <c r="M864" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N864" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O864" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P864" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q864" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="R864" t="n">
+        <v>0</v>
+      </c>
+      <c r="S864" t="inlineStr">
+        <is>
+          <t>FA1B5C97052B97C000</t>
+        </is>
+      </c>
+      <c r="T864" t="inlineStr"/>
+      <c r="U864" t="inlineStr"/>
+      <c r="V864" t="inlineStr"/>
+      <c r="W864" t="inlineStr"/>
+      <c r="X864" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y864" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True, cond_b6: False  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.124, df['MACD'].iloc[-2]: -0.150,  df['MACD_hist'].iloc[-1]: 0.029, df['MACD_hist'].iloc[-2]: -0.017,  delta_MA50_M120.iloc[-1]: 0.367, delta_MA50_M120.iloc[-2]: 0.404,\ 
+  df['MA30_RSI10'].iloc[-1]: 47.035, df['MA30_RSI10'].iloc[-2]: 46.496  delta_MA50_MA120_1m.iloc[-1]: 0.156, delta_MA50_MA120_1m.iloc[-2]: 0.155  df_1m['MA30_RSI10'].iloc[-1]: 60.995, df_1m['MA30_RSI10'].iloc[-2]: 59.902  df_1m['MACD'].iloc[-1]: 0.107, df_1m['MACD'].iloc[-2]: 0.103  df_1m['MACD_hist'].iloc[-1]: 0.063, df_1m['MACD_hist'].iloc[-2]: 0.064  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: -1.696 (more than 1.07 is good),  MACD_hist_max_amp: 0.413, MACD_hist_max_amp_1m: 0.075  
+  </t>
+        </is>
+      </c>
+      <c r="Z864" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA864" t="inlineStr"/>
+    </row>
+    <row r="865">
+      <c r="A865" s="1" t="n">
+        <v>863</v>
+      </c>
+      <c r="B865" t="n">
+        <v>4722</v>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>MASI</t>
+        </is>
+      </c>
+      <c r="D865" s="2" t="n">
+        <v>45927.21069133102</v>
+      </c>
+      <c r="E865" t="n">
+        <v>141.68</v>
+      </c>
+      <c r="F865" t="n">
+        <v>2408.56</v>
+      </c>
+      <c r="G865" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H865" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I865" t="inlineStr"/>
+      <c r="J865" t="n">
+        <v>0</v>
+      </c>
+      <c r="K865" t="n">
+        <v>0</v>
+      </c>
+      <c r="L865" t="n">
+        <v>17</v>
+      </c>
+      <c r="M865" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N865" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O865" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P865" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q865" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="R865" t="n">
+        <v>0</v>
+      </c>
+      <c r="S865" t="inlineStr">
+        <is>
+          <t>FA1B5CB6E6038AD000</t>
+        </is>
+      </c>
+      <c r="T865" t="inlineStr"/>
+      <c r="U865" t="inlineStr"/>
+      <c r="V865" t="inlineStr"/>
+      <c r="W865" t="inlineStr"/>
+      <c r="X865" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y865" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:False, cond_b5:False, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.587, df['MACD'].iloc[-2]: -0.670,  df['MACD_hist'].iloc[-1]: 0.477, df['MACD_hist'].iloc[-2]: 0.384,  delta_MA50_M120.iloc[-1]: -1.769, delta_MA50_M120.iloc[-2]: -1.724,\ 
+  df['MA30_RSI10'].iloc[-1]: 47.501, df['MA30_RSI10'].iloc[-2]: 47.182  delta_MA50_MA120_1m.iloc[-1]: -0.148, delta_MA50_MA120_1m.iloc[-2]: -0.154  df_1m['MA30_RSI10'].iloc[-1]: 62.047, df_1m['MA30_RSI10'].iloc[-2]: 60.936  df_1m['MACD'].iloc[-1]: 0.089, df_1m['MACD'].iloc[-2]: 0.078  df_1m['MACD_hist'].iloc[-1]: 0.099, df_1m['MACD_hist'].iloc[-2]: 0.092  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.241 (more than 1.07 is good),  MACD_hist_max_amp: 0.882, MACD_hist_max_amp_1m: 0.117  
+  </t>
+        </is>
+      </c>
+      <c r="Z865" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA865" t="inlineStr"/>
+    </row>
+    <row r="866">
+      <c r="A866" s="1" t="n">
+        <v>864</v>
+      </c>
+      <c r="B866" t="n">
+        <v>4723</v>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>MASI</t>
+        </is>
+      </c>
+      <c r="D866" s="2" t="n">
+        <v>45927.21739049769</v>
+      </c>
+      <c r="E866" t="n">
+        <v>141.76</v>
+      </c>
+      <c r="F866" t="n">
+        <v>2409.92</v>
+      </c>
+      <c r="G866" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H866" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I866" t="inlineStr"/>
+      <c r="J866" t="n">
+        <v>0</v>
+      </c>
+      <c r="K866" t="n">
+        <v>0</v>
+      </c>
+      <c r="L866" t="n">
+        <v>17</v>
+      </c>
+      <c r="M866" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N866" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O866" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P866" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q866" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="R866" t="n">
+        <v>0</v>
+      </c>
+      <c r="S866" t="inlineStr">
+        <is>
+          <t>FA1B5CB91B4357C000</t>
+        </is>
+      </c>
+      <c r="T866" t="inlineStr"/>
+      <c r="U866" t="inlineStr"/>
+      <c r="V866" t="inlineStr"/>
+      <c r="W866" t="inlineStr"/>
+      <c r="X866" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y866" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:False, cond_b5:False, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.575, df['MACD'].iloc[-2]: -0.670,  df['MACD_hist'].iloc[-1]: 0.498, df['MACD_hist'].iloc[-2]: 0.384,  delta_MA50_M120.iloc[-1]: -1.767, delta_MA50_M120.iloc[-2]: -1.724,\ 
+  df['MA30_RSI10'].iloc[-1]: 47.561, df['MA30_RSI10'].iloc[-2]: 47.182  delta_MA50_MA120_1m.iloc[-1]: -0.098, delta_MA50_MA120_1m.iloc[-2]: -0.108  df_1m['MA30_RSI10'].iloc[-1]: 65.985, df_1m['MA30_RSI10'].iloc[-2]: 65.716  df_1m['MACD'].iloc[-1]: 0.160, df_1m['MACD'].iloc[-2]: 0.147  df_1m['MACD_hist'].iloc[-1]: 0.131, df_1m['MACD_hist'].iloc[-2]: 0.125  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.295 (more than 1.07 is good),  MACD_hist_max_amp: 0.882, MACD_hist_max_amp_1m: 0.126  
+  </t>
+        </is>
+      </c>
+      <c r="Z866" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA866" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
before added prediction to stock_buy_condition_MA50_MA5
</commit_message>
<xml_diff>
--- a/db/real_trade_db.xlsx
+++ b/db/real_trade_db.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA866"/>
+  <dimension ref="A1:AA881"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -82729,21 +82729,23 @@
         <v>1.01</v>
       </c>
       <c r="H860" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I860" t="inlineStr"/>
+        <v>45930.02419341435</v>
+      </c>
+      <c r="I860" t="n">
+        <v>408.665</v>
+      </c>
       <c r="J860" t="n">
-        <v>0</v>
+        <v>2451.99</v>
       </c>
       <c r="K860" t="n">
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="L860" t="n">
         <v>6</v>
       </c>
       <c r="M860" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N860" t="n">
@@ -82756,10 +82758,10 @@
         <v>1.006</v>
       </c>
       <c r="Q860" t="n">
-        <v>1.25</v>
+        <v>0.05</v>
       </c>
       <c r="R860" t="n">
-        <v>0</v>
+        <v>-7.099999999999708</v>
       </c>
       <c r="S860" t="inlineStr">
         <is>
@@ -82868,16 +82870,8 @@
           <t>FA1B5C928A0C8AD000</t>
         </is>
       </c>
-      <c r="U861" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="V861" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="U861" t="inlineStr"/>
+      <c r="V861" t="inlineStr"/>
       <c r="W861" t="inlineStr">
         <is>
           <t>FA1B5C928C2A8AD000</t>
@@ -82911,41 +82905,43 @@
         <v>860</v>
       </c>
       <c r="B862" t="n">
-        <v>4719</v>
+        <v>4765</v>
       </c>
       <c r="C862" t="inlineStr">
         <is>
-          <t>CAG</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D862" s="2" t="n">
-        <v>45927.10685473379</v>
+        <v>45929.63889190972</v>
       </c>
       <c r="E862" t="n">
-        <v>18.22</v>
+        <v>164.315</v>
       </c>
       <c r="F862" t="n">
-        <v>2496.14</v>
+        <v>2464.725</v>
       </c>
       <c r="G862" t="n">
-        <v>1.111</v>
+        <v>1.04</v>
       </c>
       <c r="H862" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I862" t="inlineStr"/>
+        <v>45930.02262574074</v>
+      </c>
+      <c r="I862" t="n">
+        <v>163.95</v>
+      </c>
       <c r="J862" t="n">
-        <v>0</v>
+        <v>2459.25</v>
       </c>
       <c r="K862" t="n">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="L862" t="n">
-        <v>137</v>
+        <v>15</v>
       </c>
       <c r="M862" t="inlineStr">
         <is>
-          <t>cancelled</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N862" t="n">
@@ -82961,76 +82957,84 @@
         <v>0.45</v>
       </c>
       <c r="R862" t="n">
-        <v>0</v>
+        <v>-7.564999999999909</v>
       </c>
       <c r="S862" t="inlineStr">
         <is>
-          <t>FA1B5C94ACDCD7C000</t>
-        </is>
-      </c>
-      <c r="T862" t="inlineStr"/>
+          <t>FA1B5FD7357A8AD000</t>
+        </is>
+      </c>
+      <c r="T862" t="inlineStr">
+        <is>
+          <t>FA1B6048090757C000</t>
+        </is>
+      </c>
       <c r="U862" t="inlineStr"/>
       <c r="V862" t="inlineStr"/>
-      <c r="W862" t="inlineStr"/>
+      <c r="W862" t="inlineStr">
+        <is>
+          <t>FA1B60480B2D4AD000</t>
+        </is>
+      </c>
       <c r="X862" t="inlineStr">
         <is>
-          <t>MA50_MA5</t>
-        </is>
-      </c>
-      <c r="Y862" t="inlineStr">
-        <is>
-          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:False, cond_b5:True, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.150, df['MACD'].iloc[-2]: -0.154,  df['MACD_hist'].iloc[-1]: 0.018, df['MACD_hist'].iloc[-2]: 0.013,  delta_MA50_M120.iloc[-1]: -2.294, delta_MA50_M120.iloc[-2]: -2.229,\ 
-  df['MA30_RSI10'].iloc[-1]: 38.240, df['MA30_RSI10'].iloc[-2]: 37.385  delta_MA50_MA120_1m.iloc[-1]: -0.064, delta_MA50_MA120_1m.iloc[-2]: -0.071  df_1m['MA30_RSI10'].iloc[-1]: 57.370, df_1m['MA30_RSI10'].iloc[-2]: 56.745  df_1m['MACD'].iloc[-1]: 0.005, df_1m['MACD'].iloc[-2]: 0.004  df_1m['MACD_hist'].iloc[-1]: 0.003, df_1m['MACD_hist'].iloc[-2]: 0.002  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.359 (more than 1.07 is good),  MACD_hist_max_amp: 0.075, MACD_hist_max_amp_1m: 0.010  
-  </t>
-        </is>
-      </c>
+          <t>before_market_open_1</t>
+        </is>
+      </c>
+      <c r="Y862" t="inlineStr"/>
       <c r="Z862" t="inlineStr">
         <is>
           <t>Сиднейское время (зима)</t>
         </is>
       </c>
-      <c r="AA862" t="inlineStr"/>
+      <c r="AA862" t="inlineStr">
+        <is>
+          <t>FA1B604809C957C000</t>
+        </is>
+      </c>
     </row>
     <row r="863">
       <c r="A863" s="1" t="n">
         <v>861</v>
       </c>
       <c r="B863" t="n">
-        <v>4720</v>
+        <v>4778</v>
       </c>
       <c r="C863" t="inlineStr">
         <is>
-          <t>PNC</t>
+          <t>SPG</t>
         </is>
       </c>
       <c r="D863" s="2" t="n">
-        <v>45927.10707041666</v>
+        <v>45929.98490122685</v>
       </c>
       <c r="E863" t="n">
-        <v>203.13</v>
+        <v>184.83</v>
       </c>
       <c r="F863" t="n">
-        <v>2437.56</v>
+        <v>2402.79</v>
       </c>
       <c r="G863" t="n">
-        <v>1.111</v>
+        <v>0</v>
       </c>
       <c r="H863" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I863" t="inlineStr"/>
+        <v>45930.18602527778</v>
+      </c>
+      <c r="I863" t="n">
+        <v>185.58</v>
+      </c>
       <c r="J863" t="n">
-        <v>0</v>
+        <v>2412.54</v>
       </c>
       <c r="K863" t="n">
-        <v>0</v>
+        <v>1.04</v>
       </c>
       <c r="L863" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M863" t="inlineStr">
         <is>
-          <t>cancelled</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N863" t="n">
@@ -83043,20 +83047,28 @@
         <v>1.006</v>
       </c>
       <c r="Q863" t="n">
-        <v>0.45</v>
+        <v>0.05</v>
       </c>
       <c r="R863" t="n">
-        <v>0</v>
+        <v>8.710000000000001</v>
       </c>
       <c r="S863" t="inlineStr">
         <is>
-          <t>FA1B5C94BF088AD000</t>
-        </is>
-      </c>
-      <c r="T863" t="inlineStr"/>
+          <t>FA1B5FD7421597C000</t>
+        </is>
+      </c>
+      <c r="T863" t="inlineStr">
+        <is>
+          <t>FA1B60495B34CAD000</t>
+        </is>
+      </c>
       <c r="U863" t="inlineStr"/>
       <c r="V863" t="inlineStr"/>
-      <c r="W863" t="inlineStr"/>
+      <c r="W863" t="inlineStr">
+        <is>
+          <t>FA1B60495D5097C000</t>
+        </is>
+      </c>
       <c r="X863" t="inlineStr">
         <is>
           <t>MA50_MA5</t>
@@ -83064,9 +83076,7 @@
       </c>
       <c r="Y863" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:True, cond_b2:True, cond_b3:False, cond_b4:True, cond_b5:True, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.091, df['MACD'].iloc[-2]: -0.105,  df['MACD_hist'].iloc[-1]: -0.199, df['MACD_hist'].iloc[-2]: -0.257,  delta_MA50_M120.iloc[-1]: 0.366, delta_MA50_M120.iloc[-2]: 0.363,\ 
-  df['MA30_RSI10'].iloc[-1]: 46.340, df['MA30_RSI10'].iloc[-2]: 46.139  delta_MA50_MA120_1m.iloc[-1]: 0.059, delta_MA50_MA120_1m.iloc[-2]: 0.053  df_1m['MA30_RSI10'].iloc[-1]: 44.932, df_1m['MA30_RSI10'].iloc[-2]: 44.165  df_1m['MACD'].iloc[-1]: 0.041, df_1m['MACD'].iloc[-2]: 0.028  df_1m['MACD_hist'].iloc[-1]: 0.095, df_1m['MACD_hist'].iloc[-2]: 0.084  cond_a1:0, cond_a2:1, cond_a3:1, cond_a4:0  MACD_hist_speed: 0.775 (more than 1.07 is good),  MACD_hist_max_amp: 0.765, MACD_hist_max_amp_1m: 0.211  
-  </t>
+          <t>{}</t>
         </is>
       </c>
       <c r="Z863" t="inlineStr">
@@ -83074,48 +83084,54 @@
           <t>Сиднейское время (зима)</t>
         </is>
       </c>
-      <c r="AA863" t="inlineStr"/>
+      <c r="AA863" t="inlineStr">
+        <is>
+          <t>FA1B60495BEB8AD000</t>
+        </is>
+      </c>
     </row>
     <row r="864">
       <c r="A864" s="1" t="n">
         <v>862</v>
       </c>
       <c r="B864" t="n">
-        <v>4721</v>
+        <v>4781</v>
       </c>
       <c r="C864" t="inlineStr">
         <is>
-          <t>PLD</t>
+          <t>O</t>
         </is>
       </c>
       <c r="D864" s="2" t="n">
-        <v>45927.1139700463</v>
+        <v>45930.02352335648</v>
       </c>
       <c r="E864" t="n">
-        <v>113.64</v>
+        <v>60.3886</v>
       </c>
       <c r="F864" t="n">
-        <v>2500.08</v>
+        <v>2475.9326</v>
       </c>
       <c r="G864" t="n">
-        <v>1.111</v>
+        <v>1.11</v>
       </c>
       <c r="H864" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I864" t="inlineStr"/>
+        <v>45930.10488774306</v>
+      </c>
+      <c r="I864" t="n">
+        <v>60.265</v>
+      </c>
       <c r="J864" t="n">
-        <v>0</v>
+        <v>2470.865</v>
       </c>
       <c r="K864" t="n">
-        <v>0</v>
+        <v>1.12</v>
       </c>
       <c r="L864" t="n">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="M864" t="inlineStr">
         <is>
-          <t>cancelled</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N864" t="n">
@@ -83128,20 +83144,28 @@
         <v>1.006</v>
       </c>
       <c r="Q864" t="n">
-        <v>0.45</v>
+        <v>0.05</v>
       </c>
       <c r="R864" t="n">
-        <v>0</v>
+        <v>-7.297599999999857</v>
       </c>
       <c r="S864" t="inlineStr">
         <is>
-          <t>FA1B5C97052B97C000</t>
-        </is>
-      </c>
-      <c r="T864" t="inlineStr"/>
+          <t>FA1B6055FAF457C000</t>
+        </is>
+      </c>
+      <c r="T864" t="inlineStr">
+        <is>
+          <t>FA1B6056DE1C0AD000</t>
+        </is>
+      </c>
       <c r="U864" t="inlineStr"/>
       <c r="V864" t="inlineStr"/>
-      <c r="W864" t="inlineStr"/>
+      <c r="W864" t="inlineStr">
+        <is>
+          <t>FA1B6056E05157C000</t>
+        </is>
+      </c>
       <c r="X864" t="inlineStr">
         <is>
           <t>MA50_MA5</t>
@@ -83149,8 +83173,8 @@
       </c>
       <c r="Y864" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True, cond_b6: False  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.124, df['MACD'].iloc[-2]: -0.150,  df['MACD_hist'].iloc[-1]: 0.029, df['MACD_hist'].iloc[-2]: -0.017,  delta_MA50_M120.iloc[-1]: 0.367, delta_MA50_M120.iloc[-2]: 0.404,\ 
-  df['MA30_RSI10'].iloc[-1]: 47.035, df['MA30_RSI10'].iloc[-2]: 46.496  delta_MA50_MA120_1m.iloc[-1]: 0.156, delta_MA50_MA120_1m.iloc[-2]: 0.155  df_1m['MA30_RSI10'].iloc[-1]: 60.995, df_1m['MA30_RSI10'].iloc[-2]: 59.902  df_1m['MACD'].iloc[-1]: 0.107, df_1m['MACD'].iloc[-2]: 0.103  df_1m['MACD_hist'].iloc[-1]: 0.063, df_1m['MACD_hist'].iloc[-2]: 0.064  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: -1.696 (more than 1.07 is good),  MACD_hist_max_amp: 0.413, MACD_hist_max_amp_1m: 0.075  
+          <t xml:space="preserve">cond_b1:True, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 0.172, df['MACD'].iloc[-2]: 0.161,  df['MACD_hist'].iloc[-1]: 0.141, df['MACD_hist'].iloc[-2]: 0.141,  delta_MA50_M120.iloc[-1]: 0.003, delta_MA50_M120.iloc[-2]: -0.004,\ 
+  df['MA30_RSI10'].iloc[-1]: 61.989, df['MA30_RSI10'].iloc[-2]: 61.123  delta_MA50_MA120_1m.iloc[-1]: 0.003, delta_MA50_MA120_1m.iloc[-2]: -0.004  df_1m['MA30_RSI10'].iloc[-1]: 55.835, df_1m['MA30_RSI10'].iloc[-2]: 54.977  df_1m['MACD'].iloc[-1]: 0.020, df_1m['MACD'].iloc[-2]: 0.019  df_1m['MACD_hist'].iloc[-1]: 0.011, df_1m['MACD_hist'].iloc[-2]: 0.010  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.000 (more than 1.07 is good),  MACD_hist_max_amp: 0.296, MACD_hist_max_amp_1m: 0.026  
   </t>
         </is>
       </c>
@@ -83159,48 +83183,54 @@
           <t>Сиднейское время (зима)</t>
         </is>
       </c>
-      <c r="AA864" t="inlineStr"/>
+      <c r="AA864" t="inlineStr">
+        <is>
+          <t>FA1B6056DED7CAD000</t>
+        </is>
+      </c>
     </row>
     <row r="865">
       <c r="A865" s="1" t="n">
         <v>863</v>
       </c>
       <c r="B865" t="n">
-        <v>4722</v>
+        <v>4785</v>
       </c>
       <c r="C865" t="inlineStr">
         <is>
-          <t>MASI</t>
+          <t>HLT</t>
         </is>
       </c>
       <c r="D865" s="2" t="n">
-        <v>45927.21069133102</v>
+        <v>45930.161261875</v>
       </c>
       <c r="E865" t="n">
-        <v>141.68</v>
+        <v>262.89</v>
       </c>
       <c r="F865" t="n">
-        <v>2408.56</v>
+        <v>2366.01</v>
       </c>
       <c r="G865" t="n">
-        <v>1.111</v>
+        <v>1.02</v>
       </c>
       <c r="H865" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I865" t="inlineStr"/>
+        <v>45931.01947015047</v>
+      </c>
+      <c r="I865" t="n">
+        <v>260.3</v>
+      </c>
       <c r="J865" t="n">
-        <v>0</v>
+        <v>2342.7</v>
       </c>
       <c r="K865" t="n">
-        <v>0</v>
+        <v>1.03</v>
       </c>
       <c r="L865" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="M865" t="inlineStr">
         <is>
-          <t>cancelled</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N865" t="n">
@@ -83213,20 +83243,28 @@
         <v>1.006</v>
       </c>
       <c r="Q865" t="n">
-        <v>0.45</v>
+        <v>0.05</v>
       </c>
       <c r="R865" t="n">
-        <v>0</v>
+        <v>-25.35999999999995</v>
       </c>
       <c r="S865" t="inlineStr">
         <is>
-          <t>FA1B5CB6E6038AD000</t>
-        </is>
-      </c>
-      <c r="T865" t="inlineStr"/>
+          <t>FA1B6083607DD7C000</t>
+        </is>
+      </c>
+      <c r="T865" t="inlineStr">
+        <is>
+          <t>FA1B6083A922CAD000</t>
+        </is>
+      </c>
       <c r="U865" t="inlineStr"/>
       <c r="V865" t="inlineStr"/>
-      <c r="W865" t="inlineStr"/>
+      <c r="W865" t="inlineStr">
+        <is>
+          <t>FA1B6083AB238AD000</t>
+        </is>
+      </c>
       <c r="X865" t="inlineStr">
         <is>
           <t>MA50_MA5</t>
@@ -83234,8 +83272,8 @@
       </c>
       <c r="Y865" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:False, cond_b5:False, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.587, df['MACD'].iloc[-2]: -0.670,  df['MACD_hist'].iloc[-1]: 0.477, df['MACD_hist'].iloc[-2]: 0.384,  delta_MA50_M120.iloc[-1]: -1.769, delta_MA50_M120.iloc[-2]: -1.724,\ 
-  df['MA30_RSI10'].iloc[-1]: 47.501, df['MA30_RSI10'].iloc[-2]: 47.182  delta_MA50_MA120_1m.iloc[-1]: -0.148, delta_MA50_MA120_1m.iloc[-2]: -0.154  df_1m['MA30_RSI10'].iloc[-1]: 62.047, df_1m['MA30_RSI10'].iloc[-2]: 60.936  df_1m['MACD'].iloc[-1]: 0.089, df_1m['MACD'].iloc[-2]: 0.078  df_1m['MACD_hist'].iloc[-1]: 0.099, df_1m['MACD_hist'].iloc[-2]: 0.092  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.241 (more than 1.07 is good),  MACD_hist_max_amp: 0.882, MACD_hist_max_amp_1m: 0.117  
+          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:False, cond_b5:True, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -1.555, df['MACD'].iloc[-2]: -1.617,  df['MACD_hist'].iloc[-1]: 0.621, df['MACD_hist'].iloc[-2]: 0.593,  delta_MA50_M120.iloc[-1]: -2.062, delta_MA50_M120.iloc[-2]: -2.075,\ 
+  df['MA30_RSI10'].iloc[-1]: 39.310, df['MA30_RSI10'].iloc[-2]: 38.762  delta_MA50_MA120_1m.iloc[-1]: -0.164, delta_MA50_MA120_1m.iloc[-2]: -0.173  df_1m['MA30_RSI10'].iloc[-1]: 58.785, df_1m['MA30_RSI10'].iloc[-2]: 58.094  df_1m['MACD'].iloc[-1]: 0.070, df_1m['MACD'].iloc[-2]: 0.066  df_1m['MACD_hist'].iloc[-1]: 0.076, df_1m['MACD_hist'].iloc[-2]: 0.080  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.048 (more than 1.07 is good),  MACD_hist_max_amp: 1.143, MACD_hist_max_amp_1m: 0.180  
   </t>
         </is>
       </c>
@@ -83244,48 +83282,54 @@
           <t>Сиднейское время (зима)</t>
         </is>
       </c>
-      <c r="AA865" t="inlineStr"/>
+      <c r="AA865" t="inlineStr">
+        <is>
+          <t>FA1B6083A9DD0AD000</t>
+        </is>
+      </c>
     </row>
     <row r="866">
       <c r="A866" s="1" t="n">
         <v>864</v>
       </c>
       <c r="B866" t="n">
-        <v>4723</v>
+        <v>4786</v>
       </c>
       <c r="C866" t="inlineStr">
         <is>
-          <t>MASI</t>
+          <t>ITW</t>
         </is>
       </c>
       <c r="D866" s="2" t="n">
-        <v>45927.21739049769</v>
+        <v>45930.165284375</v>
       </c>
       <c r="E866" t="n">
-        <v>141.76</v>
+        <v>261.89</v>
       </c>
       <c r="F866" t="n">
-        <v>2409.92</v>
+        <v>2357.01</v>
       </c>
       <c r="G866" t="n">
-        <v>1.111</v>
+        <v>1.02</v>
       </c>
       <c r="H866" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I866" t="inlineStr"/>
+        <v>45930.2712137963</v>
+      </c>
+      <c r="I866" t="n">
+        <v>261.26</v>
+      </c>
       <c r="J866" t="n">
-        <v>0</v>
+        <v>2351.34</v>
       </c>
       <c r="K866" t="n">
-        <v>0</v>
+        <v>1.03</v>
       </c>
       <c r="L866" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="M866" t="inlineStr">
         <is>
-          <t>cancelled</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N866" t="n">
@@ -83298,20 +83342,28 @@
         <v>1.006</v>
       </c>
       <c r="Q866" t="n">
-        <v>0.45</v>
+        <v>0.05</v>
       </c>
       <c r="R866" t="n">
-        <v>0</v>
+        <v>-7.720000000000073</v>
       </c>
       <c r="S866" t="inlineStr">
         <is>
-          <t>FA1B5CB91B4357C000</t>
-        </is>
-      </c>
-      <c r="T866" t="inlineStr"/>
+          <t>FA1B6084B3E217C000</t>
+        </is>
+      </c>
+      <c r="T866" t="inlineStr">
+        <is>
+          <t>FA1B60857F90D7C000</t>
+        </is>
+      </c>
       <c r="U866" t="inlineStr"/>
       <c r="V866" t="inlineStr"/>
-      <c r="W866" t="inlineStr"/>
+      <c r="W866" t="inlineStr">
+        <is>
+          <t>FA1B60858180CAD000</t>
+        </is>
+      </c>
       <c r="X866" t="inlineStr">
         <is>
           <t>MA50_MA5</t>
@@ -83319,8 +83371,8 @@
       </c>
       <c r="Y866" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:False, cond_b5:False, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.575, df['MACD'].iloc[-2]: -0.670,  df['MACD_hist'].iloc[-1]: 0.498, df['MACD_hist'].iloc[-2]: 0.384,  delta_MA50_M120.iloc[-1]: -1.767, delta_MA50_M120.iloc[-2]: -1.724,\ 
-  df['MA30_RSI10'].iloc[-1]: 47.561, df['MA30_RSI10'].iloc[-2]: 47.182  delta_MA50_MA120_1m.iloc[-1]: -0.098, delta_MA50_MA120_1m.iloc[-2]: -0.108  df_1m['MA30_RSI10'].iloc[-1]: 65.985, df_1m['MA30_RSI10'].iloc[-2]: 65.716  df_1m['MACD'].iloc[-1]: 0.160, df_1m['MACD'].iloc[-2]: 0.147  df_1m['MACD_hist'].iloc[-1]: 0.131, df_1m['MACD_hist'].iloc[-2]: 0.125  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.295 (more than 1.07 is good),  MACD_hist_max_amp: 0.882, MACD_hist_max_amp_1m: 0.126  
+          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:True, cond_b5:True, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.334, df['MACD'].iloc[-2]: -0.399,  df['MACD_hist'].iloc[-1]: 0.672, df['MACD_hist'].iloc[-2]: 0.645,  delta_MA50_M120.iloc[-1]: -0.715, delta_MA50_M120.iloc[-2]: -0.708,\ 
+  df['MA30_RSI10'].iloc[-1]: 46.937, df['MA30_RSI10'].iloc[-2]: 46.590  delta_MA50_MA120_1m.iloc[-1]: -0.017, delta_MA50_MA120_1m.iloc[-2]: -0.019  df_1m['MA30_RSI10'].iloc[-1]: 49.061, df_1m['MA30_RSI10'].iloc[-2]: 48.626  df_1m['MACD'].iloc[-1]: -0.000, df_1m['MACD'].iloc[-2]: -0.015  df_1m['MACD_hist'].iloc[-1]: 0.067, df_1m['MACD_hist'].iloc[-2]: 0.048  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.042 (more than 1.07 is good),  MACD_hist_max_amp: 0.646, MACD_hist_max_amp_1m: 0.160  
   </t>
         </is>
       </c>
@@ -83329,7 +83381,1462 @@
           <t>Сиднейское время (зима)</t>
         </is>
       </c>
-      <c r="AA866" t="inlineStr"/>
+      <c r="AA866" t="inlineStr">
+        <is>
+          <t>FA1B6085803E57C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" s="1" t="n">
+        <v>865</v>
+      </c>
+      <c r="B867" t="n">
+        <v>4789</v>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>CSCO</t>
+        </is>
+      </c>
+      <c r="D867" s="2" t="n">
+        <v>45930.17633694445</v>
+      </c>
+      <c r="E867" t="n">
+        <v>67.6794</v>
+      </c>
+      <c r="F867" t="n">
+        <v>2436.4584</v>
+      </c>
+      <c r="G867" t="n">
+        <v>0</v>
+      </c>
+      <c r="H867" s="2" t="n">
+        <v>45931.09470480324</v>
+      </c>
+      <c r="I867" t="n">
+        <v>68.26009999999999</v>
+      </c>
+      <c r="J867" t="n">
+        <v>2457.3636</v>
+      </c>
+      <c r="K867" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="L867" t="n">
+        <v>36</v>
+      </c>
+      <c r="M867" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N867" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O867" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P867" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q867" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R867" t="n">
+        <v>19.7951999999997</v>
+      </c>
+      <c r="S867" t="inlineStr">
+        <is>
+          <t>FA1B60882ED397C000</t>
+        </is>
+      </c>
+      <c r="T867" t="inlineStr">
+        <is>
+          <t>FA1B608873F1D7C000</t>
+        </is>
+      </c>
+      <c r="U867" t="inlineStr"/>
+      <c r="V867" t="inlineStr"/>
+      <c r="W867" t="inlineStr">
+        <is>
+          <t>FA1B6088761A0AD000</t>
+        </is>
+      </c>
+      <c r="X867" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y867" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z867" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA867" t="inlineStr">
+        <is>
+          <t>FA1B6088749F4AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" s="1" t="n">
+        <v>866</v>
+      </c>
+      <c r="B868" t="n">
+        <v>4791</v>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="D868" s="2" t="n">
+        <v>45930.24298709491</v>
+      </c>
+      <c r="E868" t="n">
+        <v>289.2</v>
+      </c>
+      <c r="F868" t="n">
+        <v>2313.6</v>
+      </c>
+      <c r="G868" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H868" s="2" t="n">
+        <v>45931.02050689814</v>
+      </c>
+      <c r="I868" t="n">
+        <v>287.77</v>
+      </c>
+      <c r="J868" t="n">
+        <v>2302.16</v>
+      </c>
+      <c r="K868" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L868" t="n">
+        <v>8</v>
+      </c>
+      <c r="M868" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N868" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O868" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P868" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q868" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R868" t="n">
+        <v>-13.47000000000005</v>
+      </c>
+      <c r="S868" t="inlineStr">
+        <is>
+          <t>FA1B609E4FFA0AD000</t>
+        </is>
+      </c>
+      <c r="T868" t="inlineStr">
+        <is>
+          <t>FA1B609FA70917C000</t>
+        </is>
+      </c>
+      <c r="U868" t="inlineStr"/>
+      <c r="V868" t="inlineStr"/>
+      <c r="W868" t="inlineStr">
+        <is>
+          <t>FA1B609FA8F997C000</t>
+        </is>
+      </c>
+      <c r="X868" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y868" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:False, cond_b5:True, cond_b6: False  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -2.743, df['MACD'].iloc[-2]: -2.801,  df['MACD_hist'].iloc[-1]: -0.024, df['MACD_hist'].iloc[-2]: -0.143,  delta_MA50_M120.iloc[-1]: -1.263, delta_MA50_M120.iloc[-2]: -1.173,\ 
+  df['MA30_RSI10'].iloc[-1]: 35.009, df['MA30_RSI10'].iloc[-2]: 34.917  delta_MA50_MA120_1m.iloc[-1]: -0.057, delta_MA50_MA120_1m.iloc[-2]: -0.057  df_1m['MA30_RSI10'].iloc[-1]: 55.765, df_1m['MA30_RSI10'].iloc[-2]: 55.061  df_1m['MACD'].iloc[-1]: 0.098, df_1m['MACD'].iloc[-2]: 0.087  df_1m['MACD_hist'].iloc[-1]: 0.181, df_1m['MACD_hist'].iloc[-2]: 0.188  cond_a1:0, cond_a2:1, cond_a3:0, cond_a4:0  MACD_hist_speed: 0.167 (more than 1.07 is good),  MACD_hist_max_amp: 2.577, MACD_hist_max_amp_1m: 0.229  
+  </t>
+        </is>
+      </c>
+      <c r="Z868" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA868" t="inlineStr">
+        <is>
+          <t>FA1B609FA7BA4AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" s="1" t="n">
+        <v>867</v>
+      </c>
+      <c r="B869" t="n">
+        <v>4802</v>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>LIN</t>
+        </is>
+      </c>
+      <c r="D869" s="2" t="n">
+        <v>45931.16686791667</v>
+      </c>
+      <c r="E869" t="n">
+        <v>476.81</v>
+      </c>
+      <c r="F869" t="n">
+        <v>2384.05</v>
+      </c>
+      <c r="G869" t="n">
+        <v>0</v>
+      </c>
+      <c r="H869" s="2" t="n">
+        <v>45931.20534307871</v>
+      </c>
+      <c r="I869" t="n">
+        <v>475.26</v>
+      </c>
+      <c r="J869" t="n">
+        <v>2376.3</v>
+      </c>
+      <c r="K869" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L869" t="n">
+        <v>5</v>
+      </c>
+      <c r="M869" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N869" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O869" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P869" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q869" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R869" t="n">
+        <v>-8.77</v>
+      </c>
+      <c r="S869" t="inlineStr">
+        <is>
+          <t>FA1B61BBB9014AD000</t>
+        </is>
+      </c>
+      <c r="T869" t="inlineStr">
+        <is>
+          <t>FA1B61CEE9C5CAD000</t>
+        </is>
+      </c>
+      <c r="U869" t="inlineStr"/>
+      <c r="V869" t="inlineStr"/>
+      <c r="W869" t="inlineStr">
+        <is>
+          <t>FA1B61CEEBDACAD000</t>
+        </is>
+      </c>
+      <c r="X869" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y869" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z869" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA869" t="inlineStr">
+        <is>
+          <t>FA1B61CEEA754AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" s="1" t="n">
+        <v>868</v>
+      </c>
+      <c r="B870" t="n">
+        <v>4804</v>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>EMR</t>
+        </is>
+      </c>
+      <c r="D870" s="2" t="n">
+        <v>45931.21633150463</v>
+      </c>
+      <c r="E870" t="n">
+        <v>130.45</v>
+      </c>
+      <c r="F870" t="n">
+        <v>2478.55</v>
+      </c>
+      <c r="G870" t="n">
+        <v>0</v>
+      </c>
+      <c r="H870" s="2" t="n">
+        <v>45932.01812513889</v>
+      </c>
+      <c r="I870" t="n">
+        <v>129.7019</v>
+      </c>
+      <c r="J870" t="n">
+        <v>2464.3361</v>
+      </c>
+      <c r="K870" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="L870" t="n">
+        <v>19</v>
+      </c>
+      <c r="M870" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N870" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O870" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P870" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q870" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R870" t="n">
+        <v>-15.27390000000019</v>
+      </c>
+      <c r="S870" t="inlineStr">
+        <is>
+          <t>FA1B61DEFE914AD000</t>
+        </is>
+      </c>
+      <c r="T870" t="inlineStr">
+        <is>
+          <t>FA1B61DF366817C000</t>
+        </is>
+      </c>
+      <c r="U870" t="inlineStr"/>
+      <c r="V870" t="inlineStr"/>
+      <c r="W870" t="inlineStr">
+        <is>
+          <t>FA1B61DF389217C000</t>
+        </is>
+      </c>
+      <c r="X870" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y870" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z870" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA870" t="inlineStr">
+        <is>
+          <t>FA1B61DF37170AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" s="1" t="n">
+        <v>869</v>
+      </c>
+      <c r="B871" t="n">
+        <v>4867</v>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="D871" s="2" t="n">
+        <v>45931.94101333334</v>
+      </c>
+      <c r="E871" t="n">
+        <v>474.97</v>
+      </c>
+      <c r="F871" t="n">
+        <v>2374.85</v>
+      </c>
+      <c r="G871" t="n">
+        <v>0</v>
+      </c>
+      <c r="H871" s="2" t="n">
+        <v>45932.03274325231</v>
+      </c>
+      <c r="I871" t="n">
+        <v>472.555</v>
+      </c>
+      <c r="J871" t="n">
+        <v>2362.775</v>
+      </c>
+      <c r="K871" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L871" t="n">
+        <v>5</v>
+      </c>
+      <c r="M871" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N871" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O871" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P871" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q871" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R871" t="n">
+        <v>-13.09499999999982</v>
+      </c>
+      <c r="S871" t="inlineStr">
+        <is>
+          <t>FA1B627990DC57C000</t>
+        </is>
+      </c>
+      <c r="T871" t="inlineStr">
+        <is>
+          <t>FA1B62CE601DCAD000</t>
+        </is>
+      </c>
+      <c r="U871" t="inlineStr"/>
+      <c r="V871" t="inlineStr"/>
+      <c r="W871" t="inlineStr">
+        <is>
+          <t>FA1B62CE6241CAD000</t>
+        </is>
+      </c>
+      <c r="X871" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y871" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z871" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA871" t="inlineStr">
+        <is>
+          <t>FA1B62CE60DB4AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" s="1" t="n">
+        <v>870</v>
+      </c>
+      <c r="B872" t="n">
+        <v>4868</v>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>CCI</t>
+        </is>
+      </c>
+      <c r="D872" s="2" t="n">
+        <v>45931.98346862268</v>
+      </c>
+      <c r="E872" t="n">
+        <v>96.86</v>
+      </c>
+      <c r="F872" t="n">
+        <v>2518.36</v>
+      </c>
+      <c r="G872" t="n">
+        <v>0</v>
+      </c>
+      <c r="H872" s="2" t="n">
+        <v>45932.0215125</v>
+      </c>
+      <c r="I872" t="n">
+        <v>96.7</v>
+      </c>
+      <c r="J872" t="n">
+        <v>2514.2</v>
+      </c>
+      <c r="K872" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="L872" t="n">
+        <v>26</v>
+      </c>
+      <c r="M872" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N872" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O872" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P872" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q872" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R872" t="n">
+        <v>-5.239999999999855</v>
+      </c>
+      <c r="S872" t="inlineStr">
+        <is>
+          <t>FA1B627C234717C000</t>
+        </is>
+      </c>
+      <c r="T872" t="inlineStr">
+        <is>
+          <t>FA1B62DC17BC0AD000</t>
+        </is>
+      </c>
+      <c r="U872" t="inlineStr"/>
+      <c r="V872" t="inlineStr"/>
+      <c r="W872" t="inlineStr">
+        <is>
+          <t>FA1B62DC19DAD7C000</t>
+        </is>
+      </c>
+      <c r="X872" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y872" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z872" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA872" t="inlineStr">
+        <is>
+          <t>FA1B62DC186F4AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" s="1" t="n">
+        <v>871</v>
+      </c>
+      <c r="B873" t="n">
+        <v>4866</v>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="D873" s="2" t="n">
+        <v>45931.90979177083</v>
+      </c>
+      <c r="E873" t="n">
+        <v>27.96</v>
+      </c>
+      <c r="F873" t="n">
+        <v>2516.4</v>
+      </c>
+      <c r="G873" t="n">
+        <v>0</v>
+      </c>
+      <c r="H873" s="2" t="n">
+        <v>45932.06126458333</v>
+      </c>
+      <c r="I873" t="n">
+        <v>28.0301</v>
+      </c>
+      <c r="J873" t="n">
+        <v>2522.709</v>
+      </c>
+      <c r="K873" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="L873" t="n">
+        <v>90</v>
+      </c>
+      <c r="M873" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N873" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O873" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P873" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q873" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R873" t="n">
+        <v>5.039000000000197</v>
+      </c>
+      <c r="S873" t="inlineStr">
+        <is>
+          <t>FA1B627C546617C000</t>
+        </is>
+      </c>
+      <c r="T873" t="inlineStr">
+        <is>
+          <t>FA1B62C4245117C000</t>
+        </is>
+      </c>
+      <c r="U873" t="inlineStr"/>
+      <c r="V873" t="inlineStr"/>
+      <c r="W873" t="inlineStr">
+        <is>
+          <t>FA1B62C426864AD000</t>
+        </is>
+      </c>
+      <c r="X873" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y873" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z873" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA873" t="inlineStr">
+        <is>
+          <t>FA1B62C425094AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" s="1" t="n">
+        <v>872</v>
+      </c>
+      <c r="B874" t="n">
+        <v>4873</v>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>EMR</t>
+        </is>
+      </c>
+      <c r="D874" s="2" t="n">
+        <v>45932.03519949074</v>
+      </c>
+      <c r="E874" t="n">
+        <v>130.87</v>
+      </c>
+      <c r="F874" t="n">
+        <v>2486.53</v>
+      </c>
+      <c r="G874" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="H874" s="2" t="n">
+        <v>45933.05182778935</v>
+      </c>
+      <c r="I874" t="n">
+        <v>131.6426315789474</v>
+      </c>
+      <c r="J874" t="n">
+        <v>2501.21</v>
+      </c>
+      <c r="K874" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="L874" t="n">
+        <v>19</v>
+      </c>
+      <c r="M874" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N874" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O874" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P874" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q874" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R874" t="n">
+        <v>12.54999999999984</v>
+      </c>
+      <c r="S874" t="inlineStr">
+        <is>
+          <t>FA1B62ED01E997C000</t>
+        </is>
+      </c>
+      <c r="T874" t="inlineStr">
+        <is>
+          <t>FA1B62ED30CFCAD000</t>
+        </is>
+      </c>
+      <c r="U874" t="inlineStr"/>
+      <c r="V874" t="inlineStr"/>
+      <c r="W874" t="inlineStr">
+        <is>
+          <t>FA1B62ED32FD8AD000</t>
+        </is>
+      </c>
+      <c r="X874" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y874" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.392, df['MACD'].iloc[-2]: -0.439,  df['MACD_hist'].iloc[-1]: 0.395, df['MACD_hist'].iloc[-2]: 0.361,  delta_MA50_M120.iloc[-1]: -1.061, delta_MA50_M120.iloc[-2]: -1.053,\ 
+  delta_MA5_M20.iloc[-1]: 0.922, delta_MA5_M20.iloc[-2]: 0.809,  delta_MA5_M10.iloc[-1]: 0.317, delta_MA5_M10.iloc[-2]: 0.291,  df['MA30_RSI10'].iloc[-1]: 44.848, df['MA30_RSI10'].iloc[-2]: 44.574  delta_MA50_MA120_1m.iloc[-1]: -0.019, delta_MA50_MA120_1m.iloc[-2]: -0.031  df_1m['MA30_RSI10'].iloc[-1]: 59.787, df_1m['MA30_RSI10'].iloc[-2]: 59.751  df_1m['MACD'].iloc[-1]: 0.088, df_1m['MACD'].iloc[-2]: 0.085  df_1m['MACD_hist'].iloc[-1]: 0.034, df_1m['MACD_hist'].iloc[-2]: 0.033  cond_a1:1, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.093 (more than 1.07 is good),  MACD_hist_max_amp: 0.505, MACD_hist_max_amp_1m: 0.117  </t>
+        </is>
+      </c>
+      <c r="Z874" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA874" t="inlineStr">
+        <is>
+          <t>FA1B62ED3193D7C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" s="1" t="n">
+        <v>873</v>
+      </c>
+      <c r="B875" t="n">
+        <v>4884</v>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>DHI</t>
+        </is>
+      </c>
+      <c r="D875" s="2" t="n">
+        <v>45932.11125381944</v>
+      </c>
+      <c r="E875" t="n">
+        <v>170.39</v>
+      </c>
+      <c r="F875" t="n">
+        <v>2385.46</v>
+      </c>
+      <c r="G875" t="n">
+        <v>0</v>
+      </c>
+      <c r="H875" s="2" t="n">
+        <v>45932.14924921296</v>
+      </c>
+      <c r="I875" t="n">
+        <v>169.86</v>
+      </c>
+      <c r="J875" t="n">
+        <v>2378.04</v>
+      </c>
+      <c r="K875" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="L875" t="n">
+        <v>14</v>
+      </c>
+      <c r="M875" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N875" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O875" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P875" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q875" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R875" t="n">
+        <v>-8.460000000000072</v>
+      </c>
+      <c r="S875" t="inlineStr">
+        <is>
+          <t>FA1B62F65E2AD7C000</t>
+        </is>
+      </c>
+      <c r="T875" t="inlineStr">
+        <is>
+          <t>FA1B630630EBCAD000</t>
+        </is>
+      </c>
+      <c r="U875" t="inlineStr"/>
+      <c r="V875" t="inlineStr"/>
+      <c r="W875" t="inlineStr">
+        <is>
+          <t>FA1B63063314CAD000</t>
+        </is>
+      </c>
+      <c r="X875" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y875" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z875" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA875" t="inlineStr">
+        <is>
+          <t>FA1B630631A0CAD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" s="1" t="n">
+        <v>874</v>
+      </c>
+      <c r="B876" t="n">
+        <v>4883</v>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>AON</t>
+        </is>
+      </c>
+      <c r="D876" s="2" t="n">
+        <v>45932.09008663194</v>
+      </c>
+      <c r="E876" t="n">
+        <v>357.19</v>
+      </c>
+      <c r="F876" t="n">
+        <v>2143.14</v>
+      </c>
+      <c r="G876" t="inlineStr"/>
+      <c r="H876" s="2" t="n">
+        <v>45933.01998378472</v>
+      </c>
+      <c r="I876" t="n">
+        <v>355.39</v>
+      </c>
+      <c r="J876" t="n">
+        <v>2132.34</v>
+      </c>
+      <c r="K876" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L876" t="n">
+        <v>6</v>
+      </c>
+      <c r="M876" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N876" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O876" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P876" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q876" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R876" t="inlineStr"/>
+      <c r="S876" t="inlineStr">
+        <is>
+          <t>FA1B62FF18FF97C000</t>
+        </is>
+      </c>
+      <c r="T876" t="inlineStr">
+        <is>
+          <t>FA1B62FF42A817C000</t>
+        </is>
+      </c>
+      <c r="U876" t="inlineStr"/>
+      <c r="V876" t="inlineStr"/>
+      <c r="W876" t="inlineStr">
+        <is>
+          <t>FA1B62FF44C197C000</t>
+        </is>
+      </c>
+      <c r="X876" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y876" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -0.071, df['MACD'].iloc[-2]: -0.157,  df['MACD_hist'].iloc[-1]: 0.788, df['MACD_hist'].iloc[-2]: 0.737,  delta_MA50_M120.iloc[-1]: -1.456, delta_MA50_M120.iloc[-2]: -1.510,\ 
+  delta_MA5_M20.iloc[-1]: 0.226, delta_MA5_M20.iloc[-2]: 0.149,  delta_MA5_M10.iloc[-1]: 0.109, delta_MA5_M10.iloc[-2]: 0.090,  df['MA30_RSI10'].iloc[-1]: 52.685, df['MA30_RSI10'].iloc[-2]: 52.249  delta_MA50_MA120_1m.iloc[-1]: 0.294, delta_MA50_MA120_1m.iloc[-2]: 0.281  df_1m['MA30_RSI10'].iloc[-1]: 59.019, df_1m['MA30_RSI10'].iloc[-2]: 58.871  df_1m['MACD'].iloc[-1]: 0.349, df_1m['MACD'].iloc[-2]: 0.340  df_1m['MACD_hist'].iloc[-1]: -0.020, df_1m['MACD_hist'].iloc[-2]: -0.040  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.070 (more than 1.07 is good),  MACD_hist_max_amp: 1.447, MACD_hist_max_amp_1m: 0.398  </t>
+        </is>
+      </c>
+      <c r="Z876" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA876" t="inlineStr">
+        <is>
+          <t>FA1B62FF436B97C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" s="1" t="n">
+        <v>875</v>
+      </c>
+      <c r="B877" t="n">
+        <v>4887</v>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="D877" s="2" t="n">
+        <v>45932.15200112268</v>
+      </c>
+      <c r="E877" t="n">
+        <v>83.84</v>
+      </c>
+      <c r="F877" t="n">
+        <v>2431.36</v>
+      </c>
+      <c r="G877" t="n">
+        <v>0</v>
+      </c>
+      <c r="H877" s="2" t="n">
+        <v>45933.04545796297</v>
+      </c>
+      <c r="I877" t="n">
+        <v>86.02200000000001</v>
+      </c>
+      <c r="J877" t="n">
+        <v>2494.638</v>
+      </c>
+      <c r="K877" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="L877" t="n">
+        <v>29</v>
+      </c>
+      <c r="M877" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N877" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O877" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P877" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q877" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R877" t="n">
+        <v>62.18800000000024</v>
+      </c>
+      <c r="S877" t="inlineStr">
+        <is>
+          <t>FA1B631339E88AD000</t>
+        </is>
+      </c>
+      <c r="T877" t="inlineStr">
+        <is>
+          <t>FA1B63139D1D17C000</t>
+        </is>
+      </c>
+      <c r="U877" t="inlineStr"/>
+      <c r="V877" t="inlineStr"/>
+      <c r="W877" t="inlineStr">
+        <is>
+          <t>FA1B63139F4D0AD000</t>
+        </is>
+      </c>
+      <c r="X877" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y877" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z877" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA877" t="inlineStr">
+        <is>
+          <t>FA1B63139DDCCAD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" s="1" t="n">
+        <v>876</v>
+      </c>
+      <c r="B878" t="n">
+        <v>4898</v>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>ROP</t>
+        </is>
+      </c>
+      <c r="D878" s="2" t="n">
+        <v>45933.0217878125</v>
+      </c>
+      <c r="E878" t="n">
+        <v>498.59</v>
+      </c>
+      <c r="F878" t="n">
+        <v>2492.95</v>
+      </c>
+      <c r="G878" t="n">
+        <v>0</v>
+      </c>
+      <c r="H878" s="2" t="n">
+        <v>45933.06020748842</v>
+      </c>
+      <c r="I878" t="n">
+        <v>496.65</v>
+      </c>
+      <c r="J878" t="n">
+        <v>2483.25</v>
+      </c>
+      <c r="K878" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L878" t="n">
+        <v>5</v>
+      </c>
+      <c r="M878" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N878" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O878" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P878" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q878" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R878" t="n">
+        <v>-10.71999999999982</v>
+      </c>
+      <c r="S878" t="inlineStr">
+        <is>
+          <t>FA1B642A757957C000</t>
+        </is>
+      </c>
+      <c r="T878" t="inlineStr">
+        <is>
+          <t>FA1B643246C94AD000</t>
+        </is>
+      </c>
+      <c r="U878" t="inlineStr"/>
+      <c r="V878" t="inlineStr"/>
+      <c r="W878" t="inlineStr">
+        <is>
+          <t>FA1B643248ECD7C000</t>
+        </is>
+      </c>
+      <c r="X878" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y878" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z878" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA878" t="inlineStr">
+        <is>
+          <t>FA1B643247834AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" s="1" t="n">
+        <v>877</v>
+      </c>
+      <c r="B879" t="n">
+        <v>4900</v>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>EMR</t>
+        </is>
+      </c>
+      <c r="D879" s="2" t="n">
+        <v>45933.07370545139</v>
+      </c>
+      <c r="E879" t="n">
+        <v>132.32</v>
+      </c>
+      <c r="F879" t="n">
+        <v>2381.76</v>
+      </c>
+      <c r="G879" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="H879" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I879" t="inlineStr"/>
+      <c r="J879" t="n">
+        <v>0</v>
+      </c>
+      <c r="K879" t="n">
+        <v>0</v>
+      </c>
+      <c r="L879" t="n">
+        <v>18</v>
+      </c>
+      <c r="M879" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N879" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O879" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P879" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q879" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R879" t="n">
+        <v>0</v>
+      </c>
+      <c r="S879" t="inlineStr">
+        <is>
+          <t>FA1B644349DF4AD000</t>
+        </is>
+      </c>
+      <c r="T879" t="inlineStr">
+        <is>
+          <t>FA1B64437E37D7C000</t>
+        </is>
+      </c>
+      <c r="U879" t="inlineStr"/>
+      <c r="V879" t="inlineStr"/>
+      <c r="W879" t="inlineStr">
+        <is>
+          <t>FA1B644380A8D7C000</t>
+        </is>
+      </c>
+      <c r="X879" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y879" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:True, cond_b5:True, cond_b6: False  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 0.019, df['MACD'].iloc[-2]: -0.043,  df['MACD_hist'].iloc[-1]: 0.591, df['MACD_hist'].iloc[-2]: 0.557,  delta_MA50_M120.iloc[-1]: -1.160, delta_MA50_M120.iloc[-2]: -1.169,\ 
+  delta_MA5_M20.iloc[-1]: 0.789, delta_MA5_M20.iloc[-2]: 0.787,  delta_MA5_M10.iloc[-1]: 0.270, delta_MA5_M10.iloc[-2]: 0.221,  df['MA30_RSI10'].iloc[-1]: 52.014, df['MA30_RSI10'].iloc[-2]: 51.239  delta_MA50_MA120_1m.iloc[-1]: -0.051, delta_MA50_MA120_1m.iloc[-2]: -0.058  df_1m['MA30_RSI10'].iloc[-1]: 46.602, df_1m['MA30_RSI10'].iloc[-2]: 45.813  df_1m['MACD'].iloc[-1]: 0.014, df_1m['MACD'].iloc[-2]: 0.007  df_1m['MACD_hist'].iloc[-1]: 0.047, df_1m['MACD_hist'].iloc[-2]: 0.041  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.061 (more than 1.07 is good),  MACD_hist_max_amp: 0.527, MACD_hist_max_amp_1m: 0.092  </t>
+        </is>
+      </c>
+      <c r="Z879" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA879" t="inlineStr">
+        <is>
+          <t>FA1B64437F0B4AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" s="1" t="n">
+        <v>881</v>
+      </c>
+      <c r="B880" t="n">
+        <v>4904</v>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>HLT</t>
+        </is>
+      </c>
+      <c r="D880" s="2" t="n">
+        <v>45933.14281229167</v>
+      </c>
+      <c r="E880" t="n">
+        <v>258.23</v>
+      </c>
+      <c r="F880" t="n">
+        <v>2324.07</v>
+      </c>
+      <c r="G880" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="H880" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I880" t="inlineStr"/>
+      <c r="J880" t="n">
+        <v>0</v>
+      </c>
+      <c r="K880" t="n">
+        <v>0</v>
+      </c>
+      <c r="L880" t="n">
+        <v>9</v>
+      </c>
+      <c r="M880" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N880" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O880" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P880" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q880" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R880" t="n">
+        <v>0</v>
+      </c>
+      <c r="S880" t="inlineStr">
+        <is>
+          <t>FA1B645A10BE97C000</t>
+        </is>
+      </c>
+      <c r="T880" t="inlineStr">
+        <is>
+          <t>FA1B645BB3DE4AD000</t>
+        </is>
+      </c>
+      <c r="U880" t="inlineStr"/>
+      <c r="V880" t="inlineStr"/>
+      <c r="W880" t="inlineStr">
+        <is>
+          <t>FA1B645BB61BD7C000</t>
+        </is>
+      </c>
+      <c r="X880" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y880" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:False, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: -2.158, df['MACD'].iloc[-2]: -2.237,  df['MACD_hist'].iloc[-1]: -0.248, df['MACD_hist'].iloc[-2]: -0.444,  delta_MA50_M120.iloc[-1]: -2.268, delta_MA50_M120.iloc[-2]: -2.272,\ 
+  delta_MA5_M20.iloc[-1]: -0.640, delta_MA5_M20.iloc[-2]: -0.822,  delta_MA5_M10.iloc[-1]: 0.035, delta_MA5_M10.iloc[-2]: 0.012,  df['MA30_RSI10'].iloc[-1]: 40.822, df['MA30_RSI10'].iloc[-2]: 40.540  delta_MA50_MA120_1m.iloc[-1]: 0.317, delta_MA50_MA120_1m.iloc[-2]: 0.317  df_1m['MA30_RSI10'].iloc[-1]: 68.972, df_1m['MA30_RSI10'].iloc[-2]: 68.574  df_1m['MACD'].iloc[-1]: 0.346, df_1m['MACD'].iloc[-2]: 0.344  df_1m['MACD_hist'].iloc[-1]: 0.021, df_1m['MACD_hist'].iloc[-2]: 0.022  cond_a1:0, cond_a2:1, cond_a3:1, cond_a4:0  MACD_hist_speed: 0.559 (more than 1.07 is good),  MACD_hist_max_amp: 0.646, MACD_hist_max_amp_1m: 0.205  </t>
+        </is>
+      </c>
+      <c r="Z880" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA880" t="inlineStr">
+        <is>
+          <t>FA1B645BB49E4AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" s="1" t="n">
+        <v>882</v>
+      </c>
+      <c r="B881" t="n">
+        <v>4906</v>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="D881" s="2" t="n">
+        <v>45933.14629321759</v>
+      </c>
+      <c r="E881" t="n">
+        <v>576.12</v>
+      </c>
+      <c r="F881" t="n">
+        <v>2304.48</v>
+      </c>
+      <c r="G881" t="n">
+        <v>0</v>
+      </c>
+      <c r="H881" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I881" t="inlineStr"/>
+      <c r="J881" t="n">
+        <v>0</v>
+      </c>
+      <c r="K881" t="n">
+        <v>0</v>
+      </c>
+      <c r="L881" t="n">
+        <v>4</v>
+      </c>
+      <c r="M881" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N881" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O881" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P881" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q881" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R881" t="n">
+        <v>0</v>
+      </c>
+      <c r="S881" t="inlineStr">
+        <is>
+          <t>FA1B645B053E0AD000</t>
+        </is>
+      </c>
+      <c r="T881" t="inlineStr">
+        <is>
+          <t>FA1B645B51714AD000</t>
+        </is>
+      </c>
+      <c r="U881" t="inlineStr"/>
+      <c r="V881" t="inlineStr"/>
+      <c r="W881" t="inlineStr">
+        <is>
+          <t>FA1B645B53A697C000</t>
+        </is>
+      </c>
+      <c r="X881" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y881" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z881" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA881" t="inlineStr">
+        <is>
+          <t>FA1B645B523A57C000</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
before cleaning the condtions and code
</commit_message>
<xml_diff>
--- a/db/real_trade_db.xlsx
+++ b/db/real_trade_db.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA881"/>
+  <dimension ref="A1:AA887"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -84556,7 +84556,7 @@
         <v>877</v>
       </c>
       <c r="B879" t="n">
-        <v>4900</v>
+        <v>4936</v>
       </c>
       <c r="C879" t="inlineStr">
         <is>
@@ -84564,7 +84564,7 @@
         </is>
       </c>
       <c r="D879" s="2" t="n">
-        <v>45933.07370545139</v>
+        <v>45934.05161071759</v>
       </c>
       <c r="E879" t="n">
         <v>132.32</v>
@@ -84573,24 +84573,26 @@
         <v>2381.76</v>
       </c>
       <c r="G879" t="n">
-        <v>1.04</v>
+        <v>0</v>
       </c>
       <c r="H879" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I879" t="inlineStr"/>
+        <v>45934.08968305556</v>
+      </c>
+      <c r="I879" t="n">
+        <v>135.31</v>
+      </c>
       <c r="J879" t="n">
-        <v>0</v>
+        <v>2435.58</v>
       </c>
       <c r="K879" t="n">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="L879" t="n">
         <v>18</v>
       </c>
       <c r="M879" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N879" t="n">
@@ -84603,10 +84605,10 @@
         <v>1.006</v>
       </c>
       <c r="Q879" t="n">
-        <v>1.25</v>
+        <v>0.31</v>
       </c>
       <c r="R879" t="n">
-        <v>0</v>
+        <v>52.76999999999971</v>
       </c>
       <c r="S879" t="inlineStr">
         <is>
@@ -84615,14 +84617,14 @@
       </c>
       <c r="T879" t="inlineStr">
         <is>
-          <t>FA1B64437E37D7C000</t>
+          <t>FA1B6585B6F14AD000</t>
         </is>
       </c>
       <c r="U879" t="inlineStr"/>
       <c r="V879" t="inlineStr"/>
       <c r="W879" t="inlineStr">
         <is>
-          <t>FA1B644380A8D7C000</t>
+          <t>FA1B6585B9310AD000</t>
         </is>
       </c>
       <c r="X879" t="inlineStr">
@@ -84632,8 +84634,7 @@
       </c>
       <c r="Y879" t="inlineStr">
         <is>
-          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:True, cond_b5:True, cond_b6: False  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 0.019, df['MACD'].iloc[-2]: -0.043,  df['MACD_hist'].iloc[-1]: 0.591, df['MACD_hist'].iloc[-2]: 0.557,  delta_MA50_M120.iloc[-1]: -1.160, delta_MA50_M120.iloc[-2]: -1.169,\ 
-  delta_MA5_M20.iloc[-1]: 0.789, delta_MA5_M20.iloc[-2]: 0.787,  delta_MA5_M10.iloc[-1]: 0.270, delta_MA5_M10.iloc[-2]: 0.221,  df['MA30_RSI10'].iloc[-1]: 52.014, df['MA30_RSI10'].iloc[-2]: 51.239  delta_MA50_MA120_1m.iloc[-1]: -0.051, delta_MA50_MA120_1m.iloc[-2]: -0.058  df_1m['MA30_RSI10'].iloc[-1]: 46.602, df_1m['MA30_RSI10'].iloc[-2]: 45.813  df_1m['MACD'].iloc[-1]: 0.014, df_1m['MACD'].iloc[-2]: 0.007  df_1m['MACD_hist'].iloc[-1]: 0.047, df_1m['MACD_hist'].iloc[-2]: 0.041  cond_a1:0, cond_a2:0, cond_a3:0, cond_a4:0  MACD_hist_speed: 1.061 (more than 1.07 is good),  MACD_hist_max_amp: 0.527, MACD_hist_max_amp_1m: 0.092  </t>
+          <t>{}</t>
         </is>
       </c>
       <c r="Z879" t="inlineStr">
@@ -84643,13 +84644,13 @@
       </c>
       <c r="AA879" t="inlineStr">
         <is>
-          <t>FA1B64437F0B4AD000</t>
+          <t>FA1B6585B7A697C000</t>
         </is>
       </c>
     </row>
     <row r="880">
       <c r="A880" s="1" t="n">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="B880" t="n">
         <v>4904</v>
@@ -84672,21 +84673,23 @@
         <v>1.02</v>
       </c>
       <c r="H880" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I880" t="inlineStr"/>
+        <v>45934.05504837963</v>
+      </c>
+      <c r="I880" t="n">
+        <v>257.24</v>
+      </c>
       <c r="J880" t="n">
-        <v>0</v>
+        <v>2315.16</v>
       </c>
       <c r="K880" t="n">
-        <v>0</v>
+        <v>1.03</v>
       </c>
       <c r="L880" t="n">
         <v>9</v>
       </c>
       <c r="M880" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N880" t="n">
@@ -84699,10 +84702,10 @@
         <v>1.006</v>
       </c>
       <c r="Q880" t="n">
-        <v>1.25</v>
+        <v>0.05</v>
       </c>
       <c r="R880" t="n">
-        <v>0</v>
+        <v>-10.96000000000031</v>
       </c>
       <c r="S880" t="inlineStr">
         <is>
@@ -84745,7 +84748,7 @@
     </row>
     <row r="881">
       <c r="A881" s="1" t="n">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="B881" t="n">
         <v>4906</v>
@@ -84768,21 +84771,23 @@
         <v>0</v>
       </c>
       <c r="H881" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I881" t="inlineStr"/>
+        <v>45934.02064480324</v>
+      </c>
+      <c r="I881" t="n">
+        <v>577.1</v>
+      </c>
       <c r="J881" t="n">
-        <v>0</v>
+        <v>2308.4</v>
       </c>
       <c r="K881" t="n">
-        <v>0</v>
+        <v>1.101</v>
       </c>
       <c r="L881" t="n">
         <v>4</v>
       </c>
       <c r="M881" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N881" t="n">
@@ -84795,10 +84800,10 @@
         <v>1.006</v>
       </c>
       <c r="Q881" t="n">
-        <v>1.25</v>
+        <v>0.05</v>
       </c>
       <c r="R881" t="n">
-        <v>0</v>
+        <v>2.819000000000073</v>
       </c>
       <c r="S881" t="inlineStr">
         <is>
@@ -84835,6 +84840,576 @@
       <c r="AA881" t="inlineStr">
         <is>
           <t>FA1B645B523A57C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" s="1" t="n">
+        <v>880</v>
+      </c>
+      <c r="B882" t="n">
+        <v>4933</v>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>GIS</t>
+        </is>
+      </c>
+      <c r="D882" s="2" t="n">
+        <v>45934.03420574074</v>
+      </c>
+      <c r="E882" t="n">
+        <v>50.6091</v>
+      </c>
+      <c r="F882" t="n">
+        <v>2479.8459</v>
+      </c>
+      <c r="G882" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="H882" s="2" t="n">
+        <v>45934.09922538194</v>
+      </c>
+      <c r="I882" t="n">
+        <v>50.2902</v>
+      </c>
+      <c r="J882" t="n">
+        <v>2464.2198</v>
+      </c>
+      <c r="K882" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="L882" t="n">
+        <v>49</v>
+      </c>
+      <c r="M882" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N882" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O882" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P882" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q882" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R882" t="n">
+        <v>-17.91609999999995</v>
+      </c>
+      <c r="S882" t="inlineStr">
+        <is>
+          <t>FA1B657FDC1017C000</t>
+        </is>
+      </c>
+      <c r="T882" t="inlineStr">
+        <is>
+          <t>FA1B65808F2057C000</t>
+        </is>
+      </c>
+      <c r="U882" t="inlineStr"/>
+      <c r="V882" t="inlineStr"/>
+      <c r="W882" t="inlineStr">
+        <is>
+          <t>FA1B6580914C8AD000</t>
+        </is>
+      </c>
+      <c r="X882" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y882" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True, cond_b6: True  cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1  cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,  no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,  cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:1,  permit_1h_cond:0,  df['MACD'].iloc[-1]: 0.117, df['MACD'].iloc[-2]: 0.110,  df['MACD_hist'].iloc[-1]: 0.058, df['MACD_hist'].iloc[-2]: 0.052,  delta_MA50_M120.iloc[-1]: 0.247, delta_MA50_M120.iloc[-2]: 0.269,\ 
+  delta_MA5_M20.iloc[-1]: -0.006, delta_MA5_M20.iloc[-2]: -0.074,  delta_MA5_M10.iloc[-1]: -0.016, delta_MA5_M10.iloc[-2]: -0.184,  df['MA30_RSI10'].iloc[-1]: 55.199, df['MA30_RSI10'].iloc[-2]: 55.008  delta_MA50_MA120_1m.iloc[-1]: 0.239, delta_MA50_MA120_1m.iloc[-2]: 0.237  df_1m['MA30_RSI10'].iloc[-1]: 58.664, df_1m['MA30_RSI10'].iloc[-2]: 58.306  df_1m['MACD'].iloc[-1]: 0.038, df_1m['MACD'].iloc[-2]: 0.037  df_1m['MACD_hist'].iloc[-1]: -0.004, df_1m['MACD_hist'].iloc[-2]: -0.005  MACD_hist_speed: 1.108 (more than 1.07 is good)
+  </t>
+        </is>
+      </c>
+      <c r="Z882" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA882" t="inlineStr">
+        <is>
+          <t>FA1B65808FD257C000</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" s="1" t="n">
+        <v>881</v>
+      </c>
+      <c r="B883" t="n">
+        <v>4935</v>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>COST</t>
+        </is>
+      </c>
+      <c r="D883" s="2" t="n">
+        <v>45934.04008702546</v>
+      </c>
+      <c r="E883" t="n">
+        <v>913.38</v>
+      </c>
+      <c r="F883" t="n">
+        <v>1826.76</v>
+      </c>
+      <c r="G883" t="n">
+        <v>0</v>
+      </c>
+      <c r="H883" s="2" t="n">
+        <v>45934.07801328703</v>
+      </c>
+      <c r="I883" t="n">
+        <v>912.64</v>
+      </c>
+      <c r="J883" t="n">
+        <v>1825.28</v>
+      </c>
+      <c r="K883" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="L883" t="n">
+        <v>2</v>
+      </c>
+      <c r="M883" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N883" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O883" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P883" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q883" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="R883" t="n">
+        <v>-2.490000000000018</v>
+      </c>
+      <c r="S883" t="inlineStr">
+        <is>
+          <t>FA1B658062224AD000</t>
+        </is>
+      </c>
+      <c r="T883" t="inlineStr"/>
+      <c r="U883" t="inlineStr"/>
+      <c r="V883" t="inlineStr"/>
+      <c r="W883" t="inlineStr"/>
+      <c r="X883" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y883" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z883" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA883" t="inlineStr"/>
+    </row>
+    <row r="884">
+      <c r="A884" s="1" t="n">
+        <v>884</v>
+      </c>
+      <c r="B884" t="n">
+        <v>4941</v>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>WFC</t>
+        </is>
+      </c>
+      <c r="D884" s="2" t="n">
+        <v>45934.16504248843</v>
+      </c>
+      <c r="E884" t="n">
+        <v>81.1788</v>
+      </c>
+      <c r="F884" t="n">
+        <v>2435.364</v>
+      </c>
+      <c r="G884" t="n">
+        <v>0</v>
+      </c>
+      <c r="H884" s="2" t="n">
+        <v>45934.20309125</v>
+      </c>
+      <c r="I884" t="n">
+        <v>80.782</v>
+      </c>
+      <c r="J884" t="n">
+        <v>2423.46</v>
+      </c>
+      <c r="K884" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="L884" t="n">
+        <v>30</v>
+      </c>
+      <c r="M884" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N884" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O884" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P884" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q884" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R884" t="n">
+        <v>-12.994</v>
+      </c>
+      <c r="S884" t="inlineStr">
+        <is>
+          <t>FA1B65993B2FCAD000</t>
+        </is>
+      </c>
+      <c r="T884" t="inlineStr">
+        <is>
+          <t>FA1B65AB18F70AD000</t>
+        </is>
+      </c>
+      <c r="U884" t="inlineStr"/>
+      <c r="V884" t="inlineStr"/>
+      <c r="W884" t="inlineStr">
+        <is>
+          <t>FA1B65AB1B2057C000</t>
+        </is>
+      </c>
+      <c r="X884" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y884" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z884" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA884" t="inlineStr">
+        <is>
+          <t>FA1B65AB19B60AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" s="1" t="n">
+        <v>885</v>
+      </c>
+      <c r="B885" t="n">
+        <v>4939</v>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>COST</t>
+        </is>
+      </c>
+      <c r="D885" s="2" t="n">
+        <v>45934.15648304398</v>
+      </c>
+      <c r="E885" t="n">
+        <v>916.85</v>
+      </c>
+      <c r="F885" t="n">
+        <v>1833.7</v>
+      </c>
+      <c r="G885" t="n">
+        <v>1</v>
+      </c>
+      <c r="H885" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I885" t="inlineStr"/>
+      <c r="J885" t="n">
+        <v>0</v>
+      </c>
+      <c r="K885" t="n">
+        <v>0</v>
+      </c>
+      <c r="L885" t="n">
+        <v>2</v>
+      </c>
+      <c r="M885" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N885" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O885" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P885" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q885" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R885" t="n">
+        <v>0</v>
+      </c>
+      <c r="S885" t="inlineStr">
+        <is>
+          <t>FA1B65A82941CAD000</t>
+        </is>
+      </c>
+      <c r="T885" t="inlineStr">
+        <is>
+          <t>FA1B65A90BCF97C000</t>
+        </is>
+      </c>
+      <c r="U885" t="inlineStr"/>
+      <c r="V885" t="inlineStr"/>
+      <c r="W885" t="inlineStr">
+        <is>
+          <t>FA1B65A90DF617C000</t>
+        </is>
+      </c>
+      <c r="X885" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y885" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:True, cond_b3:False, cond_b4:False, cond_b5:True, cond_b6: False    cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:0    cond_delta_MA50_M120:0, cond_grad_MACD_1m:1,    no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,    cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,    permit_1h_cond:0,    df['MACD'].iloc[-1]: -5.566, df['MACD'].iloc[-2]: -5.782,    df['MACD_hist'].iloc[-1]: 1.458, df['MACD_hist'].iloc[-2]: 1.249,    delta_MA50_M120.iloc[-1]: -2.033, delta_MA50_M120.iloc[-2]: -2.004,\ 
+    delta_MA5_M20.iloc[-1]: -0.156, delta_MA5_M20.iloc[-2]: -0.224,    delta_MA5_M10.iloc[-1]: -0.107, delta_MA5_M10.iloc[-2]: -0.082,    df['MA30_RSI10'].iloc[-1]: 45.879, df['MA30_RSI10'].iloc[-2]: 44.928    delta_MA50_MA120_1m.iloc[-1]: 0.018, delta_MA50_MA120_1m.iloc[-2]: 0.017    df_1m['MA30_RSI10'].iloc[-1]: 53.836, df_1m['MA30_RSI10'].iloc[-2]: 53.179    df_1m['MACD'].iloc[-1]: 0.276, df_1m['MACD'].iloc[-2]: 0.238    df_1m['MACD_hist'].iloc[-1]: 0.371, df_1m['MACD_hist'].iloc[-2]: 0.352    MACD_hist_speed: 1.167 (more than 1.07 is good)
+    </t>
+        </is>
+      </c>
+      <c r="Z885" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA885" t="inlineStr">
+        <is>
+          <t>FA1B65A90C7CCAD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" s="1" t="n">
+        <v>886</v>
+      </c>
+      <c r="B886" t="n">
+        <v>4940</v>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>KMB</t>
+        </is>
+      </c>
+      <c r="D886" s="2" t="n">
+        <v>45934.16406825231</v>
+      </c>
+      <c r="E886" t="n">
+        <v>122.8175</v>
+      </c>
+      <c r="F886" t="n">
+        <v>2456.35</v>
+      </c>
+      <c r="G886" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="H886" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I886" t="inlineStr"/>
+      <c r="J886" t="n">
+        <v>0</v>
+      </c>
+      <c r="K886" t="n">
+        <v>0</v>
+      </c>
+      <c r="L886" t="n">
+        <v>20</v>
+      </c>
+      <c r="M886" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N886" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O886" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P886" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q886" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R886" t="n">
+        <v>0</v>
+      </c>
+      <c r="S886" t="inlineStr">
+        <is>
+          <t>FA1B65AAA9434AD000</t>
+        </is>
+      </c>
+      <c r="T886" t="inlineStr">
+        <is>
+          <t>FA1B65ABA90817C000</t>
+        </is>
+      </c>
+      <c r="U886" t="inlineStr"/>
+      <c r="V886" t="inlineStr"/>
+      <c r="W886" t="inlineStr">
+        <is>
+          <t>FA1B65ABAB2C17C000</t>
+        </is>
+      </c>
+      <c r="X886" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cond_b1:False, cond_b2:False, cond_b3:False, cond_b4:False, cond_b5:True, cond_b6: True    cond_RSI:1, cond_grad_MACD:1, cond_grad_MA5:1    cond_delta_MA50_M120:1, cond_grad_MACD_1m:1,    no_big_spikes_1h:1, cond_grad_MA50_M120_1m_120:1,    cond_grad_MA5_1m:1, cond_RSI_1m:1, cond_VR:1, ha_cond:0,    permit_1h_cond:0,    df['MACD'].iloc[-1]: -0.300, df['MACD'].iloc[-2]: -0.312,    df['MACD_hist'].iloc[-1]: 0.017, df['MACD_hist'].iloc[-2]: -0.004,    delta_MA50_M120.iloc[-1]: -1.540, delta_MA50_M120.iloc[-2]: -1.547,\ 
+    delta_MA5_M20.iloc[-1]: -0.425, delta_MA5_M20.iloc[-2]: -0.513,    delta_MA5_M10.iloc[-1]: -0.036, delta_MA5_M10.iloc[-2]: -0.076,    df['MA30_RSI10'].iloc[-1]: 52.236, df['MA30_RSI10'].iloc[-2]: 51.905    delta_MA50_MA120_1m.iloc[-1]: 0.119, delta_MA50_MA120_1m.iloc[-2]: 0.118    df_1m['MA30_RSI10'].iloc[-1]: 53.599, df_1m['MA30_RSI10'].iloc[-2]: 53.430    df_1m['MACD'].iloc[-1]: 0.039, df_1m['MACD'].iloc[-2]: 0.038    df_1m['MACD_hist'].iloc[-1]: 0.006, df_1m['MACD_hist'].iloc[-2]: 0.004    MACD_hist_speed: -4.045 (more than 1.07 is good)
+    </t>
+        </is>
+      </c>
+      <c r="Z886" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA886" t="inlineStr">
+        <is>
+          <t>FA1B65ABA9CC4AD000</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" s="1" t="n">
+        <v>888</v>
+      </c>
+      <c r="B887" t="n">
+        <v>4943</v>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>BAC</t>
+        </is>
+      </c>
+      <c r="D887" s="2" t="n">
+        <v>45934.19037908564</v>
+      </c>
+      <c r="E887" t="n">
+        <v>50.745</v>
+      </c>
+      <c r="F887" t="n">
+        <v>2486.505</v>
+      </c>
+      <c r="G887" t="n">
+        <v>0</v>
+      </c>
+      <c r="H887" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I887" t="inlineStr"/>
+      <c r="J887" t="n">
+        <v>0</v>
+      </c>
+      <c r="K887" t="n">
+        <v>0</v>
+      </c>
+      <c r="L887" t="n">
+        <v>49</v>
+      </c>
+      <c r="M887" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N887" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O887" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="P887" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q887" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R887" t="n">
+        <v>0</v>
+      </c>
+      <c r="S887" t="inlineStr">
+        <is>
+          <t>FA1B65B1AFB357C000</t>
+        </is>
+      </c>
+      <c r="T887" t="inlineStr">
+        <is>
+          <t>FA1B65B370D20AD000</t>
+        </is>
+      </c>
+      <c r="U887" t="inlineStr"/>
+      <c r="V887" t="inlineStr"/>
+      <c r="W887" t="inlineStr">
+        <is>
+          <t>FA1B65B372D54AD000</t>
+        </is>
+      </c>
+      <c r="X887" t="inlineStr">
+        <is>
+          <t>MA50_MA5</t>
+        </is>
+      </c>
+      <c r="Y887" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="Z887" t="inlineStr">
+        <is>
+          <t>Сиднейское время (зима)</t>
+        </is>
+      </c>
+      <c r="AA887" t="inlineStr">
+        <is>
+          <t>FA1B65B37181CAD000</t>
         </is>
       </c>
     </row>

</xml_diff>